<commit_message>
Add live validation and help text to address, education, and family form fields, and improve education form navigation with anchor links
Added real-time validation using wire:model.live for all form fields in the address, education, and family update forms. Implemented updatedFieldName() methods in the Livewire components to validate fields as users type. Added descriptive help text below each input field to guide users on expected format and content. Included error message displays and loading indicators
</commit_message>
<xml_diff>
--- a/public/report/pds_generated.xlsx
+++ b/public/report/pds_generated.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="440">
   <si>
     <t xml:space="preserve">        </t>
   </si>
@@ -103,19 +103,19 @@
     <t>SURNAME</t>
   </si>
   <si>
-    <t>Bergnaum</t>
+    <t>Simonis</t>
   </si>
   <si>
     <t>FIRST NAME</t>
   </si>
   <si>
-    <t>Ava</t>
+    <t>Karlie</t>
   </si>
   <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                           </t>
   </si>
   <si>
-    <t>I</t>
+    <t>Harley Gotardo</t>
   </si>
   <si>
     <t>Married</t>
@@ -143,7 +143,7 @@
 (mm/dd/yyyy)  </t>
   </si>
   <si>
-    <t>2023-03-25</t>
+    <t>1993-11-13</t>
   </si>
   <si>
     <t>16. CITIZENSHIP</t>
@@ -164,7 +164,7 @@
     <t>PLACE OF BIRTH</t>
   </si>
   <si>
-    <t>Considineshire</t>
+    <t>Zulaufville</t>
   </si>
   <si>
     <t xml:space="preserve">If holder of  dual citizenship, </t>
@@ -182,10 +182,10 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>Male ☑</t>
-  </si>
-  <si>
-    <t>Female ☐</t>
+    <t>Make ☐</t>
+  </si>
+  <si>
+    <t>Female ☑</t>
   </si>
   <si>
     <t>please indicate the details.</t>
@@ -200,16 +200,16 @@
     <t>CIVIL STATUS</t>
   </si>
   <si>
-    <t>☑Single ☐Married ☐Widowed</t>
+    <t>☐Single ☐Married ☑Widowed</t>
   </si>
   <si>
     <t>17. RESIDENTIAL ADDRESS</t>
   </si>
   <si>
-    <t>asdadsf sadfwar2345w</t>
-  </si>
-  <si>
-    <t>sadf asdfsadfg sdfg</t>
+    <t>77 Street</t>
+  </si>
+  <si>
+    <t>Kirilas</t>
   </si>
   <si>
     <t>Angola</t>
@@ -224,18 +224,15 @@
     <t>Antigua and Barbuda</t>
   </si>
   <si>
-    <t>zsdcxfv sdfy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdfgs dfgsdf gsdfghtyuk j </t>
+    <t>Hyper</t>
+  </si>
+  <si>
+    <t>Yimin</t>
   </si>
   <si>
     <t>Argentina</t>
   </si>
   <si>
-    <t>☐Separated ☐Others:</t>
-  </si>
-  <si>
     <t>Armenia</t>
   </si>
   <si>
@@ -254,10 +251,10 @@
     <t>HEIGHT (m)</t>
   </si>
   <si>
-    <t>fdsg sdfgsdfg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dsfg dfsghfdh </t>
+    <t>Jertopy</t>
+  </si>
+  <si>
+    <t>Saint Bernard</t>
   </si>
   <si>
     <t>Australia</t>
@@ -296,10 +293,10 @@
     <t>18. PERMANENT ADDRESS</t>
   </si>
   <si>
-    <t>AJAOSDJSADJASD</t>
-  </si>
-  <si>
-    <t>SAJDASDJLASKDJALSD</t>
+    <t>234 Street</t>
+  </si>
+  <si>
+    <t>Hilltop Zone</t>
   </si>
   <si>
     <t>Bahamas, The</t>
@@ -314,10 +311,10 @@
     <t>GSIS ID NO.</t>
   </si>
   <si>
-    <t>ewsdfcsdfsd</t>
-  </si>
-  <si>
-    <t>fsdfsdfsdf</t>
+    <t>Hello City</t>
+  </si>
+  <si>
+    <t>Malibago</t>
   </si>
   <si>
     <t>Bangladesh</t>
@@ -332,10 +329,10 @@
     <t>PAG-IBIG ID NO.</t>
   </si>
   <si>
-    <t>LKASJDLKASJDL</t>
-  </si>
-  <si>
-    <t>LASKJDLAKSJDLSA</t>
+    <t>San Juan</t>
+  </si>
+  <si>
+    <t>Southern Leyte</t>
   </si>
   <si>
     <t>Belarus</t>
@@ -362,7 +359,7 @@
     <t>19. TELEPHONE NO.</t>
   </si>
   <si>
-    <t>+1-808-201-0984</t>
+    <t>(737) 613-6857</t>
   </si>
   <si>
     <t>Benin</t>
@@ -374,7 +371,7 @@
     <t>20. MOBILE NO.</t>
   </si>
   <si>
-    <t>1-786-616-8834</t>
+    <t>09606623222</t>
   </si>
   <si>
     <t>Bhutan</t>
@@ -386,7 +383,7 @@
     <t>21. E-MAIL ADDRESS (if any)</t>
   </si>
   <si>
-    <t>drew.casper@example.net</t>
+    <t>hartmann.addison@example.net</t>
   </si>
   <si>
     <t>Bolivia</t>
@@ -404,9 +401,6 @@
     <t>SPOUSE'S SURNAME</t>
   </si>
   <si>
-    <t>zgsdfghsdfg h</t>
-  </si>
-  <si>
     <t>23. NAME of CHILDREN  (Write full name and list all)</t>
   </si>
   <si>
@@ -419,9 +413,6 @@
     <t xml:space="preserve">  FIRST NAME</t>
   </si>
   <si>
-    <t xml:space="preserve">3e5rtserdfgsdfg </t>
-  </si>
-  <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                     </t>
   </si>
   <si>
@@ -431,45 +422,30 @@
     <t xml:space="preserve">  MIDDLE NAME</t>
   </si>
   <si>
-    <t>sdfgsertwretasdf</t>
-  </si>
-  <si>
     <t>Brunei </t>
   </si>
   <si>
     <t>OCCUPATION</t>
   </si>
   <si>
-    <t>asdfawsera43w2er</t>
-  </si>
-  <si>
     <t>Bulgaria</t>
   </si>
   <si>
     <t>EMPLOYER/BUSINESS NAME</t>
   </si>
   <si>
-    <t>asdfasdf</t>
-  </si>
-  <si>
     <t>Burkina Faso</t>
   </si>
   <si>
     <t>BUSINESS ADDRESS</t>
   </si>
   <si>
-    <t>09123423789</t>
-  </si>
-  <si>
     <t>Burma</t>
   </si>
   <si>
     <t>TELEPHONE NO.</t>
   </si>
   <si>
-    <t>asdafafsdf sdasdf eefsdf</t>
-  </si>
-  <si>
     <t>Burundi</t>
   </si>
   <si>
@@ -479,24 +455,15 @@
     <t>FATHER'S SURNAME</t>
   </si>
   <si>
-    <t>dfghdfghdfgh</t>
-  </si>
-  <si>
     <t>Cambodia</t>
   </si>
   <si>
-    <t>asdasf sdg</t>
-  </si>
-  <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                                  </t>
   </si>
   <si>
     <t>Cameroon</t>
   </si>
   <si>
-    <t>dsgs dfghfsdhfgdh</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
@@ -509,19 +476,10 @@
     <t>Cape Verde</t>
   </si>
   <si>
-    <t>sdfgsdfgsdfg</t>
-  </si>
-  <si>
     <t>Central African Republic</t>
   </si>
   <si>
-    <t>dfghdfghdsrety</t>
-  </si>
-  <si>
     <t>Chad</t>
-  </si>
-  <si>
-    <t>sertyserygadfsg</t>
   </si>
   <si>
     <t>(Continue on separate sheet if necessary)</t>
@@ -582,15 +540,6 @@
     <t>ELEMENTARY</t>
   </si>
   <si>
-    <t>asdasdasdasd</t>
-  </si>
-  <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>asd asd</t>
-  </si>
-  <si>
     <t>Congo, Republic of the</t>
   </si>
   <si>
@@ -627,7 +576,7 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>08/30/2025</t>
+    <t>12/14/2025</t>
   </si>
   <si>
     <t>Cyprus</t>
@@ -1133,18 +1082,6 @@
 Validity</t>
   </si>
   <si>
-    <t>KASdlakdasdasd</t>
-  </si>
-  <si>
-    <t>12/23/2000</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
-    <t>03/02/2019</t>
-  </si>
-  <si>
     <t xml:space="preserve">V.  WORK EXPERIENCE </t>
   </si>
   <si>
@@ -1175,13 +1112,19 @@
     <t>GOV'T SERVICE                                                                                                                                       (Y/ N)</t>
   </si>
   <si>
-    <t>03/12/2001</t>
-  </si>
-  <si>
-    <t>03/12/2012</t>
-  </si>
-  <si>
-    <t>SAdasd</t>
+    <t>08/06/2025</t>
+  </si>
+  <si>
+    <t>03/14/2026</t>
+  </si>
+  <si>
+    <t>Junior Laravel Developer Intern</t>
+  </si>
+  <si>
+    <t>Laravel Department</t>
+  </si>
+  <si>
+    <t>Random</t>
   </si>
   <si>
     <t xml:space="preserve">                               CS FORM 212 (Revised 2017), Page 2 of 4</t>
@@ -1203,15 +1146,6 @@
   </si>
   <si>
     <t>POSITION / NATURE OF WORK</t>
-  </si>
-  <si>
-    <t>asdasdasd</t>
-  </si>
-  <si>
-    <t>02/01/2000</t>
-  </si>
-  <si>
-    <t>02/23/2004</t>
   </si>
   <si>
     <t>VII.  LEARNING AND DEVELOPMENT (L&amp;D) INTERVENTIONS/TRAINING PROGRAMS ATTENDED</t>
@@ -1234,18 +1168,6 @@
     <t xml:space="preserve"> CONDUCTED/ SPONSORED BY                                                               (Write in full)</t>
   </si>
   <si>
-    <t>aesfsdf</t>
-  </si>
-  <si>
-    <t>07/31/2025</t>
-  </si>
-  <si>
-    <t>08/27/2025</t>
-  </si>
-  <si>
-    <t>sdfsdf</t>
-  </si>
-  <si>
     <t>VIII.  OTHER INFORMATION</t>
   </si>
   <si>
@@ -1267,12 +1189,6 @@
     <t>MEMBERSHIP IN ASSOCIATION/ORGANIZATION                                                                                         (Write in full)</t>
   </si>
   <si>
-    <t>dsfgsdgfdg</t>
-  </si>
-  <si>
-    <t>sdfsdfdsf</t>
-  </si>
-  <si>
     <t xml:space="preserve"> CS FORM 212 (Revised 2017), Page 3 of 4</t>
   </si>
   <si>
@@ -1297,10 +1213,13 @@
     <t>b. within the fourth degree (for Local Government Unit - Career Employees)?</t>
   </si>
   <si>
+    <t>☐ Yes   ☑ No</t>
+  </si>
+  <si>
     <t xml:space="preserve">     If YES, give details: ________________________________  ________________________________</t>
   </si>
   <si>
-    <t>asdsad</t>
+    <t>asdasdasd</t>
   </si>
   <si>
     <t>35.</t>
@@ -1309,7 +1228,7 @@
     <t>a. Have you ever been found guilty of any administrative offense?</t>
   </si>
   <si>
-    <t>☐ Yes   ☑ No</t>
+    <t>asdasdas</t>
   </si>
   <si>
     <t xml:space="preserve">b. Have you been criminally charged before any court?
@@ -1401,6 +1320,9 @@
   </si>
   <si>
     <t>Are you a solo parent?</t>
+  </si>
+  <si>
+    <t>asdasd</t>
   </si>
   <si>
     <t>41.</t>
@@ -7417,9 +7339,7 @@
       <c r="A20" s="431"/>
       <c r="B20" s="228"/>
       <c r="C20" s="143"/>
-      <c r="D20" s="391" t="s">
-        <v>56</v>
-      </c>
+      <c r="D20" s="391"/>
       <c r="E20" s="392"/>
       <c r="F20" s="393"/>
       <c r="G20" s="154"/>
@@ -7431,7 +7351,7 @@
       <c r="M20" s="424"/>
       <c r="N20" s="427"/>
       <c r="Q20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:19" customHeight="1" ht="9">
@@ -7444,46 +7364,46 @@
       <c r="G21" s="154"/>
       <c r="H21" s="162"/>
       <c r="I21" s="428" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J21" s="429"/>
       <c r="K21" s="429"/>
       <c r="L21" s="328" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M21" s="329"/>
       <c r="N21" s="330"/>
       <c r="Q21" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:19" customHeight="1" ht="15.75">
       <c r="A22" s="433" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="404" t="s">
         <v>61</v>
-      </c>
-      <c r="B22" s="404" t="s">
-        <v>62</v>
       </c>
       <c r="C22" s="405"/>
       <c r="D22" s="397">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="E22" s="374"/>
       <c r="F22" s="398"/>
       <c r="G22" s="154"/>
       <c r="H22" s="162"/>
       <c r="I22" s="331" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J22" s="332"/>
       <c r="K22" s="332"/>
       <c r="L22" s="332" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M22" s="332"/>
       <c r="N22" s="333"/>
       <c r="Q22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:19" customHeight="1" ht="8.25">
@@ -7496,38 +7416,38 @@
       <c r="G23" s="154"/>
       <c r="H23" s="162"/>
       <c r="I23" s="336" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J23" s="337"/>
       <c r="K23" s="337"/>
       <c r="L23" s="334" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M23" s="334"/>
       <c r="N23" s="335"/>
       <c r="Q23" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:19" customHeight="1" ht="22.5">
       <c r="A24" s="172" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="408" t="s">
         <v>69</v>
-      </c>
-      <c r="B24" s="408" t="s">
-        <v>70</v>
       </c>
       <c r="C24" s="382"/>
       <c r="D24" s="415">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="E24" s="415"/>
       <c r="F24" s="415"/>
       <c r="G24" s="343" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H24" s="321"/>
       <c r="I24" s="344">
-        <v>234234</v>
+        <v>8834</v>
       </c>
       <c r="J24" s="345"/>
       <c r="K24" s="345"/>
@@ -7535,38 +7455,38 @@
       <c r="M24" s="345"/>
       <c r="N24" s="346"/>
       <c r="Q24" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:19" customHeight="1" ht="15.75">
       <c r="A25" s="402" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="404" t="s">
         <v>73</v>
-      </c>
-      <c r="B25" s="404" t="s">
-        <v>74</v>
       </c>
       <c r="C25" s="405"/>
       <c r="D25" s="374" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E25" s="374"/>
       <c r="F25" s="374"/>
       <c r="G25" s="114" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H25" s="103"/>
       <c r="I25" s="347" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J25" s="341"/>
       <c r="K25" s="341"/>
       <c r="L25" s="341" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M25" s="341"/>
       <c r="N25" s="342"/>
       <c r="Q25" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:19" customHeight="1" ht="9">
@@ -7589,36 +7509,36 @@
       <c r="M26" s="419"/>
       <c r="N26" s="420"/>
       <c r="Q26" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:19" customHeight="1" ht="15.75">
       <c r="A27" s="402" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="404" t="s">
         <v>81</v>
-      </c>
-      <c r="B27" s="404" t="s">
-        <v>82</v>
       </c>
       <c r="C27" s="405"/>
       <c r="D27" s="374">
-        <v>68802517806</v>
+        <v>63719383365</v>
       </c>
       <c r="E27" s="374"/>
       <c r="F27" s="374"/>
       <c r="G27" s="156"/>
       <c r="H27" s="109"/>
       <c r="I27" s="347" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J27" s="341"/>
       <c r="K27" s="341"/>
       <c r="L27" s="341" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M27" s="341"/>
       <c r="N27" s="342"/>
       <c r="Q27" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:19" customHeight="1" ht="9">
@@ -7631,46 +7551,46 @@
       <c r="G28" s="156"/>
       <c r="H28" s="109"/>
       <c r="I28" s="409" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J28" s="410"/>
       <c r="K28" s="410"/>
       <c r="L28" s="411" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M28" s="410"/>
       <c r="N28" s="412"/>
       <c r="Q28" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:19" customHeight="1" ht="15.75">
       <c r="A29" s="402" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="404" t="s">
         <v>87</v>
-      </c>
-      <c r="B29" s="404" t="s">
-        <v>88</v>
       </c>
       <c r="C29" s="405"/>
       <c r="D29" s="374">
-        <v>15613961801</v>
+        <v>49050253977</v>
       </c>
       <c r="E29" s="374"/>
       <c r="F29" s="374"/>
       <c r="G29" s="156"/>
       <c r="H29" s="165"/>
       <c r="I29" s="158" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J29" s="159"/>
       <c r="K29" s="159"/>
       <c r="L29" s="159" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M29" s="159"/>
       <c r="N29" s="177"/>
       <c r="Q29" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:19" customHeight="1" ht="9.75">
@@ -7683,38 +7603,38 @@
       <c r="G30" s="156"/>
       <c r="H30" s="165"/>
       <c r="I30" s="338" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J30" s="338"/>
       <c r="K30" s="338"/>
       <c r="L30" s="338" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M30" s="338"/>
       <c r="N30" s="339"/>
       <c r="Q30" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:19" customHeight="1" ht="24.75">
       <c r="A31" s="174" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="101" t="s">
         <v>93</v>
-      </c>
-      <c r="B31" s="101" t="s">
-        <v>94</v>
       </c>
       <c r="C31" s="102"/>
       <c r="D31" s="453">
-        <v>95549606079</v>
+        <v>27606717237</v>
       </c>
       <c r="E31" s="453"/>
       <c r="F31" s="453"/>
       <c r="G31" s="343" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H31" s="321"/>
       <c r="I31" s="336">
-        <v>2323</v>
+        <v>7712</v>
       </c>
       <c r="J31" s="337"/>
       <c r="K31" s="337"/>
@@ -7722,28 +7642,28 @@
       <c r="M31" s="328"/>
       <c r="N31" s="340"/>
       <c r="Q31" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:19" customHeight="1" ht="24.75">
       <c r="A32" s="172" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="101" t="s">
         <v>96</v>
-      </c>
-      <c r="B32" s="101" t="s">
-        <v>97</v>
       </c>
       <c r="C32" s="102"/>
       <c r="D32" s="415">
-        <v>8121145429</v>
+        <v>1234567890</v>
       </c>
       <c r="E32" s="415"/>
       <c r="F32" s="415"/>
       <c r="G32" s="153" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H32" s="157"/>
       <c r="I32" s="344" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J32" s="345"/>
       <c r="K32" s="345"/>
@@ -7751,26 +7671,26 @@
       <c r="M32" s="345"/>
       <c r="N32" s="346"/>
       <c r="Q32" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:19" customHeight="1" ht="24.75">
       <c r="A33" s="381" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B33" s="382"/>
       <c r="C33" s="383"/>
       <c r="D33" s="384">
-        <v>60289781281</v>
+        <v>123456789012</v>
       </c>
       <c r="E33" s="384"/>
       <c r="F33" s="384"/>
       <c r="G33" s="211" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H33" s="155"/>
       <c r="I33" s="344" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J33" s="345"/>
       <c r="K33" s="345"/>
@@ -7778,26 +7698,26 @@
       <c r="M33" s="345"/>
       <c r="N33" s="346"/>
       <c r="Q33" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:19" customHeight="1" ht="24.75">
       <c r="A34" s="178" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B34" s="230"/>
       <c r="C34" s="160"/>
       <c r="D34" s="374">
-        <v>2632359</v>
+        <v>3347651</v>
       </c>
       <c r="E34" s="374"/>
       <c r="F34" s="374"/>
       <c r="G34" s="114" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H34" s="103"/>
       <c r="I34" s="394" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J34" s="395"/>
       <c r="K34" s="395"/>
@@ -7805,12 +7725,12 @@
       <c r="M34" s="395"/>
       <c r="N34" s="396"/>
       <c r="Q34" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:19" customHeight="1" ht="16.5">
       <c r="A35" s="221" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" s="222"/>
       <c r="C35" s="222"/>
@@ -7826,51 +7746,51 @@
       <c r="M35" s="222"/>
       <c r="N35" s="223"/>
       <c r="Q35" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:19" customHeight="1" ht="21">
       <c r="A36" s="106" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="234" t="s">
         <v>111</v>
-      </c>
-      <c r="B36" s="234" t="s">
-        <v>112</v>
       </c>
       <c r="C36" s="235"/>
       <c r="D36" s="463" t="s">
-        <v>113</v>
+        <v>21</v>
       </c>
       <c r="E36" s="463"/>
       <c r="F36" s="463"/>
       <c r="G36" s="463"/>
       <c r="H36" s="463"/>
       <c r="I36" s="348" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J36" s="348"/>
       <c r="K36" s="348"/>
       <c r="L36" s="349"/>
       <c r="M36" s="364" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N36" s="365"/>
       <c r="Q36" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:19" customHeight="1" ht="21">
       <c r="A37" s="154"/>
       <c r="B37" s="109" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C37" s="165"/>
       <c r="D37" s="285" t="s">
-        <v>118</v>
+        <v>21</v>
       </c>
       <c r="E37" s="286"/>
       <c r="F37" s="287"/>
       <c r="G37" s="300" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H37" s="300" t="s">
         <v>21</v>
@@ -7886,17 +7806,17 @@
       </c>
       <c r="N37" s="282"/>
       <c r="Q37" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:19" customHeight="1" ht="21">
       <c r="A38" s="179"/>
       <c r="B38" s="226" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C38" s="225"/>
       <c r="D38" s="285" t="s">
-        <v>122</v>
+        <v>21</v>
       </c>
       <c r="E38" s="286"/>
       <c r="F38" s="286"/>
@@ -7909,17 +7829,17 @@
       <c r="M38" s="281"/>
       <c r="N38" s="282"/>
       <c r="Q38" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:19" customHeight="1" ht="21">
       <c r="A39" s="180"/>
       <c r="B39" s="101" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C39" s="102"/>
       <c r="D39" s="298" t="s">
-        <v>125</v>
+        <v>21</v>
       </c>
       <c r="E39" s="298"/>
       <c r="F39" s="298"/>
@@ -7932,17 +7852,17 @@
       <c r="M39" s="281"/>
       <c r="N39" s="282"/>
       <c r="Q39" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:19" customHeight="1" ht="21">
       <c r="A40" s="180"/>
       <c r="B40" s="101" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C40" s="102"/>
       <c r="D40" s="298" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="E40" s="298"/>
       <c r="F40" s="298"/>
@@ -7955,17 +7875,17 @@
       <c r="M40" s="281"/>
       <c r="N40" s="282"/>
       <c r="Q40" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:19" customHeight="1" ht="21">
       <c r="A41" s="180"/>
       <c r="B41" s="101" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C41" s="102"/>
       <c r="D41" s="298" t="s">
-        <v>131</v>
+        <v>21</v>
       </c>
       <c r="E41" s="298"/>
       <c r="F41" s="298"/>
@@ -7978,17 +7898,17 @@
       <c r="M41" s="281"/>
       <c r="N41" s="282"/>
       <c r="Q41" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:19" customHeight="1" ht="21">
       <c r="A42" s="107"/>
       <c r="B42" s="108" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C42" s="142"/>
       <c r="D42" s="298" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
       <c r="E42" s="298"/>
       <c r="F42" s="298"/>
@@ -8001,19 +7921,19 @@
       <c r="M42" s="281"/>
       <c r="N42" s="282"/>
       <c r="Q42" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:19" customHeight="1" ht="21">
       <c r="A43" s="224" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B43" s="231" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C43" s="108"/>
       <c r="D43" s="298" t="s">
-        <v>138</v>
+        <v>21</v>
       </c>
       <c r="E43" s="298"/>
       <c r="F43" s="298"/>
@@ -8026,7 +7946,7 @@
       <c r="M43" s="281"/>
       <c r="N43" s="282"/>
       <c r="Q43" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:19" customHeight="1" ht="21">
@@ -8036,12 +7956,12 @@
       </c>
       <c r="C44" s="162"/>
       <c r="D44" s="285" t="s">
-        <v>140</v>
+        <v>21</v>
       </c>
       <c r="E44" s="286"/>
       <c r="F44" s="287"/>
       <c r="G44" s="300" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="H44" s="300" t="s">
         <v>21</v>
@@ -8053,7 +7973,7 @@
       <c r="M44" s="281"/>
       <c r="N44" s="282"/>
       <c r="Q44" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:19" customHeight="1" ht="21">
@@ -8063,7 +7983,7 @@
       </c>
       <c r="C45" s="218"/>
       <c r="D45" s="285" t="s">
-        <v>143</v>
+        <v>21</v>
       </c>
       <c r="E45" s="286"/>
       <c r="F45" s="286"/>
@@ -8076,15 +7996,15 @@
       <c r="M45" s="281"/>
       <c r="N45" s="282"/>
       <c r="Q45" s="3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:19" customHeight="1" ht="21">
       <c r="A46" s="154" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B46" s="404" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C46" s="404"/>
       <c r="D46" s="404"/>
@@ -8099,7 +8019,7 @@
       <c r="M46" s="281"/>
       <c r="N46" s="282"/>
       <c r="Q46" s="3" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:19" customHeight="1" ht="21">
@@ -8109,7 +8029,7 @@
       </c>
       <c r="C47" s="162"/>
       <c r="D47" s="299" t="s">
-        <v>148</v>
+        <v>21</v>
       </c>
       <c r="E47" s="299"/>
       <c r="F47" s="299"/>
@@ -8122,7 +8042,7 @@
       <c r="M47" s="281"/>
       <c r="N47" s="282"/>
       <c r="Q47" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:19" customHeight="1" ht="21">
@@ -8132,7 +8052,7 @@
       </c>
       <c r="C48" s="162"/>
       <c r="D48" s="299" t="s">
-        <v>150</v>
+        <v>21</v>
       </c>
       <c r="E48" s="299"/>
       <c r="F48" s="299"/>
@@ -8145,7 +8065,7 @@
       <c r="M48" s="281"/>
       <c r="N48" s="282"/>
       <c r="Q48" s="3" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:19" customHeight="1" ht="21">
@@ -8155,14 +8075,14 @@
       </c>
       <c r="C49" s="220"/>
       <c r="D49" s="448" t="s">
-        <v>152</v>
+        <v>21</v>
       </c>
       <c r="E49" s="448"/>
       <c r="F49" s="448"/>
       <c r="G49" s="448"/>
       <c r="H49" s="448"/>
       <c r="I49" s="446" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="J49" s="446"/>
       <c r="K49" s="446"/>
@@ -8170,12 +8090,12 @@
       <c r="M49" s="446"/>
       <c r="N49" s="447"/>
       <c r="Q49" s="3" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:19" customHeight="1" ht="15.75">
       <c r="A50" s="182" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B50" s="182"/>
       <c r="C50" s="104"/>
@@ -8185,7 +8105,7 @@
       <c r="G50" s="105"/>
       <c r="H50" s="105"/>
       <c r="I50" s="372" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="J50" s="372"/>
       <c r="K50" s="372"/>
@@ -8193,42 +8113,42 @@
       <c r="M50" s="372"/>
       <c r="N50" s="373"/>
       <c r="Q50" s="3" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:19" customHeight="1" ht="14.25">
       <c r="A51" s="366" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B51" s="316" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C51" s="316"/>
       <c r="D51" s="301" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E51" s="302"/>
       <c r="F51" s="319"/>
       <c r="G51" s="301" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="H51" s="302"/>
       <c r="I51" s="303"/>
       <c r="J51" s="449" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="K51" s="450"/>
       <c r="L51" s="293" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="M51" s="368" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="N51" s="362" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:19" customHeight="1" ht="19.5">
@@ -8247,7 +8167,7 @@
       <c r="M52" s="368"/>
       <c r="N52" s="362"/>
       <c r="Q52" s="3" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:19" customHeight="1" ht="14.25">
@@ -8261,10 +8181,10 @@
       <c r="H53" s="308"/>
       <c r="I53" s="309"/>
       <c r="J53" s="110" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="K53" s="111" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="L53" s="294"/>
       <c r="M53" s="369"/>
@@ -8272,83 +8192,83 @@
       <c r="O53" s="112"/>
       <c r="P53" s="112"/>
       <c r="Q53" s="3" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:19" customHeight="1" ht="28.5">
       <c r="A54" s="238"/>
       <c r="B54" s="239" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C54" s="239"/>
       <c r="D54" s="322" t="s">
-        <v>172</v>
+        <v>21</v>
       </c>
       <c r="E54" s="323"/>
       <c r="F54" s="324"/>
       <c r="G54" s="295" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="H54" s="296"/>
       <c r="I54" s="297"/>
-      <c r="J54" s="26">
-        <v>5</v>
-      </c>
-      <c r="K54" s="232">
-        <v>5</v>
+      <c r="J54" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="K54" s="232" t="s">
+        <v>21</v>
       </c>
       <c r="L54" s="166" t="s">
-        <v>174</v>
-      </c>
-      <c r="M54" s="18">
-        <v>2002</v>
+        <v>21</v>
+      </c>
+      <c r="M54" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="N54" s="161" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:19" customHeight="1" ht="28.5">
       <c r="A55" s="238"/>
       <c r="B55" s="239" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="C55" s="239"/>
       <c r="D55" s="322" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="E55" s="323"/>
       <c r="F55" s="324"/>
       <c r="G55" s="295" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="H55" s="296"/>
       <c r="I55" s="297"/>
-      <c r="J55" s="26">
-        <v>4</v>
-      </c>
-      <c r="K55" s="27">
-        <v>200</v>
-      </c>
-      <c r="L55" s="242">
-        <v>2</v>
-      </c>
-      <c r="M55" s="19">
-        <v>2000</v>
+      <c r="J55" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="K55" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="L55" s="242" t="s">
+        <v>21</v>
+      </c>
+      <c r="M55" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="N55" s="161" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:19" customHeight="1" ht="28.5">
       <c r="A56" s="238"/>
       <c r="B56" s="239" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="C56" s="239"/>
       <c r="D56" s="322" t="s">
@@ -8377,13 +8297,13 @@
         <v>21</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:19" customHeight="1" ht="28.5">
       <c r="A57" s="238"/>
       <c r="B57" s="239" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="C57" s="239"/>
       <c r="D57" s="322" t="s">
@@ -8412,13 +8332,13 @@
         <v>21</v>
       </c>
       <c r="Q57" s="3" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:19" customHeight="1" ht="28.5">
       <c r="A58" s="240"/>
       <c r="B58" s="241" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C58" s="241"/>
       <c r="D58" s="325" t="s">
@@ -8447,12 +8367,12 @@
         <v>21</v>
       </c>
       <c r="Q58" s="3" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:19" customHeight="1" ht="12">
       <c r="A59" s="275" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B59" s="276"/>
       <c r="C59" s="276"/>
@@ -8468,12 +8388,12 @@
       <c r="M59" s="276"/>
       <c r="N59" s="277"/>
       <c r="Q59" s="3" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:19" customHeight="1" ht="27.75">
       <c r="A60" s="272" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="B60" s="273"/>
       <c r="C60" s="274"/>
@@ -8484,21 +8404,21 @@
       <c r="H60" s="289"/>
       <c r="I60" s="290"/>
       <c r="J60" s="291" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="K60" s="292"/>
       <c r="L60" s="278" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="M60" s="279"/>
       <c r="N60" s="280"/>
       <c r="Q60" s="3" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:19" customHeight="1" ht="12" s="147" customFormat="1">
       <c r="A61" s="271" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B61" s="271"/>
       <c r="C61" s="271"/>
@@ -8514,7 +8434,7 @@
       <c r="M61" s="271"/>
       <c r="N61" s="271"/>
       <c r="Q61" s="253" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:19" customHeight="1" ht="14.25">
@@ -8533,7 +8453,7 @@
       <c r="M62" s="113"/>
       <c r="N62" s="113"/>
       <c r="Q62" s="3" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:19" customHeight="1" ht="14.25">
@@ -8552,7 +8472,7 @@
       <c r="M63" s="113"/>
       <c r="N63" s="113"/>
       <c r="Q63" s="3" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:19" customHeight="1" ht="28.5">
@@ -8571,7 +8491,7 @@
       <c r="M64" s="113"/>
       <c r="N64" s="113"/>
       <c r="Q64" s="3" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65" spans="1:19" customHeight="1" ht="14.25">
@@ -8590,7 +8510,7 @@
       <c r="M65" s="113"/>
       <c r="N65" s="113"/>
       <c r="Q65" s="3" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:19" customHeight="1" ht="14.25">
@@ -8609,7 +8529,7 @@
       <c r="M66" s="113"/>
       <c r="N66" s="113"/>
       <c r="Q66" s="3" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:19" customHeight="1" ht="14.25">
@@ -8628,7 +8548,7 @@
       <c r="M67" s="113"/>
       <c r="N67" s="113"/>
       <c r="Q67" s="3" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" spans="1:19" customHeight="1" ht="14.25">
@@ -8647,7 +8567,7 @@
       <c r="M68" s="113"/>
       <c r="N68" s="113"/>
       <c r="Q68" s="3" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:19" customHeight="1" ht="28.5">
@@ -8666,7 +8586,7 @@
       <c r="M69" s="113"/>
       <c r="N69" s="113"/>
       <c r="Q69" s="3" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:19" customHeight="1" ht="14.25">
@@ -8685,7 +8605,7 @@
       <c r="M70" s="113"/>
       <c r="N70" s="113"/>
       <c r="Q70" s="3" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
     </row>
     <row r="71" spans="1:19" customHeight="1" ht="14.25">
@@ -8704,7 +8624,7 @@
       <c r="M71" s="113"/>
       <c r="N71" s="113"/>
       <c r="Q71" s="3" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:19" customHeight="1" ht="14.25">
@@ -8723,7 +8643,7 @@
       <c r="M72" s="113"/>
       <c r="N72" s="113"/>
       <c r="Q72" s="3" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
     </row>
     <row r="73" spans="1:19" customHeight="1" ht="14.25">
@@ -8742,7 +8662,7 @@
       <c r="M73" s="113"/>
       <c r="N73" s="113"/>
       <c r="Q73" s="3" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:19" customHeight="1" ht="14.25">
@@ -8761,7 +8681,7 @@
       <c r="M74" s="113"/>
       <c r="N74" s="113"/>
       <c r="Q74" s="3" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:19" customHeight="1" ht="14.25">
@@ -8780,7 +8700,7 @@
       <c r="M75" s="113"/>
       <c r="N75" s="113"/>
       <c r="Q75" s="3" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:19" customHeight="1" ht="14.25">
@@ -8799,7 +8719,7 @@
       <c r="M76" s="113"/>
       <c r="N76" s="113"/>
       <c r="Q76" s="3" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:19" customHeight="1" ht="14.25">
@@ -8818,7 +8738,7 @@
       <c r="M77" s="113"/>
       <c r="N77" s="113"/>
       <c r="Q77" s="3" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:19" customHeight="1" ht="14.25">
@@ -8837,7 +8757,7 @@
       <c r="M78" s="113"/>
       <c r="N78" s="113"/>
       <c r="Q78" s="3" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:19" customHeight="1" ht="14.25">
@@ -8856,7 +8776,7 @@
       <c r="M79" s="113"/>
       <c r="N79" s="113"/>
       <c r="Q79" s="3" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:19" customHeight="1" ht="14.25">
@@ -8875,7 +8795,7 @@
       <c r="M80" s="113"/>
       <c r="N80" s="113"/>
       <c r="Q80" s="3" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
     </row>
     <row r="81" spans="1:19" customHeight="1" ht="14.25">
@@ -8894,7 +8814,7 @@
       <c r="M81" s="113"/>
       <c r="N81" s="113"/>
       <c r="Q81" s="3" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:19" customHeight="1" ht="14.25">
@@ -8913,7 +8833,7 @@
       <c r="M82" s="113"/>
       <c r="N82" s="113"/>
       <c r="Q82" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="1:19" customHeight="1" ht="14.25">
@@ -8932,7 +8852,7 @@
       <c r="M83" s="113"/>
       <c r="N83" s="113"/>
       <c r="Q83" s="3" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" spans="1:19" customHeight="1" ht="14.25">
@@ -8951,7 +8871,7 @@
       <c r="M84" s="113"/>
       <c r="N84" s="113"/>
       <c r="Q84" s="3" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
     </row>
     <row r="85" spans="1:19" customHeight="1" ht="28.5">
@@ -8970,7 +8890,7 @@
       <c r="M85" s="113"/>
       <c r="N85" s="113"/>
       <c r="Q85" s="3" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="86" spans="1:19" customHeight="1" ht="14.25">
@@ -8989,7 +8909,7 @@
       <c r="M86" s="113"/>
       <c r="N86" s="113"/>
       <c r="Q86" s="3" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
     </row>
     <row r="87" spans="1:19" customHeight="1" ht="14.25">
@@ -9008,7 +8928,7 @@
       <c r="M87" s="113"/>
       <c r="N87" s="113"/>
       <c r="Q87" s="3" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
     </row>
     <row r="88" spans="1:19" customHeight="1" ht="14.25">
@@ -9027,7 +8947,7 @@
       <c r="M88" s="113"/>
       <c r="N88" s="113"/>
       <c r="Q88" s="3" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
     </row>
     <row r="89" spans="1:19" customHeight="1" ht="14.25">
@@ -9046,7 +8966,7 @@
       <c r="M89" s="113"/>
       <c r="N89" s="113"/>
       <c r="Q89" s="3" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:19" customHeight="1" ht="14.25">
@@ -9065,7 +8985,7 @@
       <c r="M90" s="113"/>
       <c r="N90" s="113"/>
       <c r="Q90" s="3" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
     </row>
     <row r="91" spans="1:19" customHeight="1" ht="14.25">
@@ -9084,7 +9004,7 @@
       <c r="M91" s="113"/>
       <c r="N91" s="113"/>
       <c r="Q91" s="3" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
     </row>
     <row r="92" spans="1:19" customHeight="1" ht="14.25">
@@ -9103,7 +9023,7 @@
       <c r="M92" s="113"/>
       <c r="N92" s="113"/>
       <c r="Q92" s="3" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="1:19" customHeight="1" ht="14.25">
@@ -9122,7 +9042,7 @@
       <c r="M93" s="113"/>
       <c r="N93" s="113"/>
       <c r="Q93" s="3" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" spans="1:19" customHeight="1" ht="14.25">
@@ -9141,7 +9061,7 @@
       <c r="M94" s="113"/>
       <c r="N94" s="113"/>
       <c r="Q94" s="3" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
     </row>
     <row r="95" spans="1:19" customHeight="1" ht="14.25">
@@ -9160,7 +9080,7 @@
       <c r="M95" s="113"/>
       <c r="N95" s="113"/>
       <c r="Q95" s="3" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
     </row>
     <row r="96" spans="1:19" customHeight="1" ht="14.25">
@@ -9179,7 +9099,7 @@
       <c r="M96" s="113"/>
       <c r="N96" s="113"/>
       <c r="Q96" s="3" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="97" spans="1:19" customHeight="1" ht="14.25">
@@ -9198,7 +9118,7 @@
       <c r="M97" s="113"/>
       <c r="N97" s="113"/>
       <c r="Q97" s="3" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
     </row>
     <row r="98" spans="1:19" customHeight="1" ht="14.25">
@@ -9217,7 +9137,7 @@
       <c r="M98" s="113"/>
       <c r="N98" s="113"/>
       <c r="Q98" s="3" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
     </row>
     <row r="99" spans="1:19" customHeight="1" ht="14.25">
@@ -9236,7 +9156,7 @@
       <c r="M99" s="113"/>
       <c r="N99" s="113"/>
       <c r="Q99" s="3" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
     </row>
     <row r="100" spans="1:19" customHeight="1" ht="14.25">
@@ -9255,7 +9175,7 @@
       <c r="M100" s="113"/>
       <c r="N100" s="113"/>
       <c r="Q100" s="3" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
     </row>
     <row r="101" spans="1:19" customHeight="1" ht="14.25">
@@ -9274,7 +9194,7 @@
       <c r="M101" s="113"/>
       <c r="N101" s="113"/>
       <c r="Q101" s="3" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
     </row>
     <row r="102" spans="1:19" customHeight="1" ht="14.25">
@@ -9293,7 +9213,7 @@
       <c r="M102" s="113"/>
       <c r="N102" s="113"/>
       <c r="Q102" s="3" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="103" spans="1:19" customHeight="1" ht="14.25">
@@ -9312,7 +9232,7 @@
       <c r="M103" s="113"/>
       <c r="N103" s="113"/>
       <c r="Q103" s="3" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
     </row>
     <row r="104" spans="1:19" customHeight="1" ht="14.25">
@@ -9331,7 +9251,7 @@
       <c r="M104" s="113"/>
       <c r="N104" s="113"/>
       <c r="Q104" s="3" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
     </row>
     <row r="105" spans="1:19" customHeight="1" ht="14.25">
@@ -9350,7 +9270,7 @@
       <c r="M105" s="113"/>
       <c r="N105" s="113"/>
       <c r="Q105" s="3" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
     </row>
     <row r="106" spans="1:19" customHeight="1" ht="14.25">
@@ -9369,7 +9289,7 @@
       <c r="M106" s="113"/>
       <c r="N106" s="113"/>
       <c r="Q106" s="3" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
     </row>
     <row r="107" spans="1:19" customHeight="1" ht="14.25">
@@ -9388,7 +9308,7 @@
       <c r="M107" s="113"/>
       <c r="N107" s="113"/>
       <c r="Q107" s="3" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
     </row>
     <row r="108" spans="1:19" customHeight="1" ht="14.25">
@@ -9407,7 +9327,7 @@
       <c r="M108" s="113"/>
       <c r="N108" s="113"/>
       <c r="Q108" s="3" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
     </row>
     <row r="109" spans="1:19" customHeight="1" ht="14.25">
@@ -9426,7 +9346,7 @@
       <c r="M109" s="113"/>
       <c r="N109" s="113"/>
       <c r="Q109" s="3" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
     </row>
     <row r="110" spans="1:19" customHeight="1" ht="14.25">
@@ -9445,7 +9365,7 @@
       <c r="M110" s="113"/>
       <c r="N110" s="113"/>
       <c r="Q110" s="3" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
     </row>
     <row r="111" spans="1:19" customHeight="1" ht="14.25">
@@ -9464,7 +9384,7 @@
       <c r="M111" s="113"/>
       <c r="N111" s="113"/>
       <c r="Q111" s="3" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
     </row>
     <row r="112" spans="1:19" customHeight="1" ht="14.25">
@@ -9483,7 +9403,7 @@
       <c r="M112" s="113"/>
       <c r="N112" s="113"/>
       <c r="Q112" s="3" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="113" spans="1:19" customHeight="1" ht="14.25">
@@ -9502,7 +9422,7 @@
       <c r="M113" s="113"/>
       <c r="N113" s="113"/>
       <c r="Q113" s="3" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
     <row r="114" spans="1:19" customHeight="1" ht="14.25">
@@ -9521,7 +9441,7 @@
       <c r="M114" s="113"/>
       <c r="N114" s="113"/>
       <c r="Q114" s="3" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
     <row r="115" spans="1:19" customHeight="1" ht="14.25">
@@ -9540,7 +9460,7 @@
       <c r="M115" s="113"/>
       <c r="N115" s="113"/>
       <c r="Q115" s="3" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
     </row>
     <row r="116" spans="1:19" customHeight="1" ht="14.25">
@@ -9559,7 +9479,7 @@
       <c r="M116" s="113"/>
       <c r="N116" s="113"/>
       <c r="Q116" s="3" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
     </row>
     <row r="117" spans="1:19" customHeight="1" ht="14.25">
@@ -9578,7 +9498,7 @@
       <c r="M117" s="113"/>
       <c r="N117" s="113"/>
       <c r="Q117" s="3" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="118" spans="1:19" customHeight="1" ht="14.25">
@@ -9597,7 +9517,7 @@
       <c r="M118" s="113"/>
       <c r="N118" s="113"/>
       <c r="Q118" s="3" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
     </row>
     <row r="119" spans="1:19" customHeight="1" ht="14.25">
@@ -9616,7 +9536,7 @@
       <c r="M119" s="113"/>
       <c r="N119" s="113"/>
       <c r="Q119" s="3" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
     </row>
     <row r="120" spans="1:19" customHeight="1" ht="14.25">
@@ -9635,7 +9555,7 @@
       <c r="M120" s="113"/>
       <c r="N120" s="113"/>
       <c r="Q120" s="3" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
     </row>
     <row r="121" spans="1:19" customHeight="1" ht="14.25">
@@ -9654,7 +9574,7 @@
       <c r="M121" s="113"/>
       <c r="N121" s="113"/>
       <c r="Q121" s="3" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
     </row>
     <row r="122" spans="1:19" customHeight="1" ht="14.25">
@@ -9673,7 +9593,7 @@
       <c r="M122" s="113"/>
       <c r="N122" s="113"/>
       <c r="Q122" s="3" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
     </row>
     <row r="123" spans="1:19" customHeight="1" ht="14.25">
@@ -9692,7 +9612,7 @@
       <c r="M123" s="113"/>
       <c r="N123" s="113"/>
       <c r="Q123" s="3" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
     </row>
     <row r="124" spans="1:19" customHeight="1" ht="14.25">
@@ -9711,7 +9631,7 @@
       <c r="M124" s="113"/>
       <c r="N124" s="113"/>
       <c r="Q124" s="3" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
     </row>
     <row r="125" spans="1:19" customHeight="1" ht="14.25">
@@ -9730,7 +9650,7 @@
       <c r="M125" s="113"/>
       <c r="N125" s="113"/>
       <c r="Q125" s="3" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
     </row>
     <row r="126" spans="1:19" customHeight="1" ht="14.25">
@@ -9749,7 +9669,7 @@
       <c r="M126" s="113"/>
       <c r="N126" s="113"/>
       <c r="Q126" s="3" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
     </row>
     <row r="127" spans="1:19" customHeight="1" ht="14.25">
@@ -9768,7 +9688,7 @@
       <c r="M127" s="113"/>
       <c r="N127" s="113"/>
       <c r="Q127" s="3" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
     </row>
     <row r="128" spans="1:19" customHeight="1" ht="28.5">
@@ -9787,7 +9707,7 @@
       <c r="M128" s="113"/>
       <c r="N128" s="113"/>
       <c r="Q128" s="3" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
     </row>
     <row r="129" spans="1:19" customHeight="1" ht="14.25">
@@ -9806,7 +9726,7 @@
       <c r="M129" s="113"/>
       <c r="N129" s="113"/>
       <c r="Q129" s="3" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
     </row>
     <row r="130" spans="1:19" customHeight="1" ht="14.25">
@@ -9825,7 +9745,7 @@
       <c r="M130" s="113"/>
       <c r="N130" s="113"/>
       <c r="Q130" s="3" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
     </row>
     <row r="131" spans="1:19" customHeight="1" ht="14.25">
@@ -9844,7 +9764,7 @@
       <c r="M131" s="113"/>
       <c r="N131" s="113"/>
       <c r="Q131" s="3" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
     </row>
     <row r="132" spans="1:19" customHeight="1" ht="14.25">
@@ -9863,7 +9783,7 @@
       <c r="M132" s="113"/>
       <c r="N132" s="113"/>
       <c r="Q132" s="3" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
     </row>
     <row r="133" spans="1:19" customHeight="1" ht="14.25">
@@ -9882,7 +9802,7 @@
       <c r="M133" s="113"/>
       <c r="N133" s="113"/>
       <c r="Q133" s="3" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
     </row>
     <row r="134" spans="1:19" customHeight="1" ht="14.25">
@@ -9901,7 +9821,7 @@
       <c r="M134" s="113"/>
       <c r="N134" s="113"/>
       <c r="Q134" s="3" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
     </row>
     <row r="135" spans="1:19" customHeight="1" ht="14.25">
@@ -9920,7 +9840,7 @@
       <c r="M135" s="113"/>
       <c r="N135" s="113"/>
       <c r="Q135" s="3" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
     </row>
     <row r="136" spans="1:19" customHeight="1" ht="14.25">
@@ -9939,7 +9859,7 @@
       <c r="M136" s="113"/>
       <c r="N136" s="113"/>
       <c r="Q136" s="3" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
     </row>
     <row r="137" spans="1:19" customHeight="1" ht="14.25">
@@ -9958,7 +9878,7 @@
       <c r="M137" s="113"/>
       <c r="N137" s="113"/>
       <c r="Q137" s="3" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
     </row>
     <row r="138" spans="1:19" customHeight="1" ht="14.25">
@@ -9977,7 +9897,7 @@
       <c r="M138" s="113"/>
       <c r="N138" s="113"/>
       <c r="Q138" s="3" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="139" spans="1:19" customHeight="1" ht="14.25">
@@ -9996,7 +9916,7 @@
       <c r="M139" s="113"/>
       <c r="N139" s="113"/>
       <c r="Q139" s="3" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
     </row>
     <row r="140" spans="1:19" customHeight="1" ht="14.25">
@@ -10015,7 +9935,7 @@
       <c r="M140" s="113"/>
       <c r="N140" s="113"/>
       <c r="Q140" s="3" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
     </row>
     <row r="141" spans="1:19" customHeight="1" ht="14.25">
@@ -10034,7 +9954,7 @@
       <c r="M141" s="113"/>
       <c r="N141" s="113"/>
       <c r="Q141" s="3" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
     </row>
     <row r="142" spans="1:19" customHeight="1" ht="14.25">
@@ -10053,7 +9973,7 @@
       <c r="M142" s="113"/>
       <c r="N142" s="113"/>
       <c r="Q142" s="3" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
     </row>
     <row r="143" spans="1:19" customHeight="1" ht="28.5">
@@ -10072,7 +9992,7 @@
       <c r="M143" s="113"/>
       <c r="N143" s="113"/>
       <c r="Q143" s="3" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
     </row>
     <row r="144" spans="1:19" customHeight="1" ht="14.25">
@@ -10091,7 +10011,7 @@
       <c r="M144" s="113"/>
       <c r="N144" s="113"/>
       <c r="Q144" s="3" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
     </row>
     <row r="145" spans="1:19" customHeight="1" ht="14.25">
@@ -10110,7 +10030,7 @@
       <c r="M145" s="113"/>
       <c r="N145" s="113"/>
       <c r="Q145" s="3" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
     </row>
     <row r="146" spans="1:19" customHeight="1" ht="14.25">
@@ -10129,7 +10049,7 @@
       <c r="M146" s="113"/>
       <c r="N146" s="113"/>
       <c r="Q146" s="3" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
     </row>
     <row r="147" spans="1:19" customHeight="1" ht="14.25">
@@ -10148,7 +10068,7 @@
       <c r="M147" s="113"/>
       <c r="N147" s="113"/>
       <c r="Q147" s="3" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
     </row>
     <row r="148" spans="1:19" customHeight="1" ht="14.25">
@@ -10167,7 +10087,7 @@
       <c r="M148" s="113"/>
       <c r="N148" s="113"/>
       <c r="Q148" s="3" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
     </row>
     <row r="149" spans="1:19" customHeight="1" ht="14.25">
@@ -10186,7 +10106,7 @@
       <c r="M149" s="113"/>
       <c r="N149" s="113"/>
       <c r="Q149" s="3" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
     <row r="150" spans="1:19" customHeight="1" ht="14.25">
@@ -10205,7 +10125,7 @@
       <c r="M150" s="113"/>
       <c r="N150" s="113"/>
       <c r="Q150" s="3" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="151" spans="1:19" customHeight="1" ht="14.25">
@@ -10224,7 +10144,7 @@
       <c r="M151" s="113"/>
       <c r="N151" s="113"/>
       <c r="Q151" s="3" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="152" spans="1:19" customHeight="1" ht="14.25">
@@ -10243,7 +10163,7 @@
       <c r="M152" s="113"/>
       <c r="N152" s="113"/>
       <c r="Q152" s="3" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="153" spans="1:19" customHeight="1" ht="28.5">
@@ -10262,7 +10182,7 @@
       <c r="M153" s="113"/>
       <c r="N153" s="113"/>
       <c r="Q153" s="3" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
     </row>
     <row r="154" spans="1:19" customHeight="1" ht="14.25">
@@ -10281,7 +10201,7 @@
       <c r="M154" s="113"/>
       <c r="N154" s="113"/>
       <c r="Q154" s="3" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
     </row>
     <row r="155" spans="1:19" customHeight="1" ht="28.5">
@@ -10300,7 +10220,7 @@
       <c r="M155" s="113"/>
       <c r="N155" s="113"/>
       <c r="Q155" s="3" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
     </row>
     <row r="156" spans="1:19" customHeight="1" ht="14.25">
@@ -10319,7 +10239,7 @@
       <c r="M156" s="113"/>
       <c r="N156" s="113"/>
       <c r="Q156" s="3" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
     </row>
     <row r="157" spans="1:19" customHeight="1" ht="14.25">
@@ -10338,7 +10258,7 @@
       <c r="M157" s="113"/>
       <c r="N157" s="113"/>
       <c r="Q157" s="3" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
     </row>
     <row r="158" spans="1:19" customHeight="1" ht="14.25">
@@ -10357,7 +10277,7 @@
       <c r="M158" s="113"/>
       <c r="N158" s="113"/>
       <c r="Q158" s="3" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
     </row>
     <row r="159" spans="1:19" customHeight="1" ht="14.25">
@@ -10376,7 +10296,7 @@
       <c r="M159" s="113"/>
       <c r="N159" s="113"/>
       <c r="Q159" s="3" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
     </row>
     <row r="160" spans="1:19" customHeight="1" ht="14.25">
@@ -10395,7 +10315,7 @@
       <c r="M160" s="113"/>
       <c r="N160" s="113"/>
       <c r="Q160" s="3" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
     </row>
     <row r="161" spans="1:19" customHeight="1" ht="14.25">
@@ -10414,7 +10334,7 @@
       <c r="M161" s="113"/>
       <c r="N161" s="113"/>
       <c r="Q161" s="3" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
     </row>
     <row r="162" spans="1:19" customHeight="1" ht="14.25">
@@ -10433,7 +10353,7 @@
       <c r="M162" s="113"/>
       <c r="N162" s="113"/>
       <c r="Q162" s="3" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
     </row>
     <row r="163" spans="1:19" customHeight="1" ht="14.25">
@@ -10452,7 +10372,7 @@
       <c r="M163" s="113"/>
       <c r="N163" s="113"/>
       <c r="Q163" s="3" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
     </row>
     <row r="164" spans="1:19" customHeight="1" ht="14.25">
@@ -10471,7 +10391,7 @@
       <c r="M164" s="113"/>
       <c r="N164" s="113"/>
       <c r="Q164" s="3" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
     </row>
     <row r="165" spans="1:19" customHeight="1" ht="28.5">
@@ -10490,7 +10410,7 @@
       <c r="M165" s="113"/>
       <c r="N165" s="113"/>
       <c r="Q165" s="3" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
     </row>
     <row r="166" spans="1:19" customHeight="1" ht="14.25">
@@ -10509,7 +10429,7 @@
       <c r="M166" s="113"/>
       <c r="N166" s="113"/>
       <c r="Q166" s="3" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
     </row>
     <row r="167" spans="1:19" customHeight="1" ht="42.75">
@@ -10528,7 +10448,7 @@
       <c r="M167" s="113"/>
       <c r="N167" s="113"/>
       <c r="Q167" s="3" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
     </row>
     <row r="168" spans="1:19" customHeight="1" ht="14.25">
@@ -10547,7 +10467,7 @@
       <c r="M168" s="113"/>
       <c r="N168" s="113"/>
       <c r="Q168" s="3" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
     </row>
     <row r="169" spans="1:19" customHeight="1" ht="14.25">
@@ -10566,7 +10486,7 @@
       <c r="M169" s="113"/>
       <c r="N169" s="113"/>
       <c r="Q169" s="3" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
     </row>
     <row r="170" spans="1:19" customHeight="1" ht="28.5">
@@ -10585,7 +10505,7 @@
       <c r="M170" s="113"/>
       <c r="N170" s="113"/>
       <c r="Q170" s="3" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
     </row>
     <row r="171" spans="1:19" customHeight="1" ht="14.25">
@@ -10604,7 +10524,7 @@
       <c r="M171" s="113"/>
       <c r="N171" s="113"/>
       <c r="Q171" s="3" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
     <row r="172" spans="1:19" customHeight="1" ht="14.25">
@@ -10623,7 +10543,7 @@
       <c r="M172" s="113"/>
       <c r="N172" s="113"/>
       <c r="Q172" s="3" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
     </row>
     <row r="173" spans="1:19" customHeight="1" ht="14.25">
@@ -10642,7 +10562,7 @@
       <c r="M173" s="113"/>
       <c r="N173" s="113"/>
       <c r="Q173" s="3" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
     </row>
     <row r="174" spans="1:19" customHeight="1" ht="14.25">
@@ -10661,7 +10581,7 @@
       <c r="M174" s="113"/>
       <c r="N174" s="113"/>
       <c r="Q174" s="3" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
     </row>
     <row r="175" spans="1:19" customHeight="1" ht="14.25">
@@ -10680,7 +10600,7 @@
       <c r="M175" s="113"/>
       <c r="N175" s="113"/>
       <c r="Q175" s="3" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
     </row>
     <row r="176" spans="1:19" customHeight="1" ht="14.25">
@@ -10699,7 +10619,7 @@
       <c r="M176" s="113"/>
       <c r="N176" s="113"/>
       <c r="Q176" s="3" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
     </row>
     <row r="177" spans="1:19" customHeight="1" ht="14.25">
@@ -10718,7 +10638,7 @@
       <c r="M177" s="113"/>
       <c r="N177" s="113"/>
       <c r="Q177" s="3" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
     </row>
     <row r="178" spans="1:19" customHeight="1" ht="14.25">
@@ -10737,7 +10657,7 @@
       <c r="M178" s="113"/>
       <c r="N178" s="113"/>
       <c r="Q178" s="3" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
     </row>
     <row r="179" spans="1:19" customHeight="1" ht="14.25">
@@ -10756,7 +10676,7 @@
       <c r="M179" s="113"/>
       <c r="N179" s="113"/>
       <c r="Q179" s="3" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
     </row>
     <row r="180" spans="1:19" customHeight="1" ht="28.5">
@@ -10775,7 +10695,7 @@
       <c r="M180" s="113"/>
       <c r="N180" s="113"/>
       <c r="Q180" s="3" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
     </row>
     <row r="181" spans="1:19" customHeight="1" ht="14.25">
@@ -10794,7 +10714,7 @@
       <c r="M181" s="113"/>
       <c r="N181" s="113"/>
       <c r="Q181" s="3" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
     </row>
     <row r="182" spans="1:19" customHeight="1" ht="14.25">
@@ -10813,7 +10733,7 @@
       <c r="M182" s="113"/>
       <c r="N182" s="113"/>
       <c r="Q182" s="3" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
     </row>
     <row r="183" spans="1:19" customHeight="1" ht="14.25">
@@ -10832,7 +10752,7 @@
       <c r="M183" s="113"/>
       <c r="N183" s="113"/>
       <c r="Q183" s="3" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
     </row>
     <row r="184" spans="1:19" customHeight="1" ht="14.25">
@@ -10851,7 +10771,7 @@
       <c r="M184" s="113"/>
       <c r="N184" s="113"/>
       <c r="Q184" s="3" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
     </row>
     <row r="185" spans="1:19" customHeight="1" ht="14.25">
@@ -10870,7 +10790,7 @@
       <c r="M185" s="113"/>
       <c r="N185" s="113"/>
       <c r="Q185" s="3" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
     </row>
     <row r="186" spans="1:19" customHeight="1" ht="14.25">
@@ -10889,7 +10809,7 @@
       <c r="M186" s="113"/>
       <c r="N186" s="113"/>
       <c r="Q186" s="3" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
     </row>
     <row r="187" spans="1:19" customHeight="1" ht="14.25">
@@ -10908,7 +10828,7 @@
       <c r="M187" s="113"/>
       <c r="N187" s="113"/>
       <c r="Q187" s="3" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
     </row>
     <row r="188" spans="1:19" customHeight="1" ht="14.25">
@@ -10927,7 +10847,7 @@
       <c r="M188" s="113"/>
       <c r="N188" s="113"/>
       <c r="Q188" s="3" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
     </row>
     <row r="189" spans="1:19" customHeight="1" ht="14.25">
@@ -10946,7 +10866,7 @@
       <c r="M189" s="113"/>
       <c r="N189" s="113"/>
       <c r="Q189" s="3" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
     </row>
     <row r="190" spans="1:19" customHeight="1" ht="14.25">
@@ -10965,7 +10885,7 @@
       <c r="M190" s="113"/>
       <c r="N190" s="113"/>
       <c r="Q190" s="3" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
     </row>
     <row r="191" spans="1:19" customHeight="1" ht="14.25">
@@ -10984,7 +10904,7 @@
       <c r="M191" s="113"/>
       <c r="N191" s="113"/>
       <c r="Q191" s="3" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
     </row>
     <row r="192" spans="1:19" customHeight="1" ht="14.25">
@@ -11003,7 +10923,7 @@
       <c r="M192" s="113"/>
       <c r="N192" s="113"/>
       <c r="Q192" s="3" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
     </row>
     <row r="193" spans="1:19" customHeight="1" ht="14.25">
@@ -11022,7 +10942,7 @@
       <c r="M193" s="113"/>
       <c r="N193" s="113"/>
       <c r="Q193" s="3" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
     </row>
     <row r="194" spans="1:19" customHeight="1" ht="14.25">
@@ -11041,7 +10961,7 @@
       <c r="M194" s="113"/>
       <c r="N194" s="113"/>
       <c r="Q194" s="3" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
     </row>
     <row r="195" spans="1:19" customHeight="1" ht="14.25">
@@ -11060,7 +10980,7 @@
       <c r="M195" s="113"/>
       <c r="N195" s="113"/>
       <c r="Q195" s="3" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
     </row>
     <row r="196" spans="1:19" customHeight="1" ht="14.25">
@@ -11079,7 +10999,7 @@
       <c r="M196" s="113"/>
       <c r="N196" s="113"/>
       <c r="Q196" s="3" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
     </row>
     <row r="197" spans="1:19" customHeight="1" ht="14.25">
@@ -11098,7 +11018,7 @@
       <c r="M197" s="113"/>
       <c r="N197" s="113"/>
       <c r="Q197" s="3" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
     </row>
     <row r="198" spans="1:19" customHeight="1" ht="14.25">
@@ -11117,7 +11037,7 @@
       <c r="M198" s="113"/>
       <c r="N198" s="113"/>
       <c r="Q198" s="3" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
     </row>
     <row r="199" spans="1:19" customHeight="1" ht="14.25">
@@ -11136,7 +11056,7 @@
       <c r="M199" s="113"/>
       <c r="N199" s="113"/>
       <c r="Q199" s="3" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
     </row>
     <row r="200" spans="1:19" customHeight="1" ht="28.5">
@@ -11155,7 +11075,7 @@
       <c r="M200" s="113"/>
       <c r="N200" s="113"/>
       <c r="Q200" s="3" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
     </row>
     <row r="201" spans="1:19" customHeight="1" ht="14.25">
@@ -11174,7 +11094,7 @@
       <c r="M201" s="113"/>
       <c r="N201" s="113"/>
       <c r="Q201" s="3" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
     </row>
     <row r="202" spans="1:19" customHeight="1" ht="14.25">
@@ -11193,7 +11113,7 @@
       <c r="M202" s="113"/>
       <c r="N202" s="113"/>
       <c r="Q202" s="3" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
     </row>
     <row r="203" spans="1:19" customHeight="1" ht="14.25">
@@ -11212,7 +11132,7 @@
       <c r="M203" s="113"/>
       <c r="N203" s="113"/>
       <c r="Q203" s="3" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
     </row>
     <row r="204" spans="1:19" customHeight="1" ht="14.25">
@@ -11231,7 +11151,7 @@
       <c r="M204" s="113"/>
       <c r="N204" s="113"/>
       <c r="Q204" s="3" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
     </row>
     <row r="205" spans="1:19" customHeight="1" ht="14.25">
@@ -11250,7 +11170,7 @@
       <c r="M205" s="113"/>
       <c r="N205" s="113"/>
       <c r="Q205" s="3" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
     </row>
     <row r="206" spans="1:19" customHeight="1" ht="14.25">
@@ -11269,7 +11189,7 @@
       <c r="M206" s="113"/>
       <c r="N206" s="113"/>
       <c r="Q206" s="3" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
     </row>
     <row r="207" spans="1:19" customHeight="1" ht="28.5">
@@ -11288,7 +11208,7 @@
       <c r="M207" s="113"/>
       <c r="N207" s="113"/>
       <c r="Q207" s="3" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
     </row>
     <row r="208" spans="1:19" customHeight="1" ht="28.5">
@@ -11307,7 +11227,7 @@
       <c r="M208" s="113"/>
       <c r="N208" s="113"/>
       <c r="Q208" s="3" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
     </row>
     <row r="209" spans="1:19" customHeight="1" ht="14.25">
@@ -11326,7 +11246,7 @@
       <c r="M209" s="113"/>
       <c r="N209" s="113"/>
       <c r="Q209" s="3" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
     </row>
     <row r="210" spans="1:19" customHeight="1" ht="14.25">
@@ -11345,7 +11265,7 @@
       <c r="M210" s="113"/>
       <c r="N210" s="113"/>
       <c r="Q210" s="3" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
     </row>
     <row r="211" spans="1:19" customHeight="1" ht="14.25">
@@ -11364,7 +11284,7 @@
       <c r="M211" s="113"/>
       <c r="N211" s="113"/>
       <c r="Q211" s="3" t="s">
-        <v>340</v>
+        <v>323</v>
       </c>
     </row>
     <row r="212" spans="1:19" customHeight="1" ht="14.25">
@@ -11383,7 +11303,7 @@
       <c r="M212" s="113"/>
       <c r="N212" s="113"/>
       <c r="Q212" s="3" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
     </row>
     <row r="213" spans="1:19" customHeight="1" ht="14.25">
@@ -11402,7 +11322,7 @@
       <c r="M213" s="113"/>
       <c r="N213" s="113"/>
       <c r="Q213" s="3" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
     </row>
     <row r="214" spans="1:19" customHeight="1" ht="14.25">
@@ -11421,7 +11341,7 @@
       <c r="M214" s="113"/>
       <c r="N214" s="113"/>
       <c r="Q214" s="3" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
     </row>
     <row r="215" spans="1:19" customHeight="1" ht="14.25">
@@ -11440,7 +11360,7 @@
       <c r="M215" s="113"/>
       <c r="N215" s="113"/>
       <c r="Q215" s="3" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
     </row>
     <row r="216" spans="1:19" customHeight="1" ht="14.25">
@@ -11459,7 +11379,7 @@
       <c r="M216" s="113"/>
       <c r="N216" s="113"/>
       <c r="Q216" s="3" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
     </row>
     <row r="217" spans="1:19">
@@ -12639,7 +12559,7 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="18">
       <c r="A2" s="490" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="B2" s="491"/>
       <c r="C2" s="491"/>
@@ -12656,28 +12576,28 @@
     </row>
     <row r="3" spans="1:14" customHeight="1" ht="15">
       <c r="A3" s="144" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="B3" s="480" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="C3" s="480"/>
       <c r="D3" s="480"/>
       <c r="E3" s="481"/>
       <c r="F3" s="488" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="G3" s="484" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="H3" s="481"/>
       <c r="I3" s="484" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="J3" s="480"/>
       <c r="K3" s="481"/>
       <c r="L3" s="486" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="M3" s="487"/>
     </row>
@@ -12694,37 +12614,37 @@
       <c r="J4" s="482"/>
       <c r="K4" s="483"/>
       <c r="L4" s="5" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:14" customHeight="1" ht="27">
       <c r="A5" s="497" t="s">
-        <v>355</v>
+        <v>21</v>
       </c>
       <c r="B5" s="498"/>
       <c r="C5" s="498"/>
       <c r="D5" s="498"/>
       <c r="E5" s="498"/>
-      <c r="F5" s="16">
-        <v>2323</v>
+      <c r="F5" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="G5" s="495" t="s">
-        <v>356</v>
+        <v>21</v>
       </c>
       <c r="H5" s="495"/>
       <c r="I5" s="496" t="s">
-        <v>357</v>
+        <v>21</v>
       </c>
       <c r="J5" s="496"/>
       <c r="K5" s="496"/>
-      <c r="L5" s="9">
-        <v>232321</v>
+      <c r="L5" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>358</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:14" customHeight="1" ht="27">
@@ -12819,7 +12739,7 @@
     </row>
     <row r="12" spans="1:14" customHeight="1" ht="12">
       <c r="A12" s="515" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B12" s="516"/>
       <c r="C12" s="516"/>
@@ -12836,7 +12756,7 @@
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="518" t="s">
-        <v>359</v>
+        <v>338</v>
       </c>
       <c r="B13" s="519"/>
       <c r="C13" s="519"/>
@@ -12853,7 +12773,7 @@
     </row>
     <row r="14" spans="1:14" customHeight="1" ht="12">
       <c r="A14" s="217" t="s">
-        <v>360</v>
+        <v>339</v>
       </c>
       <c r="B14" s="105"/>
       <c r="C14" s="105"/>
@@ -12870,33 +12790,33 @@
     </row>
     <row r="15" spans="1:14" customHeight="1" ht="18">
       <c r="A15" s="4" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
       <c r="B15" s="504" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="C15" s="505"/>
       <c r="D15" s="503" t="s">
-        <v>363</v>
+        <v>342</v>
       </c>
       <c r="E15" s="504"/>
       <c r="F15" s="505"/>
       <c r="G15" s="503" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
       <c r="H15" s="504"/>
       <c r="I15" s="505"/>
       <c r="J15" s="509" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
       <c r="K15" s="499" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="L15" s="524" t="s">
-        <v>367</v>
+        <v>346</v>
       </c>
       <c r="M15" s="493" t="s">
-        <v>368</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16" spans="1:14" customHeight="1" ht="15">
@@ -12916,11 +12836,11 @@
     </row>
     <row r="17" spans="1:14" customHeight="1" ht="18.75">
       <c r="A17" s="501" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B17" s="502"/>
       <c r="C17" s="8" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="D17" s="485"/>
       <c r="E17" s="482"/>
@@ -12935,30 +12855,30 @@
     </row>
     <row r="18" spans="1:14" customHeight="1" ht="24" s="13" customFormat="1">
       <c r="A18" s="511" t="s">
-        <v>369</v>
+        <v>348</v>
       </c>
       <c r="B18" s="512"/>
       <c r="C18" s="24" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="D18" s="498" t="s">
-        <v>371</v>
+        <v>350</v>
       </c>
       <c r="E18" s="498"/>
       <c r="F18" s="498"/>
       <c r="G18" s="498" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="H18" s="498"/>
       <c r="I18" s="498"/>
       <c r="J18" s="14">
-        <v>2312</v>
+        <v>25000</v>
       </c>
       <c r="K18" s="9">
-        <v>213</v>
+        <v>5</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="M18" s="10">
         <v>0</v>
@@ -13371,7 +13291,7 @@
     </row>
     <row r="46" spans="1:14" customHeight="1" ht="9.75">
       <c r="A46" s="526" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B46" s="527"/>
       <c r="C46" s="527"/>
@@ -13388,7 +13308,7 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="27.75">
       <c r="A47" s="272" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="B47" s="273"/>
       <c r="C47" s="274"/>
@@ -13398,10 +13318,10 @@
       <c r="G47" s="475"/>
       <c r="H47" s="476"/>
       <c r="I47" s="248" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="J47" s="249" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="K47" s="250"/>
       <c r="L47" s="250"/>
@@ -13410,7 +13330,7 @@
     </row>
     <row r="48" spans="1:14" customHeight="1" ht="9">
       <c r="A48" s="473" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
       <c r="B48" s="473"/>
       <c r="C48" s="473"/>
@@ -13614,7 +13534,7 @@
     </row>
     <row r="2" spans="1:13" customHeight="1" ht="22.5">
       <c r="A2" s="579" t="s">
-        <v>373</v>
+        <v>354</v>
       </c>
       <c r="B2" s="580"/>
       <c r="C2" s="580"/>
@@ -13629,22 +13549,22 @@
     </row>
     <row r="3" spans="1:13" customHeight="1" ht="15">
       <c r="A3" s="565" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
       <c r="B3" s="567" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="C3" s="567"/>
       <c r="D3" s="568"/>
       <c r="E3" s="480" t="s">
-        <v>376</v>
+        <v>357</v>
       </c>
       <c r="F3" s="481"/>
       <c r="G3" s="543" t="s">
-        <v>377</v>
+        <v>358</v>
       </c>
       <c r="H3" s="484" t="s">
-        <v>378</v>
+        <v>359</v>
       </c>
       <c r="I3" s="574"/>
       <c r="J3" s="574"/>
@@ -13669,10 +13589,10 @@
       <c r="C5" s="582"/>
       <c r="D5" s="583"/>
       <c r="E5" s="29" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="G5" s="500"/>
       <c r="H5" s="578"/>
@@ -13682,22 +13602,22 @@
     </row>
     <row r="6" spans="1:13" customHeight="1" ht="27.75">
       <c r="A6" s="540" t="s">
-        <v>379</v>
+        <v>21</v>
       </c>
       <c r="B6" s="541"/>
       <c r="C6" s="541"/>
       <c r="D6" s="542"/>
       <c r="E6" s="38" t="s">
-        <v>380</v>
+        <v>21</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>381</v>
-      </c>
-      <c r="G6" s="39">
-        <v>2342</v>
+        <v>21</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>21</v>
       </c>
       <c r="H6" s="544" t="s">
-        <v>379</v>
+        <v>21</v>
       </c>
       <c r="I6" s="545"/>
       <c r="J6" s="545"/>
@@ -13783,7 +13703,7 @@
     </row>
     <row r="13" spans="1:13" customHeight="1" ht="11.25">
       <c r="A13" s="515" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B13" s="516"/>
       <c r="C13" s="516"/>
@@ -13798,7 +13718,7 @@
     </row>
     <row r="14" spans="1:13" customHeight="1" ht="18">
       <c r="A14" s="587" t="s">
-        <v>382</v>
+        <v>360</v>
       </c>
       <c r="B14" s="588"/>
       <c r="C14" s="588"/>
@@ -13813,25 +13733,25 @@
     </row>
     <row r="15" spans="1:13" customHeight="1" ht="18">
       <c r="A15" s="566" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="B15" s="504" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
       <c r="C15" s="562"/>
       <c r="D15" s="563"/>
       <c r="E15" s="504" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="F15" s="505"/>
       <c r="G15" s="499" t="s">
-        <v>377</v>
+        <v>358</v>
       </c>
       <c r="H15" s="509" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
       <c r="I15" s="503" t="s">
-        <v>387</v>
+        <v>365</v>
       </c>
       <c r="J15" s="562"/>
       <c r="K15" s="577"/>
@@ -13855,10 +13775,10 @@
       <c r="C17" s="329"/>
       <c r="D17" s="564"/>
       <c r="E17" s="29" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="G17" s="500"/>
       <c r="H17" s="510"/>
@@ -13868,25 +13788,25 @@
     </row>
     <row r="18" spans="1:13" customHeight="1" ht="24.75">
       <c r="A18" s="547" t="s">
-        <v>388</v>
+        <v>21</v>
       </c>
       <c r="B18" s="548"/>
       <c r="C18" s="548"/>
       <c r="D18" s="549"/>
       <c r="E18" s="30" t="s">
-        <v>389</v>
+        <v>21</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>390</v>
-      </c>
-      <c r="G18" s="32">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>21</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>357</v>
+        <v>21</v>
       </c>
       <c r="I18" s="553" t="s">
-        <v>391</v>
+        <v>21</v>
       </c>
       <c r="J18" s="554"/>
       <c r="K18" s="555"/>
@@ -14153,7 +14073,7 @@
     </row>
     <row r="39" spans="1:13" customHeight="1" ht="13.5">
       <c r="A39" s="275" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B39" s="276"/>
       <c r="C39" s="276"/>
@@ -14168,7 +14088,7 @@
     </row>
     <row r="40" spans="1:13" customHeight="1" ht="22.5">
       <c r="A40" s="556" t="s">
-        <v>392</v>
+        <v>366</v>
       </c>
       <c r="B40" s="557"/>
       <c r="C40" s="557"/>
@@ -14183,26 +14103,26 @@
     </row>
     <row r="41" spans="1:13" customHeight="1" ht="33.75">
       <c r="A41" s="145" t="s">
-        <v>393</v>
+        <v>367</v>
       </c>
       <c r="B41" s="150" t="s">
-        <v>394</v>
+        <v>368</v>
       </c>
       <c r="C41" s="146" t="s">
-        <v>395</v>
+        <v>369</v>
       </c>
       <c r="D41" s="537" t="s">
-        <v>396</v>
+        <v>370</v>
       </c>
       <c r="E41" s="537"/>
       <c r="F41" s="537"/>
       <c r="G41" s="537"/>
       <c r="H41" s="538"/>
       <c r="I41" s="146" t="s">
-        <v>397</v>
+        <v>371</v>
       </c>
       <c r="J41" s="537" t="s">
-        <v>398</v>
+        <v>372</v>
       </c>
       <c r="K41" s="539"/>
     </row>
@@ -14212,23 +14132,23 @@
       </c>
       <c r="B42" s="533"/>
       <c r="C42" s="534" t="s">
-        <v>357</v>
+        <v>21</v>
       </c>
       <c r="D42" s="535"/>
       <c r="E42" s="535"/>
       <c r="F42" s="535"/>
       <c r="G42" s="535"/>
       <c r="H42" s="533"/>
-      <c r="I42" s="534"/>
+      <c r="I42" s="534" t="s">
+        <v>21</v>
+      </c>
       <c r="J42" s="535"/>
       <c r="K42" s="536"/>
     </row>
     <row r="43" spans="1:13" customHeight="1" ht="24.75">
       <c r="A43" s="532"/>
       <c r="B43" s="533"/>
-      <c r="C43" s="534" t="s">
-        <v>399</v>
-      </c>
+      <c r="C43" s="534"/>
       <c r="D43" s="535"/>
       <c r="E43" s="535"/>
       <c r="F43" s="535"/>
@@ -14247,9 +14167,7 @@
       <c r="F44" s="535"/>
       <c r="G44" s="535"/>
       <c r="H44" s="533"/>
-      <c r="I44" s="534" t="s">
-        <v>357</v>
-      </c>
+      <c r="I44" s="534"/>
       <c r="J44" s="535"/>
       <c r="K44" s="536"/>
     </row>
@@ -14262,9 +14180,7 @@
       <c r="F45" s="535"/>
       <c r="G45" s="535"/>
       <c r="H45" s="533"/>
-      <c r="I45" s="534" t="s">
-        <v>400</v>
-      </c>
+      <c r="I45" s="534"/>
       <c r="J45" s="535"/>
       <c r="K45" s="536"/>
     </row>
@@ -14309,7 +14225,7 @@
     </row>
     <row r="49" spans="1:13" customHeight="1" ht="11.25">
       <c r="A49" s="275" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B49" s="276"/>
       <c r="C49" s="276"/>
@@ -14324,7 +14240,7 @@
     </row>
     <row r="50" spans="1:13" customHeight="1" ht="28.5">
       <c r="A50" s="272" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="B50" s="274"/>
       <c r="C50" s="474"/>
@@ -14332,11 +14248,11 @@
       <c r="E50" s="475"/>
       <c r="F50" s="476"/>
       <c r="G50" s="530" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="H50" s="531"/>
       <c r="I50" s="474" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="J50" s="475"/>
       <c r="K50" s="476"/>
@@ -14345,7 +14261,7 @@
     </row>
     <row r="51" spans="1:13" customHeight="1" ht="9.75">
       <c r="K51" s="256" t="s">
-        <v>401</v>
+        <v>373</v>
       </c>
     </row>
     <row r="52" spans="1:13" customHeight="1" ht="3"/>
@@ -14496,11 +14412,11 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="13.5">
       <c r="A2" s="694" t="s">
-        <v>402</v>
+        <v>374</v>
       </c>
       <c r="B2" s="695"/>
       <c r="C2" s="721" t="s">
-        <v>403</v>
+        <v>375</v>
       </c>
       <c r="D2" s="721"/>
       <c r="E2" s="721"/>
@@ -14517,7 +14433,7 @@
       <c r="A3" s="44"/>
       <c r="B3" s="45"/>
       <c r="C3" s="710" t="s">
-        <v>404</v>
+        <v>376</v>
       </c>
       <c r="D3" s="710"/>
       <c r="E3" s="710"/>
@@ -14534,7 +14450,7 @@
       <c r="A4" s="44"/>
       <c r="B4" s="45"/>
       <c r="C4" s="710" t="s">
-        <v>405</v>
+        <v>377</v>
       </c>
       <c r="D4" s="710"/>
       <c r="E4" s="710"/>
@@ -14560,13 +14476,13 @@
       <c r="A6" s="44"/>
       <c r="B6" s="45"/>
       <c r="C6" s="710" t="s">
-        <v>406</v>
+        <v>378</v>
       </c>
       <c r="D6" s="710"/>
       <c r="E6" s="710"/>
       <c r="F6" s="711"/>
       <c r="G6" s="618" t="s">
-        <v>407</v>
+        <v>379</v>
       </c>
       <c r="H6" s="619"/>
       <c r="I6" s="619"/>
@@ -14592,13 +14508,13 @@
       <c r="A8" s="44"/>
       <c r="B8" s="45"/>
       <c r="C8" s="710" t="s">
-        <v>408</v>
+        <v>380</v>
       </c>
       <c r="D8" s="710"/>
       <c r="E8" s="710"/>
       <c r="F8" s="711"/>
       <c r="G8" s="618" t="s">
-        <v>407</v>
+        <v>381</v>
       </c>
       <c r="H8" s="619"/>
       <c r="I8" s="619"/>
@@ -14624,7 +14540,7 @@
       <c r="E10" s="710"/>
       <c r="F10" s="711"/>
       <c r="G10" s="601" t="s">
-        <v>409</v>
+        <v>382</v>
       </c>
       <c r="H10" s="601"/>
       <c r="I10" s="601"/>
@@ -14642,7 +14558,7 @@
       <c r="F11" s="711"/>
       <c r="G11" s="151"/>
       <c r="H11" s="715" t="s">
-        <v>410</v>
+        <v>383</v>
       </c>
       <c r="I11" s="715"/>
       <c r="J11" s="715"/>
@@ -14667,17 +14583,17 @@
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="733" t="s">
-        <v>411</v>
+        <v>384</v>
       </c>
       <c r="B13" s="734"/>
       <c r="C13" s="729" t="s">
-        <v>412</v>
+        <v>385</v>
       </c>
       <c r="D13" s="729"/>
       <c r="E13" s="562"/>
       <c r="F13" s="563"/>
       <c r="G13" s="615" t="s">
-        <v>413</v>
+        <v>379</v>
       </c>
       <c r="H13" s="616"/>
       <c r="I13" s="616"/>
@@ -14694,7 +14610,7 @@
       <c r="E14" s="562"/>
       <c r="F14" s="563"/>
       <c r="G14" s="600" t="s">
-        <v>409</v>
+        <v>382</v>
       </c>
       <c r="H14" s="601"/>
       <c r="I14" s="601"/>
@@ -14712,7 +14628,7 @@
       <c r="F15" s="563"/>
       <c r="G15" s="46"/>
       <c r="H15" s="735" t="s">
-        <v>21</v>
+        <v>386</v>
       </c>
       <c r="I15" s="735"/>
       <c r="J15" s="735"/>
@@ -14754,13 +14670,13 @@
       <c r="A18" s="55"/>
       <c r="B18" s="56"/>
       <c r="C18" s="603" t="s">
-        <v>414</v>
+        <v>387</v>
       </c>
       <c r="D18" s="603"/>
       <c r="E18" s="604"/>
       <c r="F18" s="605"/>
       <c r="G18" s="737" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="H18" s="738"/>
       <c r="I18" s="738"/>
@@ -14777,7 +14693,7 @@
       <c r="E19" s="604"/>
       <c r="F19" s="605"/>
       <c r="G19" s="600" t="s">
-        <v>409</v>
+        <v>382</v>
       </c>
       <c r="H19" s="601"/>
       <c r="I19" s="601"/>
@@ -14795,7 +14711,7 @@
       <c r="F20" s="605"/>
       <c r="G20" s="60"/>
       <c r="H20" s="742" t="s">
-        <v>415</v>
+        <v>388</v>
       </c>
       <c r="I20" s="742"/>
       <c r="J20" s="266"/>
@@ -14813,7 +14729,7 @@
       <c r="E21" s="604"/>
       <c r="F21" s="605"/>
       <c r="G21" s="743" t="s">
-        <v>416</v>
+        <v>389</v>
       </c>
       <c r="H21" s="744"/>
       <c r="I21" s="744"/>
@@ -14832,7 +14748,7 @@
       <c r="E22" s="606"/>
       <c r="F22" s="607"/>
       <c r="G22" s="130" t="s">
-        <v>417</v>
+        <v>390</v>
       </c>
       <c r="H22" s="257"/>
       <c r="I22" s="608"/>
@@ -14843,17 +14759,17 @@
     </row>
     <row r="23" spans="1:14" customHeight="1" ht="18">
       <c r="A23" s="596" t="s">
-        <v>418</v>
+        <v>391</v>
       </c>
       <c r="B23" s="597"/>
       <c r="C23" s="609" t="s">
-        <v>419</v>
+        <v>392</v>
       </c>
       <c r="D23" s="609"/>
       <c r="E23" s="609"/>
       <c r="F23" s="610"/>
       <c r="G23" s="615" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="H23" s="616"/>
       <c r="I23" s="616"/>
@@ -14870,7 +14786,7 @@
       <c r="E24" s="611"/>
       <c r="F24" s="612"/>
       <c r="G24" s="600" t="s">
-        <v>409</v>
+        <v>382</v>
       </c>
       <c r="H24" s="601"/>
       <c r="I24" s="601"/>
@@ -14913,17 +14829,17 @@
     </row>
     <row r="27" spans="1:14" customHeight="1" ht="14.25">
       <c r="A27" s="596" t="s">
-        <v>420</v>
+        <v>393</v>
       </c>
       <c r="B27" s="597"/>
       <c r="C27" s="609" t="s">
-        <v>421</v>
+        <v>394</v>
       </c>
       <c r="D27" s="609"/>
       <c r="E27" s="609"/>
       <c r="F27" s="610"/>
       <c r="G27" s="615" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="H27" s="616"/>
       <c r="I27" s="616"/>
@@ -14940,7 +14856,7 @@
       <c r="E28" s="611"/>
       <c r="F28" s="612"/>
       <c r="G28" s="600" t="s">
-        <v>409</v>
+        <v>382</v>
       </c>
       <c r="H28" s="601"/>
       <c r="I28" s="601"/>
@@ -14982,17 +14898,17 @@
     </row>
     <row r="31" spans="1:14" customHeight="1" ht="18">
       <c r="A31" s="596" t="s">
-        <v>422</v>
+        <v>395</v>
       </c>
       <c r="B31" s="597"/>
       <c r="C31" s="609" t="s">
-        <v>423</v>
+        <v>396</v>
       </c>
       <c r="D31" s="609"/>
       <c r="E31" s="609"/>
       <c r="F31" s="610"/>
       <c r="G31" s="615" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="H31" s="616"/>
       <c r="I31" s="616"/>
@@ -15009,7 +14925,7 @@
       <c r="E32" s="611"/>
       <c r="F32" s="612"/>
       <c r="G32" s="669" t="s">
-        <v>424</v>
+        <v>397</v>
       </c>
       <c r="H32" s="670"/>
       <c r="I32" s="670"/>
@@ -15039,13 +14955,13 @@
       <c r="A34" s="53"/>
       <c r="B34" s="54"/>
       <c r="C34" s="611" t="s">
-        <v>425</v>
+        <v>398</v>
       </c>
       <c r="D34" s="611"/>
       <c r="E34" s="611"/>
       <c r="F34" s="612"/>
       <c r="G34" s="671" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="H34" s="672"/>
       <c r="I34" s="672"/>
@@ -15062,7 +14978,7 @@
       <c r="E35" s="611"/>
       <c r="F35" s="612"/>
       <c r="G35" s="669" t="s">
-        <v>424</v>
+        <v>397</v>
       </c>
       <c r="H35" s="670"/>
       <c r="I35" s="670"/>
@@ -15089,17 +15005,17 @@
     </row>
     <row r="37" spans="1:14" customHeight="1" ht="18">
       <c r="A37" s="596" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
       <c r="B37" s="597"/>
       <c r="C37" s="727" t="s">
-        <v>427</v>
+        <v>400</v>
       </c>
       <c r="D37" s="727"/>
       <c r="E37" s="727"/>
       <c r="F37" s="728"/>
       <c r="G37" s="615" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="H37" s="616"/>
       <c r="I37" s="616"/>
@@ -15116,7 +15032,7 @@
       <c r="E38" s="729"/>
       <c r="F38" s="730"/>
       <c r="G38" s="600" t="s">
-        <v>428</v>
+        <v>401</v>
       </c>
       <c r="H38" s="601"/>
       <c r="I38" s="601"/>
@@ -15159,11 +15075,11 @@
     </row>
     <row r="41" spans="1:14" customHeight="1" ht="28.5">
       <c r="A41" s="724" t="s">
-        <v>429</v>
+        <v>402</v>
       </c>
       <c r="B41" s="725"/>
       <c r="C41" s="611" t="s">
-        <v>430</v>
+        <v>403</v>
       </c>
       <c r="D41" s="611"/>
       <c r="E41" s="611"/>
@@ -15193,17 +15109,17 @@
     </row>
     <row r="43" spans="1:14" customHeight="1" ht="13.5">
       <c r="A43" s="68" t="s">
-        <v>431</v>
+        <v>404</v>
       </c>
       <c r="B43" s="69"/>
       <c r="C43" s="611" t="s">
-        <v>432</v>
+        <v>405</v>
       </c>
       <c r="D43" s="611"/>
       <c r="E43" s="611"/>
       <c r="F43" s="612"/>
       <c r="G43" s="618" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="H43" s="619"/>
       <c r="I43" s="619"/>
@@ -15220,7 +15136,7 @@
       <c r="E44" s="611"/>
       <c r="F44" s="612"/>
       <c r="G44" s="198" t="s">
-        <v>433</v>
+        <v>406</v>
       </c>
       <c r="H44" s="259"/>
       <c r="I44" s="123"/>
@@ -15233,17 +15149,17 @@
     </row>
     <row r="45" spans="1:14" customHeight="1" ht="13.5">
       <c r="A45" s="68" t="s">
-        <v>434</v>
+        <v>407</v>
       </c>
       <c r="B45" s="69"/>
       <c r="C45" s="612" t="s">
-        <v>435</v>
+        <v>408</v>
       </c>
       <c r="D45" s="612"/>
       <c r="E45" s="612"/>
       <c r="F45" s="612"/>
       <c r="G45" s="618" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="H45" s="619"/>
       <c r="I45" s="619"/>
@@ -15260,7 +15176,7 @@
       <c r="E46" s="612"/>
       <c r="F46" s="612"/>
       <c r="G46" s="199" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
       <c r="H46" s="260"/>
       <c r="I46" s="123"/>
@@ -15274,17 +15190,17 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="13.5">
       <c r="A47" s="68" t="s">
-        <v>437</v>
+        <v>410</v>
       </c>
       <c r="B47" s="69"/>
       <c r="C47" s="611" t="s">
-        <v>438</v>
+        <v>411</v>
       </c>
       <c r="D47" s="611"/>
       <c r="E47" s="120"/>
       <c r="F47" s="121"/>
       <c r="G47" s="618" t="s">
-        <v>413</v>
+        <v>379</v>
       </c>
       <c r="H47" s="619"/>
       <c r="I47" s="619"/>
@@ -15301,14 +15217,14 @@
       <c r="E48" s="688"/>
       <c r="F48" s="689"/>
       <c r="G48" s="200" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
       <c r="H48" s="261"/>
       <c r="I48" s="125"/>
       <c r="J48" s="125"/>
       <c r="K48" s="125"/>
       <c r="L48" s="127" t="s">
-        <v>21</v>
+        <v>412</v>
       </c>
       <c r="M48" s="126"/>
       <c r="N48" s="75"/>
@@ -15331,11 +15247,11 @@
     </row>
     <row r="50" spans="1:14" customHeight="1" ht="23.25">
       <c r="A50" s="598" t="s">
-        <v>439</v>
+        <v>413</v>
       </c>
       <c r="B50" s="599"/>
       <c r="C50" s="196" t="s">
-        <v>440</v>
+        <v>414</v>
       </c>
       <c r="D50" s="196"/>
       <c r="E50" s="196"/>
@@ -15350,17 +15266,17 @@
     </row>
     <row r="51" spans="1:14" customHeight="1" ht="18">
       <c r="A51" s="684" t="s">
-        <v>441</v>
+        <v>415</v>
       </c>
       <c r="B51" s="685"/>
       <c r="C51" s="685"/>
       <c r="D51" s="685"/>
       <c r="E51" s="686"/>
       <c r="F51" s="187" t="s">
-        <v>442</v>
+        <v>416</v>
       </c>
       <c r="G51" s="693" t="s">
-        <v>443</v>
+        <v>417</v>
       </c>
       <c r="H51" s="537"/>
       <c r="I51" s="539"/>
@@ -15371,17 +15287,17 @@
     </row>
     <row r="52" spans="1:14" customHeight="1" ht="24">
       <c r="A52" s="703" t="s">
-        <v>357</v>
+        <v>21</v>
       </c>
       <c r="B52" s="704"/>
       <c r="C52" s="706"/>
       <c r="D52" s="706"/>
       <c r="E52" s="707"/>
       <c r="F52" s="76" t="s">
-        <v>357</v>
-      </c>
-      <c r="G52" s="696">
-        <v>232131</v>
+        <v>21</v>
+      </c>
+      <c r="G52" s="696" t="s">
+        <v>21</v>
       </c>
       <c r="H52" s="697"/>
       <c r="I52" s="698"/>
@@ -15422,11 +15338,11 @@
     </row>
     <row r="55" spans="1:14" customHeight="1" ht="39.75">
       <c r="A55" s="694" t="s">
-        <v>444</v>
+        <v>418</v>
       </c>
       <c r="B55" s="695"/>
       <c r="C55" s="708" t="s">
-        <v>445</v>
+        <v>419</v>
       </c>
       <c r="D55" s="708"/>
       <c r="E55" s="708"/>
@@ -15451,7 +15367,7 @@
       <c r="I56" s="263"/>
       <c r="J56" s="207"/>
       <c r="K56" s="680" t="s">
-        <v>446</v>
+        <v>420</v>
       </c>
       <c r="L56" s="680"/>
       <c r="M56" s="186"/>
@@ -15501,7 +15417,7 @@
     <row r="60" spans="1:14" customHeight="1" ht="25.5">
       <c r="A60" s="79"/>
       <c r="B60" s="661" t="s">
-        <v>447</v>
+        <v>421</v>
       </c>
       <c r="C60" s="662"/>
       <c r="D60" s="663"/>
@@ -15516,7 +15432,7 @@
     <row r="61" spans="1:14" customHeight="1" ht="20.25">
       <c r="A61" s="79"/>
       <c r="B61" s="648" t="s">
-        <v>448</v>
+        <v>422</v>
       </c>
       <c r="C61" s="649"/>
       <c r="D61" s="136"/>
@@ -15531,7 +15447,7 @@
     <row r="62" spans="1:14" customHeight="1" ht="9">
       <c r="A62" s="79"/>
       <c r="B62" s="636" t="s">
-        <v>449</v>
+        <v>423</v>
       </c>
       <c r="C62" s="637"/>
       <c r="D62" s="640"/>
@@ -15549,7 +15465,7 @@
       <c r="C63" s="651"/>
       <c r="D63" s="664"/>
       <c r="F63" s="665" t="s">
-        <v>450</v>
+        <v>424</v>
       </c>
       <c r="G63" s="666"/>
       <c r="H63" s="666"/>
@@ -15561,12 +15477,12 @@
     <row r="64" spans="1:14" customHeight="1" ht="10.5">
       <c r="A64" s="79"/>
       <c r="B64" s="636" t="s">
-        <v>451</v>
+        <v>425</v>
       </c>
       <c r="C64" s="637"/>
       <c r="D64" s="640"/>
       <c r="F64" s="81" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="G64" s="188"/>
       <c r="H64" s="188"/>
@@ -15582,14 +15498,14 @@
       <c r="C65" s="639"/>
       <c r="D65" s="641"/>
       <c r="F65" s="633" t="s">
-        <v>452</v>
+        <v>426</v>
       </c>
       <c r="G65" s="634"/>
       <c r="H65" s="634"/>
       <c r="I65" s="635"/>
       <c r="J65" s="82"/>
       <c r="K65" s="631" t="s">
-        <v>453</v>
+        <v>427</v>
       </c>
       <c r="L65" s="632"/>
       <c r="M65" s="80"/>
@@ -15611,7 +15527,7 @@
     </row>
     <row r="67" spans="1:14" customHeight="1" ht="28.5">
       <c r="A67" s="628" t="s">
-        <v>454</v>
+        <v>428</v>
       </c>
       <c r="B67" s="629"/>
       <c r="C67" s="629"/>
@@ -15646,7 +15562,7 @@
       <c r="C69" s="247"/>
       <c r="D69" s="247"/>
       <c r="E69" s="622" t="s">
-        <v>455</v>
+        <v>429</v>
       </c>
       <c r="F69" s="623"/>
       <c r="G69" s="623"/>
@@ -15674,7 +15590,7 @@
     </row>
     <row r="71" spans="1:14" customHeight="1" ht="10.5">
       <c r="A71" s="621" t="s">
-        <v>456</v>
+        <v>430</v>
       </c>
       <c r="B71" s="621"/>
       <c r="C71" s="621"/>
@@ -15853,35 +15769,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>457</v>
+        <v>431</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>458</v>
+        <v>432</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>459</v>
+        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>460</v>
+        <v>434</v>
       </c>
       <c r="B2" t="s">
-        <v>461</v>
+        <v>435</v>
       </c>
       <c r="C2" t="s">
-        <v>462</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>463</v>
+        <v>437</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>464</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -15891,7 +15807,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>465</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update personnel relations in controller and .env example
Refactored relation names in PersonnelController to match updated model relationships (e.g., 'education' to 'educations', 'familyBackground' to 'families', etc.). Updated .env.example with a sample APP_KEY and removed extra blank lines. Updated generated Excel report.
</commit_message>
<xml_diff>
--- a/public/report/pds_generated.xlsx
+++ b/public/report/pds_generated.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="419">
   <si>
     <t xml:space="preserve">        </t>
   </si>
@@ -103,19 +103,19 @@
     <t>SURNAME</t>
   </si>
   <si>
-    <t>Simonis</t>
+    <t>Moen</t>
   </si>
   <si>
     <t>FIRST NAME</t>
   </si>
   <si>
-    <t>Karlie</t>
+    <t>Cristina</t>
   </si>
   <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                           </t>
   </si>
   <si>
-    <t>Harley Gotardo</t>
+    <t>N/A</t>
   </si>
   <si>
     <t>Married</t>
@@ -127,7 +127,7 @@
     <t>MIDDLE NAME</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>Pascale</t>
   </si>
   <si>
     <t>Widow/er</t>
@@ -143,7 +143,7 @@
 (mm/dd/yyyy)  </t>
   </si>
   <si>
-    <t>1993-11-13</t>
+    <t>1978-01-20</t>
   </si>
   <si>
     <t>16. CITIZENSHIP</t>
@@ -164,7 +164,7 @@
     <t>PLACE OF BIRTH</t>
   </si>
   <si>
-    <t>Zulaufville</t>
+    <t>Port Jessycafort</t>
   </si>
   <si>
     <t xml:space="preserve">If holder of  dual citizenship, </t>
@@ -182,10 +182,10 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>Make ☐</t>
-  </si>
-  <si>
-    <t>Female ☑</t>
+    <t>Male ☑</t>
+  </si>
+  <si>
+    <t>Female ☐</t>
   </si>
   <si>
     <t>please indicate the details.</t>
@@ -200,18 +200,12 @@
     <t>CIVIL STATUS</t>
   </si>
   <si>
-    <t>☐Single ☐Married ☑Widowed</t>
+    <t>☐Single ☑Married ☐Widowed</t>
   </si>
   <si>
     <t>17. RESIDENTIAL ADDRESS</t>
   </si>
   <si>
-    <t>77 Street</t>
-  </si>
-  <si>
-    <t>Kirilas</t>
-  </si>
-  <si>
     <t>Angola</t>
   </si>
   <si>
@@ -224,15 +218,12 @@
     <t>Antigua and Barbuda</t>
   </si>
   <si>
-    <t>Hyper</t>
-  </si>
-  <si>
-    <t>Yimin</t>
-  </si>
-  <si>
     <t>Argentina</t>
   </si>
   <si>
+    <t>☐Separated ☐Others:</t>
+  </si>
+  <si>
     <t>Armenia</t>
   </si>
   <si>
@@ -251,12 +242,6 @@
     <t>HEIGHT (m)</t>
   </si>
   <si>
-    <t>Jertopy</t>
-  </si>
-  <si>
-    <t>Saint Bernard</t>
-  </si>
-  <si>
     <t>Australia</t>
   </si>
   <si>
@@ -293,12 +278,6 @@
     <t>18. PERMANENT ADDRESS</t>
   </si>
   <si>
-    <t>234 Street</t>
-  </si>
-  <si>
-    <t>Hilltop Zone</t>
-  </si>
-  <si>
     <t>Bahamas, The</t>
   </si>
   <si>
@@ -311,12 +290,6 @@
     <t>GSIS ID NO.</t>
   </si>
   <si>
-    <t>Hello City</t>
-  </si>
-  <si>
-    <t>Malibago</t>
-  </si>
-  <si>
     <t>Bangladesh</t>
   </si>
   <si>
@@ -329,12 +302,6 @@
     <t>PAG-IBIG ID NO.</t>
   </si>
   <si>
-    <t>San Juan</t>
-  </si>
-  <si>
-    <t>Southern Leyte</t>
-  </si>
-  <si>
     <t>Belarus</t>
   </si>
   <si>
@@ -359,7 +326,7 @@
     <t>19. TELEPHONE NO.</t>
   </si>
   <si>
-    <t>(737) 613-6857</t>
+    <t>+1-732-672-7585</t>
   </si>
   <si>
     <t>Benin</t>
@@ -371,7 +338,7 @@
     <t>20. MOBILE NO.</t>
   </si>
   <si>
-    <t>09606623222</t>
+    <t>(479) 970-1393</t>
   </si>
   <si>
     <t>Bhutan</t>
@@ -383,7 +350,7 @@
     <t>21. E-MAIL ADDRESS (if any)</t>
   </si>
   <si>
-    <t>hartmann.addison@example.net</t>
+    <t>rutherford.daren@example.com</t>
   </si>
   <si>
     <t>Bolivia</t>
@@ -576,7 +543,7 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>12/14/2025</t>
+    <t>12/16/2025</t>
   </si>
   <si>
     <t>Cyprus</t>
@@ -1110,21 +1077,6 @@
   </si>
   <si>
     <t>GOV'T SERVICE                                                                                                                                       (Y/ N)</t>
-  </si>
-  <si>
-    <t>08/06/2025</t>
-  </si>
-  <si>
-    <t>03/14/2026</t>
-  </si>
-  <si>
-    <t>Junior Laravel Developer Intern</t>
-  </si>
-  <si>
-    <t>Laravel Department</t>
-  </si>
-  <si>
-    <t>Random</t>
   </si>
   <si>
     <t xml:space="preserve">                               CS FORM 212 (Revised 2017), Page 2 of 4</t>
@@ -1207,28 +1159,16 @@
     <t>a. within the third degree?</t>
   </si>
   <si>
-    <t>☑ Yes   ☐ No</t>
-  </si>
-  <si>
     <t>b. within the fourth degree (for Local Government Unit - Career Employees)?</t>
   </si>
   <si>
-    <t>☐ Yes   ☑ No</t>
-  </si>
-  <si>
     <t xml:space="preserve">     If YES, give details: ________________________________  ________________________________</t>
   </si>
   <si>
-    <t>asdasdasd</t>
-  </si>
-  <si>
     <t>35.</t>
   </si>
   <si>
     <t>a. Have you ever been found guilty of any administrative offense?</t>
-  </si>
-  <si>
-    <t>asdasdas</t>
   </si>
   <si>
     <t xml:space="preserve">b. Have you been criminally charged before any court?
@@ -1320,9 +1260,6 @@
   </si>
   <si>
     <t>Are you a solo parent?</t>
-  </si>
-  <si>
-    <t>asdasd</t>
   </si>
   <si>
     <t>41.</t>
@@ -7276,17 +7213,17 @@
       </c>
       <c r="H17" s="108"/>
       <c r="I17" s="331" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="J17" s="332"/>
       <c r="K17" s="332"/>
       <c r="L17" s="332" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="M17" s="332"/>
       <c r="N17" s="333"/>
       <c r="Q17" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:19" customHeight="1" ht="9">
@@ -7299,17 +7236,17 @@
       <c r="G18" s="156"/>
       <c r="H18" s="109"/>
       <c r="I18" s="454" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J18" s="419"/>
       <c r="K18" s="419"/>
       <c r="L18" s="419" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M18" s="419"/>
       <c r="N18" s="420"/>
       <c r="Q18" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:19" customHeight="1" ht="5.25">
@@ -7322,24 +7259,26 @@
       <c r="G19" s="156"/>
       <c r="H19" s="109"/>
       <c r="I19" s="421" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="J19" s="422"/>
       <c r="K19" s="422"/>
       <c r="L19" s="425" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="M19" s="422"/>
       <c r="N19" s="426"/>
       <c r="Q19" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:19" customHeight="1" ht="9.75">
       <c r="A20" s="431"/>
       <c r="B20" s="228"/>
       <c r="C20" s="143"/>
-      <c r="D20" s="391"/>
+      <c r="D20" s="391" t="s">
+        <v>52</v>
+      </c>
       <c r="E20" s="392"/>
       <c r="F20" s="393"/>
       <c r="G20" s="154"/>
@@ -7351,7 +7290,7 @@
       <c r="M20" s="424"/>
       <c r="N20" s="427"/>
       <c r="Q20" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:19" customHeight="1" ht="9">
@@ -7364,46 +7303,46 @@
       <c r="G21" s="154"/>
       <c r="H21" s="162"/>
       <c r="I21" s="428" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J21" s="429"/>
       <c r="K21" s="429"/>
       <c r="L21" s="328" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M21" s="329"/>
       <c r="N21" s="330"/>
       <c r="Q21" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:19" customHeight="1" ht="15.75">
       <c r="A22" s="433" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" s="404" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C22" s="405"/>
       <c r="D22" s="397">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E22" s="374"/>
       <c r="F22" s="398"/>
       <c r="G22" s="154"/>
       <c r="H22" s="162"/>
       <c r="I22" s="331" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="J22" s="332"/>
       <c r="K22" s="332"/>
       <c r="L22" s="332" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="M22" s="332"/>
       <c r="N22" s="333"/>
       <c r="Q22" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:19" customHeight="1" ht="8.25">
@@ -7416,38 +7355,38 @@
       <c r="G23" s="154"/>
       <c r="H23" s="162"/>
       <c r="I23" s="336" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J23" s="337"/>
       <c r="K23" s="337"/>
       <c r="L23" s="334" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M23" s="334"/>
       <c r="N23" s="335"/>
       <c r="Q23" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:19" customHeight="1" ht="22.5">
       <c r="A24" s="172" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B24" s="408" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C24" s="382"/>
       <c r="D24" s="415">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E24" s="415"/>
       <c r="F24" s="415"/>
       <c r="G24" s="343" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H24" s="321"/>
-      <c r="I24" s="344">
-        <v>8834</v>
+      <c r="I24" s="344" t="s">
+        <v>17</v>
       </c>
       <c r="J24" s="345"/>
       <c r="K24" s="345"/>
@@ -7455,38 +7394,38 @@
       <c r="M24" s="345"/>
       <c r="N24" s="346"/>
       <c r="Q24" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:19" customHeight="1" ht="15.75">
       <c r="A25" s="402" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B25" s="404" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C25" s="405"/>
       <c r="D25" s="374" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E25" s="374"/>
       <c r="F25" s="374"/>
       <c r="G25" s="114" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H25" s="103"/>
       <c r="I25" s="347" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="J25" s="341"/>
       <c r="K25" s="341"/>
       <c r="L25" s="341" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="M25" s="341"/>
       <c r="N25" s="342"/>
       <c r="Q25" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:19" customHeight="1" ht="9">
@@ -7499,46 +7438,46 @@
       <c r="G26" s="154"/>
       <c r="H26" s="162"/>
       <c r="I26" s="454" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J26" s="419"/>
       <c r="K26" s="419"/>
       <c r="L26" s="419" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M26" s="419"/>
       <c r="N26" s="420"/>
       <c r="Q26" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:19" customHeight="1" ht="15.75">
       <c r="A27" s="402" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B27" s="404" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C27" s="405"/>
       <c r="D27" s="374">
-        <v>63719383365</v>
+        <v>12338687692</v>
       </c>
       <c r="E27" s="374"/>
       <c r="F27" s="374"/>
       <c r="G27" s="156"/>
       <c r="H27" s="109"/>
       <c r="I27" s="347" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="J27" s="341"/>
       <c r="K27" s="341"/>
       <c r="L27" s="341" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="M27" s="341"/>
       <c r="N27" s="342"/>
       <c r="Q27" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:19" customHeight="1" ht="9">
@@ -7551,46 +7490,46 @@
       <c r="G28" s="156"/>
       <c r="H28" s="109"/>
       <c r="I28" s="409" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J28" s="410"/>
       <c r="K28" s="410"/>
       <c r="L28" s="411" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M28" s="410"/>
       <c r="N28" s="412"/>
       <c r="Q28" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:19" customHeight="1" ht="15.75">
       <c r="A29" s="402" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B29" s="404" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C29" s="405"/>
       <c r="D29" s="374">
-        <v>49050253977</v>
+        <v>50256946020</v>
       </c>
       <c r="E29" s="374"/>
       <c r="F29" s="374"/>
       <c r="G29" s="156"/>
       <c r="H29" s="165"/>
       <c r="I29" s="158" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="J29" s="159"/>
       <c r="K29" s="159"/>
       <c r="L29" s="159" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="M29" s="159"/>
       <c r="N29" s="177"/>
       <c r="Q29" s="3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:19" customHeight="1" ht="9.75">
@@ -7603,38 +7542,38 @@
       <c r="G30" s="156"/>
       <c r="H30" s="165"/>
       <c r="I30" s="338" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J30" s="338"/>
       <c r="K30" s="338"/>
       <c r="L30" s="338" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M30" s="338"/>
       <c r="N30" s="339"/>
       <c r="Q30" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:19" customHeight="1" ht="24.75">
       <c r="A31" s="174" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B31" s="101" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C31" s="102"/>
       <c r="D31" s="453">
-        <v>27606717237</v>
+        <v>45496335892</v>
       </c>
       <c r="E31" s="453"/>
       <c r="F31" s="453"/>
       <c r="G31" s="343" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H31" s="321"/>
-      <c r="I31" s="336">
-        <v>7712</v>
+      <c r="I31" s="336" t="s">
+        <v>17</v>
       </c>
       <c r="J31" s="337"/>
       <c r="K31" s="337"/>
@@ -7642,28 +7581,28 @@
       <c r="M31" s="328"/>
       <c r="N31" s="340"/>
       <c r="Q31" s="3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:19" customHeight="1" ht="24.75">
       <c r="A32" s="172" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B32" s="101" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C32" s="102"/>
       <c r="D32" s="415">
-        <v>1234567890</v>
+        <v>6262025914</v>
       </c>
       <c r="E32" s="415"/>
       <c r="F32" s="415"/>
       <c r="G32" s="153" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="H32" s="157"/>
       <c r="I32" s="344" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="J32" s="345"/>
       <c r="K32" s="345"/>
@@ -7671,26 +7610,26 @@
       <c r="M32" s="345"/>
       <c r="N32" s="346"/>
       <c r="Q32" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:19" customHeight="1" ht="24.75">
       <c r="A33" s="381" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B33" s="382"/>
       <c r="C33" s="383"/>
       <c r="D33" s="384">
-        <v>123456789012</v>
+        <v>69987792505</v>
       </c>
       <c r="E33" s="384"/>
       <c r="F33" s="384"/>
       <c r="G33" s="211" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="H33" s="155"/>
       <c r="I33" s="344" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="J33" s="345"/>
       <c r="K33" s="345"/>
@@ -7698,26 +7637,26 @@
       <c r="M33" s="345"/>
       <c r="N33" s="346"/>
       <c r="Q33" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:19" customHeight="1" ht="24.75">
       <c r="A34" s="178" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B34" s="230"/>
       <c r="C34" s="160"/>
       <c r="D34" s="374">
-        <v>3347651</v>
+        <v>1829661</v>
       </c>
       <c r="E34" s="374"/>
       <c r="F34" s="374"/>
       <c r="G34" s="114" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="H34" s="103"/>
       <c r="I34" s="394" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="J34" s="395"/>
       <c r="K34" s="395"/>
@@ -7725,12 +7664,12 @@
       <c r="M34" s="395"/>
       <c r="N34" s="396"/>
       <c r="Q34" s="3" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:19" customHeight="1" ht="16.5">
       <c r="A35" s="221" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B35" s="222"/>
       <c r="C35" s="222"/>
@@ -7746,77 +7685,77 @@
       <c r="M35" s="222"/>
       <c r="N35" s="223"/>
       <c r="Q35" s="3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:19" customHeight="1" ht="21">
       <c r="A36" s="106" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B36" s="234" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C36" s="235"/>
       <c r="D36" s="463" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E36" s="463"/>
       <c r="F36" s="463"/>
       <c r="G36" s="463"/>
       <c r="H36" s="463"/>
       <c r="I36" s="348" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J36" s="348"/>
       <c r="K36" s="348"/>
       <c r="L36" s="349"/>
       <c r="M36" s="364" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="N36" s="365"/>
       <c r="Q36" s="3" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:19" customHeight="1" ht="21">
       <c r="A37" s="154"/>
       <c r="B37" s="109" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C37" s="165"/>
       <c r="D37" s="285" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E37" s="286"/>
       <c r="F37" s="287"/>
       <c r="G37" s="300" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H37" s="300" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I37" s="283" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J37" s="283"/>
       <c r="K37" s="283"/>
       <c r="L37" s="284"/>
       <c r="M37" s="281" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N37" s="282"/>
       <c r="Q37" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:19" customHeight="1" ht="21">
       <c r="A38" s="179"/>
       <c r="B38" s="226" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C38" s="225"/>
       <c r="D38" s="285" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E38" s="286"/>
       <c r="F38" s="286"/>
@@ -7829,17 +7768,17 @@
       <c r="M38" s="281"/>
       <c r="N38" s="282"/>
       <c r="Q38" s="3" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:19" customHeight="1" ht="21">
       <c r="A39" s="180"/>
       <c r="B39" s="101" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C39" s="102"/>
       <c r="D39" s="298" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E39" s="298"/>
       <c r="F39" s="298"/>
@@ -7852,17 +7791,17 @@
       <c r="M39" s="281"/>
       <c r="N39" s="282"/>
       <c r="Q39" s="3" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:19" customHeight="1" ht="21">
       <c r="A40" s="180"/>
       <c r="B40" s="101" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C40" s="102"/>
       <c r="D40" s="298" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E40" s="298"/>
       <c r="F40" s="298"/>
@@ -7875,17 +7814,17 @@
       <c r="M40" s="281"/>
       <c r="N40" s="282"/>
       <c r="Q40" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:19" customHeight="1" ht="21">
       <c r="A41" s="180"/>
       <c r="B41" s="101" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C41" s="102"/>
       <c r="D41" s="298" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E41" s="298"/>
       <c r="F41" s="298"/>
@@ -7898,17 +7837,17 @@
       <c r="M41" s="281"/>
       <c r="N41" s="282"/>
       <c r="Q41" s="3" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:19" customHeight="1" ht="21">
       <c r="A42" s="107"/>
       <c r="B42" s="108" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C42" s="142"/>
       <c r="D42" s="298" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E42" s="298"/>
       <c r="F42" s="298"/>
@@ -7921,19 +7860,19 @@
       <c r="M42" s="281"/>
       <c r="N42" s="282"/>
       <c r="Q42" s="3" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:19" customHeight="1" ht="21">
       <c r="A43" s="224" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B43" s="231" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C43" s="108"/>
       <c r="D43" s="298" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E43" s="298"/>
       <c r="F43" s="298"/>
@@ -7946,7 +7885,7 @@
       <c r="M43" s="281"/>
       <c r="N43" s="282"/>
       <c r="Q43" s="3" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:19" customHeight="1" ht="21">
@@ -7956,15 +7895,15 @@
       </c>
       <c r="C44" s="162"/>
       <c r="D44" s="285" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E44" s="286"/>
       <c r="F44" s="287"/>
       <c r="G44" s="300" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="H44" s="300" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I44" s="283"/>
       <c r="J44" s="283"/>
@@ -7973,7 +7912,7 @@
       <c r="M44" s="281"/>
       <c r="N44" s="282"/>
       <c r="Q44" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:19" customHeight="1" ht="21">
@@ -7983,7 +7922,7 @@
       </c>
       <c r="C45" s="218"/>
       <c r="D45" s="285" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E45" s="286"/>
       <c r="F45" s="286"/>
@@ -7996,15 +7935,15 @@
       <c r="M45" s="281"/>
       <c r="N45" s="282"/>
       <c r="Q45" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:19" customHeight="1" ht="21">
       <c r="A46" s="154" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B46" s="404" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C46" s="404"/>
       <c r="D46" s="404"/>
@@ -8019,7 +7958,7 @@
       <c r="M46" s="281"/>
       <c r="N46" s="282"/>
       <c r="Q46" s="3" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:19" customHeight="1" ht="21">
@@ -8029,7 +7968,7 @@
       </c>
       <c r="C47" s="162"/>
       <c r="D47" s="299" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E47" s="299"/>
       <c r="F47" s="299"/>
@@ -8042,7 +7981,7 @@
       <c r="M47" s="281"/>
       <c r="N47" s="282"/>
       <c r="Q47" s="3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:19" customHeight="1" ht="21">
@@ -8052,7 +7991,7 @@
       </c>
       <c r="C48" s="162"/>
       <c r="D48" s="299" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E48" s="299"/>
       <c r="F48" s="299"/>
@@ -8065,7 +8004,7 @@
       <c r="M48" s="281"/>
       <c r="N48" s="282"/>
       <c r="Q48" s="3" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:19" customHeight="1" ht="21">
@@ -8075,14 +8014,14 @@
       </c>
       <c r="C49" s="220"/>
       <c r="D49" s="448" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E49" s="448"/>
       <c r="F49" s="448"/>
       <c r="G49" s="448"/>
       <c r="H49" s="448"/>
       <c r="I49" s="446" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="J49" s="446"/>
       <c r="K49" s="446"/>
@@ -8090,12 +8029,12 @@
       <c r="M49" s="446"/>
       <c r="N49" s="447"/>
       <c r="Q49" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:19" customHeight="1" ht="15.75">
       <c r="A50" s="182" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B50" s="182"/>
       <c r="C50" s="104"/>
@@ -8105,7 +8044,7 @@
       <c r="G50" s="105"/>
       <c r="H50" s="105"/>
       <c r="I50" s="372" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="J50" s="372"/>
       <c r="K50" s="372"/>
@@ -8113,42 +8052,42 @@
       <c r="M50" s="372"/>
       <c r="N50" s="373"/>
       <c r="Q50" s="3" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:19" customHeight="1" ht="14.25">
       <c r="A51" s="366" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B51" s="316" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C51" s="316"/>
       <c r="D51" s="301" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E51" s="302"/>
       <c r="F51" s="319"/>
       <c r="G51" s="301" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="H51" s="302"/>
       <c r="I51" s="303"/>
       <c r="J51" s="449" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="K51" s="450"/>
       <c r="L51" s="293" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="M51" s="368" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="N51" s="362" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:19" customHeight="1" ht="19.5">
@@ -8167,7 +8106,7 @@
       <c r="M52" s="368"/>
       <c r="N52" s="362"/>
       <c r="Q52" s="3" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:19" customHeight="1" ht="14.25">
@@ -8181,10 +8120,10 @@
       <c r="H53" s="308"/>
       <c r="I53" s="309"/>
       <c r="J53" s="110" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="K53" s="111" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="L53" s="294"/>
       <c r="M53" s="369"/>
@@ -8192,187 +8131,187 @@
       <c r="O53" s="112"/>
       <c r="P53" s="112"/>
       <c r="Q53" s="3" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:19" customHeight="1" ht="28.5">
       <c r="A54" s="238"/>
       <c r="B54" s="239" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C54" s="239"/>
       <c r="D54" s="322" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E54" s="323"/>
       <c r="F54" s="324"/>
       <c r="G54" s="295" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H54" s="296"/>
       <c r="I54" s="297"/>
       <c r="J54" s="26" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K54" s="232" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L54" s="166" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M54" s="18" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N54" s="161" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:19" customHeight="1" ht="28.5">
       <c r="A55" s="238"/>
       <c r="B55" s="239" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C55" s="239"/>
       <c r="D55" s="322" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E55" s="323"/>
       <c r="F55" s="324"/>
       <c r="G55" s="295" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H55" s="296"/>
       <c r="I55" s="297"/>
       <c r="J55" s="26" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K55" s="27" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L55" s="242" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M55" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N55" s="161" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:19" customHeight="1" ht="28.5">
       <c r="A56" s="238"/>
       <c r="B56" s="239" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C56" s="239"/>
       <c r="D56" s="322" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E56" s="323"/>
       <c r="F56" s="324"/>
       <c r="G56" s="310" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H56" s="311"/>
       <c r="I56" s="312"/>
       <c r="J56" s="26" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K56" s="27" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L56" s="166" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M56" s="18" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N56" s="161" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:19" customHeight="1" ht="28.5">
       <c r="A57" s="238"/>
       <c r="B57" s="239" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C57" s="239"/>
       <c r="D57" s="322" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E57" s="323"/>
       <c r="F57" s="324"/>
       <c r="G57" s="310" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H57" s="311"/>
       <c r="I57" s="312"/>
       <c r="J57" s="26" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K57" s="27" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L57" s="166" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M57" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N57" s="161" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="Q57" s="3" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:19" customHeight="1" ht="28.5">
       <c r="A58" s="240"/>
       <c r="B58" s="241" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C58" s="241"/>
       <c r="D58" s="325" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E58" s="326"/>
       <c r="F58" s="327"/>
       <c r="G58" s="313" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H58" s="314"/>
       <c r="I58" s="315"/>
       <c r="J58" s="236" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K58" s="237" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L58" s="20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M58" s="21" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N58" s="161" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="Q58" s="3" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:19" customHeight="1" ht="12">
       <c r="A59" s="275" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B59" s="276"/>
       <c r="C59" s="276"/>
@@ -8388,12 +8327,12 @@
       <c r="M59" s="276"/>
       <c r="N59" s="277"/>
       <c r="Q59" s="3" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:19" customHeight="1" ht="27.75">
       <c r="A60" s="272" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B60" s="273"/>
       <c r="C60" s="274"/>
@@ -8404,21 +8343,21 @@
       <c r="H60" s="289"/>
       <c r="I60" s="290"/>
       <c r="J60" s="291" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="K60" s="292"/>
       <c r="L60" s="278" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="M60" s="279"/>
       <c r="N60" s="280"/>
       <c r="Q60" s="3" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:19" customHeight="1" ht="12" s="147" customFormat="1">
       <c r="A61" s="271" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B61" s="271"/>
       <c r="C61" s="271"/>
@@ -8434,7 +8373,7 @@
       <c r="M61" s="271"/>
       <c r="N61" s="271"/>
       <c r="Q61" s="253" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:19" customHeight="1" ht="14.25">
@@ -8453,7 +8392,7 @@
       <c r="M62" s="113"/>
       <c r="N62" s="113"/>
       <c r="Q62" s="3" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:19" customHeight="1" ht="14.25">
@@ -8472,7 +8411,7 @@
       <c r="M63" s="113"/>
       <c r="N63" s="113"/>
       <c r="Q63" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:19" customHeight="1" ht="28.5">
@@ -8491,7 +8430,7 @@
       <c r="M64" s="113"/>
       <c r="N64" s="113"/>
       <c r="Q64" s="3" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:19" customHeight="1" ht="14.25">
@@ -8510,7 +8449,7 @@
       <c r="M65" s="113"/>
       <c r="N65" s="113"/>
       <c r="Q65" s="3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="1:19" customHeight="1" ht="14.25">
@@ -8529,7 +8468,7 @@
       <c r="M66" s="113"/>
       <c r="N66" s="113"/>
       <c r="Q66" s="3" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:19" customHeight="1" ht="14.25">
@@ -8548,7 +8487,7 @@
       <c r="M67" s="113"/>
       <c r="N67" s="113"/>
       <c r="Q67" s="3" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="68" spans="1:19" customHeight="1" ht="14.25">
@@ -8567,7 +8506,7 @@
       <c r="M68" s="113"/>
       <c r="N68" s="113"/>
       <c r="Q68" s="3" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="69" spans="1:19" customHeight="1" ht="28.5">
@@ -8586,7 +8525,7 @@
       <c r="M69" s="113"/>
       <c r="N69" s="113"/>
       <c r="Q69" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:19" customHeight="1" ht="14.25">
@@ -8605,7 +8544,7 @@
       <c r="M70" s="113"/>
       <c r="N70" s="113"/>
       <c r="Q70" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:19" customHeight="1" ht="14.25">
@@ -8624,7 +8563,7 @@
       <c r="M71" s="113"/>
       <c r="N71" s="113"/>
       <c r="Q71" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="72" spans="1:19" customHeight="1" ht="14.25">
@@ -8643,7 +8582,7 @@
       <c r="M72" s="113"/>
       <c r="N72" s="113"/>
       <c r="Q72" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:19" customHeight="1" ht="14.25">
@@ -8662,7 +8601,7 @@
       <c r="M73" s="113"/>
       <c r="N73" s="113"/>
       <c r="Q73" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="74" spans="1:19" customHeight="1" ht="14.25">
@@ -8681,7 +8620,7 @@
       <c r="M74" s="113"/>
       <c r="N74" s="113"/>
       <c r="Q74" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="75" spans="1:19" customHeight="1" ht="14.25">
@@ -8700,7 +8639,7 @@
       <c r="M75" s="113"/>
       <c r="N75" s="113"/>
       <c r="Q75" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" spans="1:19" customHeight="1" ht="14.25">
@@ -8719,7 +8658,7 @@
       <c r="M76" s="113"/>
       <c r="N76" s="113"/>
       <c r="Q76" s="3" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="77" spans="1:19" customHeight="1" ht="14.25">
@@ -8738,7 +8677,7 @@
       <c r="M77" s="113"/>
       <c r="N77" s="113"/>
       <c r="Q77" s="3" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="78" spans="1:19" customHeight="1" ht="14.25">
@@ -8757,7 +8696,7 @@
       <c r="M78" s="113"/>
       <c r="N78" s="113"/>
       <c r="Q78" s="3" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:19" customHeight="1" ht="14.25">
@@ -8776,7 +8715,7 @@
       <c r="M79" s="113"/>
       <c r="N79" s="113"/>
       <c r="Q79" s="3" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:19" customHeight="1" ht="14.25">
@@ -8795,7 +8734,7 @@
       <c r="M80" s="113"/>
       <c r="N80" s="113"/>
       <c r="Q80" s="3" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:19" customHeight="1" ht="14.25">
@@ -8814,7 +8753,7 @@
       <c r="M81" s="113"/>
       <c r="N81" s="113"/>
       <c r="Q81" s="3" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="82" spans="1:19" customHeight="1" ht="14.25">
@@ -8833,7 +8772,7 @@
       <c r="M82" s="113"/>
       <c r="N82" s="113"/>
       <c r="Q82" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:19" customHeight="1" ht="14.25">
@@ -8852,7 +8791,7 @@
       <c r="M83" s="113"/>
       <c r="N83" s="113"/>
       <c r="Q83" s="3" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="84" spans="1:19" customHeight="1" ht="14.25">
@@ -8871,7 +8810,7 @@
       <c r="M84" s="113"/>
       <c r="N84" s="113"/>
       <c r="Q84" s="3" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" spans="1:19" customHeight="1" ht="28.5">
@@ -8890,7 +8829,7 @@
       <c r="M85" s="113"/>
       <c r="N85" s="113"/>
       <c r="Q85" s="3" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="86" spans="1:19" customHeight="1" ht="14.25">
@@ -8909,7 +8848,7 @@
       <c r="M86" s="113"/>
       <c r="N86" s="113"/>
       <c r="Q86" s="3" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="87" spans="1:19" customHeight="1" ht="14.25">
@@ -8928,7 +8867,7 @@
       <c r="M87" s="113"/>
       <c r="N87" s="113"/>
       <c r="Q87" s="3" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="88" spans="1:19" customHeight="1" ht="14.25">
@@ -8947,7 +8886,7 @@
       <c r="M88" s="113"/>
       <c r="N88" s="113"/>
       <c r="Q88" s="3" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="89" spans="1:19" customHeight="1" ht="14.25">
@@ -8966,7 +8905,7 @@
       <c r="M89" s="113"/>
       <c r="N89" s="113"/>
       <c r="Q89" s="3" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="90" spans="1:19" customHeight="1" ht="14.25">
@@ -8985,7 +8924,7 @@
       <c r="M90" s="113"/>
       <c r="N90" s="113"/>
       <c r="Q90" s="3" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="91" spans="1:19" customHeight="1" ht="14.25">
@@ -9004,7 +8943,7 @@
       <c r="M91" s="113"/>
       <c r="N91" s="113"/>
       <c r="Q91" s="3" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="92" spans="1:19" customHeight="1" ht="14.25">
@@ -9023,7 +8962,7 @@
       <c r="M92" s="113"/>
       <c r="N92" s="113"/>
       <c r="Q92" s="3" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93" spans="1:19" customHeight="1" ht="14.25">
@@ -9042,7 +8981,7 @@
       <c r="M93" s="113"/>
       <c r="N93" s="113"/>
       <c r="Q93" s="3" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="94" spans="1:19" customHeight="1" ht="14.25">
@@ -9061,7 +9000,7 @@
       <c r="M94" s="113"/>
       <c r="N94" s="113"/>
       <c r="Q94" s="3" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:19" customHeight="1" ht="14.25">
@@ -9080,7 +9019,7 @@
       <c r="M95" s="113"/>
       <c r="N95" s="113"/>
       <c r="Q95" s="3" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="96" spans="1:19" customHeight="1" ht="14.25">
@@ -9099,7 +9038,7 @@
       <c r="M96" s="113"/>
       <c r="N96" s="113"/>
       <c r="Q96" s="3" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:19" customHeight="1" ht="14.25">
@@ -9118,7 +9057,7 @@
       <c r="M97" s="113"/>
       <c r="N97" s="113"/>
       <c r="Q97" s="3" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="98" spans="1:19" customHeight="1" ht="14.25">
@@ -9137,7 +9076,7 @@
       <c r="M98" s="113"/>
       <c r="N98" s="113"/>
       <c r="Q98" s="3" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="99" spans="1:19" customHeight="1" ht="14.25">
@@ -9156,7 +9095,7 @@
       <c r="M99" s="113"/>
       <c r="N99" s="113"/>
       <c r="Q99" s="3" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:19" customHeight="1" ht="14.25">
@@ -9175,7 +9114,7 @@
       <c r="M100" s="113"/>
       <c r="N100" s="113"/>
       <c r="Q100" s="3" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
     </row>
     <row r="101" spans="1:19" customHeight="1" ht="14.25">
@@ -9194,7 +9133,7 @@
       <c r="M101" s="113"/>
       <c r="N101" s="113"/>
       <c r="Q101" s="3" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="102" spans="1:19" customHeight="1" ht="14.25">
@@ -9213,7 +9152,7 @@
       <c r="M102" s="113"/>
       <c r="N102" s="113"/>
       <c r="Q102" s="3" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:19" customHeight="1" ht="14.25">
@@ -9232,7 +9171,7 @@
       <c r="M103" s="113"/>
       <c r="N103" s="113"/>
       <c r="Q103" s="3" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="104" spans="1:19" customHeight="1" ht="14.25">
@@ -9251,7 +9190,7 @@
       <c r="M104" s="113"/>
       <c r="N104" s="113"/>
       <c r="Q104" s="3" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="105" spans="1:19" customHeight="1" ht="14.25">
@@ -9270,7 +9209,7 @@
       <c r="M105" s="113"/>
       <c r="N105" s="113"/>
       <c r="Q105" s="3" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="106" spans="1:19" customHeight="1" ht="14.25">
@@ -9289,7 +9228,7 @@
       <c r="M106" s="113"/>
       <c r="N106" s="113"/>
       <c r="Q106" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="107" spans="1:19" customHeight="1" ht="14.25">
@@ -9308,7 +9247,7 @@
       <c r="M107" s="113"/>
       <c r="N107" s="113"/>
       <c r="Q107" s="3" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="108" spans="1:19" customHeight="1" ht="14.25">
@@ -9327,7 +9266,7 @@
       <c r="M108" s="113"/>
       <c r="N108" s="113"/>
       <c r="Q108" s="3" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="109" spans="1:19" customHeight="1" ht="14.25">
@@ -9346,7 +9285,7 @@
       <c r="M109" s="113"/>
       <c r="N109" s="113"/>
       <c r="Q109" s="3" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="110" spans="1:19" customHeight="1" ht="14.25">
@@ -9365,7 +9304,7 @@
       <c r="M110" s="113"/>
       <c r="N110" s="113"/>
       <c r="Q110" s="3" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:19" customHeight="1" ht="14.25">
@@ -9384,7 +9323,7 @@
       <c r="M111" s="113"/>
       <c r="N111" s="113"/>
       <c r="Q111" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="112" spans="1:19" customHeight="1" ht="14.25">
@@ -9403,7 +9342,7 @@
       <c r="M112" s="113"/>
       <c r="N112" s="113"/>
       <c r="Q112" s="3" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="113" spans="1:19" customHeight="1" ht="14.25">
@@ -9422,7 +9361,7 @@
       <c r="M113" s="113"/>
       <c r="N113" s="113"/>
       <c r="Q113" s="3" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="114" spans="1:19" customHeight="1" ht="14.25">
@@ -9441,7 +9380,7 @@
       <c r="M114" s="113"/>
       <c r="N114" s="113"/>
       <c r="Q114" s="3" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="115" spans="1:19" customHeight="1" ht="14.25">
@@ -9460,7 +9399,7 @@
       <c r="M115" s="113"/>
       <c r="N115" s="113"/>
       <c r="Q115" s="3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="116" spans="1:19" customHeight="1" ht="14.25">
@@ -9479,7 +9418,7 @@
       <c r="M116" s="113"/>
       <c r="N116" s="113"/>
       <c r="Q116" s="3" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="117" spans="1:19" customHeight="1" ht="14.25">
@@ -9498,7 +9437,7 @@
       <c r="M117" s="113"/>
       <c r="N117" s="113"/>
       <c r="Q117" s="3" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="118" spans="1:19" customHeight="1" ht="14.25">
@@ -9517,7 +9456,7 @@
       <c r="M118" s="113"/>
       <c r="N118" s="113"/>
       <c r="Q118" s="3" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="119" spans="1:19" customHeight="1" ht="14.25">
@@ -9536,7 +9475,7 @@
       <c r="M119" s="113"/>
       <c r="N119" s="113"/>
       <c r="Q119" s="3" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="120" spans="1:19" customHeight="1" ht="14.25">
@@ -9555,7 +9494,7 @@
       <c r="M120" s="113"/>
       <c r="N120" s="113"/>
       <c r="Q120" s="3" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
     </row>
     <row r="121" spans="1:19" customHeight="1" ht="14.25">
@@ -9574,7 +9513,7 @@
       <c r="M121" s="113"/>
       <c r="N121" s="113"/>
       <c r="Q121" s="3" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="122" spans="1:19" customHeight="1" ht="14.25">
@@ -9593,7 +9532,7 @@
       <c r="M122" s="113"/>
       <c r="N122" s="113"/>
       <c r="Q122" s="3" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="123" spans="1:19" customHeight="1" ht="14.25">
@@ -9612,7 +9551,7 @@
       <c r="M123" s="113"/>
       <c r="N123" s="113"/>
       <c r="Q123" s="3" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="124" spans="1:19" customHeight="1" ht="14.25">
@@ -9631,7 +9570,7 @@
       <c r="M124" s="113"/>
       <c r="N124" s="113"/>
       <c r="Q124" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="125" spans="1:19" customHeight="1" ht="14.25">
@@ -9650,7 +9589,7 @@
       <c r="M125" s="113"/>
       <c r="N125" s="113"/>
       <c r="Q125" s="3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="126" spans="1:19" customHeight="1" ht="14.25">
@@ -9669,7 +9608,7 @@
       <c r="M126" s="113"/>
       <c r="N126" s="113"/>
       <c r="Q126" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="127" spans="1:19" customHeight="1" ht="14.25">
@@ -9688,7 +9627,7 @@
       <c r="M127" s="113"/>
       <c r="N127" s="113"/>
       <c r="Q127" s="3" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="128" spans="1:19" customHeight="1" ht="28.5">
@@ -9707,7 +9646,7 @@
       <c r="M128" s="113"/>
       <c r="N128" s="113"/>
       <c r="Q128" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
     <row r="129" spans="1:19" customHeight="1" ht="14.25">
@@ -9726,7 +9665,7 @@
       <c r="M129" s="113"/>
       <c r="N129" s="113"/>
       <c r="Q129" s="3" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="130" spans="1:19" customHeight="1" ht="14.25">
@@ -9745,7 +9684,7 @@
       <c r="M130" s="113"/>
       <c r="N130" s="113"/>
       <c r="Q130" s="3" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="131" spans="1:19" customHeight="1" ht="14.25">
@@ -9764,7 +9703,7 @@
       <c r="M131" s="113"/>
       <c r="N131" s="113"/>
       <c r="Q131" s="3" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="132" spans="1:19" customHeight="1" ht="14.25">
@@ -9783,7 +9722,7 @@
       <c r="M132" s="113"/>
       <c r="N132" s="113"/>
       <c r="Q132" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="133" spans="1:19" customHeight="1" ht="14.25">
@@ -9802,7 +9741,7 @@
       <c r="M133" s="113"/>
       <c r="N133" s="113"/>
       <c r="Q133" s="3" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="134" spans="1:19" customHeight="1" ht="14.25">
@@ -9821,7 +9760,7 @@
       <c r="M134" s="113"/>
       <c r="N134" s="113"/>
       <c r="Q134" s="3" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="135" spans="1:19" customHeight="1" ht="14.25">
@@ -9840,7 +9779,7 @@
       <c r="M135" s="113"/>
       <c r="N135" s="113"/>
       <c r="Q135" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
     </row>
     <row r="136" spans="1:19" customHeight="1" ht="14.25">
@@ -9859,7 +9798,7 @@
       <c r="M136" s="113"/>
       <c r="N136" s="113"/>
       <c r="Q136" s="3" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="137" spans="1:19" customHeight="1" ht="14.25">
@@ -9878,7 +9817,7 @@
       <c r="M137" s="113"/>
       <c r="N137" s="113"/>
       <c r="Q137" s="3" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="138" spans="1:19" customHeight="1" ht="14.25">
@@ -9897,7 +9836,7 @@
       <c r="M138" s="113"/>
       <c r="N138" s="113"/>
       <c r="Q138" s="3" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="139" spans="1:19" customHeight="1" ht="14.25">
@@ -9916,7 +9855,7 @@
       <c r="M139" s="113"/>
       <c r="N139" s="113"/>
       <c r="Q139" s="3" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
     </row>
     <row r="140" spans="1:19" customHeight="1" ht="14.25">
@@ -9935,7 +9874,7 @@
       <c r="M140" s="113"/>
       <c r="N140" s="113"/>
       <c r="Q140" s="3" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="141" spans="1:19" customHeight="1" ht="14.25">
@@ -9954,7 +9893,7 @@
       <c r="M141" s="113"/>
       <c r="N141" s="113"/>
       <c r="Q141" s="3" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
     </row>
     <row r="142" spans="1:19" customHeight="1" ht="14.25">
@@ -9973,7 +9912,7 @@
       <c r="M142" s="113"/>
       <c r="N142" s="113"/>
       <c r="Q142" s="3" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="143" spans="1:19" customHeight="1" ht="28.5">
@@ -9992,7 +9931,7 @@
       <c r="M143" s="113"/>
       <c r="N143" s="113"/>
       <c r="Q143" s="3" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
     </row>
     <row r="144" spans="1:19" customHeight="1" ht="14.25">
@@ -10011,7 +9950,7 @@
       <c r="M144" s="113"/>
       <c r="N144" s="113"/>
       <c r="Q144" s="3" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="145" spans="1:19" customHeight="1" ht="14.25">
@@ -10030,7 +9969,7 @@
       <c r="M145" s="113"/>
       <c r="N145" s="113"/>
       <c r="Q145" s="3" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="146" spans="1:19" customHeight="1" ht="14.25">
@@ -10049,7 +9988,7 @@
       <c r="M146" s="113"/>
       <c r="N146" s="113"/>
       <c r="Q146" s="3" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
     </row>
     <row r="147" spans="1:19" customHeight="1" ht="14.25">
@@ -10068,7 +10007,7 @@
       <c r="M147" s="113"/>
       <c r="N147" s="113"/>
       <c r="Q147" s="3" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="148" spans="1:19" customHeight="1" ht="14.25">
@@ -10087,7 +10026,7 @@
       <c r="M148" s="113"/>
       <c r="N148" s="113"/>
       <c r="Q148" s="3" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="149" spans="1:19" customHeight="1" ht="14.25">
@@ -10106,7 +10045,7 @@
       <c r="M149" s="113"/>
       <c r="N149" s="113"/>
       <c r="Q149" s="3" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="150" spans="1:19" customHeight="1" ht="14.25">
@@ -10125,7 +10064,7 @@
       <c r="M150" s="113"/>
       <c r="N150" s="113"/>
       <c r="Q150" s="3" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
     <row r="151" spans="1:19" customHeight="1" ht="14.25">
@@ -10144,7 +10083,7 @@
       <c r="M151" s="113"/>
       <c r="N151" s="113"/>
       <c r="Q151" s="3" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="152" spans="1:19" customHeight="1" ht="14.25">
@@ -10163,7 +10102,7 @@
       <c r="M152" s="113"/>
       <c r="N152" s="113"/>
       <c r="Q152" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
     <row r="153" spans="1:19" customHeight="1" ht="28.5">
@@ -10182,7 +10121,7 @@
       <c r="M153" s="113"/>
       <c r="N153" s="113"/>
       <c r="Q153" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="154" spans="1:19" customHeight="1" ht="14.25">
@@ -10201,7 +10140,7 @@
       <c r="M154" s="113"/>
       <c r="N154" s="113"/>
       <c r="Q154" s="3" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="155" spans="1:19" customHeight="1" ht="28.5">
@@ -10220,7 +10159,7 @@
       <c r="M155" s="113"/>
       <c r="N155" s="113"/>
       <c r="Q155" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="156" spans="1:19" customHeight="1" ht="14.25">
@@ -10239,7 +10178,7 @@
       <c r="M156" s="113"/>
       <c r="N156" s="113"/>
       <c r="Q156" s="3" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="157" spans="1:19" customHeight="1" ht="14.25">
@@ -10258,7 +10197,7 @@
       <c r="M157" s="113"/>
       <c r="N157" s="113"/>
       <c r="Q157" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="158" spans="1:19" customHeight="1" ht="14.25">
@@ -10277,7 +10216,7 @@
       <c r="M158" s="113"/>
       <c r="N158" s="113"/>
       <c r="Q158" s="3" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="159" spans="1:19" customHeight="1" ht="14.25">
@@ -10296,7 +10235,7 @@
       <c r="M159" s="113"/>
       <c r="N159" s="113"/>
       <c r="Q159" s="3" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="160" spans="1:19" customHeight="1" ht="14.25">
@@ -10315,7 +10254,7 @@
       <c r="M160" s="113"/>
       <c r="N160" s="113"/>
       <c r="Q160" s="3" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="161" spans="1:19" customHeight="1" ht="14.25">
@@ -10334,7 +10273,7 @@
       <c r="M161" s="113"/>
       <c r="N161" s="113"/>
       <c r="Q161" s="3" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="162" spans="1:19" customHeight="1" ht="14.25">
@@ -10353,7 +10292,7 @@
       <c r="M162" s="113"/>
       <c r="N162" s="113"/>
       <c r="Q162" s="3" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
     </row>
     <row r="163" spans="1:19" customHeight="1" ht="14.25">
@@ -10372,7 +10311,7 @@
       <c r="M163" s="113"/>
       <c r="N163" s="113"/>
       <c r="Q163" s="3" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
     </row>
     <row r="164" spans="1:19" customHeight="1" ht="14.25">
@@ -10391,7 +10330,7 @@
       <c r="M164" s="113"/>
       <c r="N164" s="113"/>
       <c r="Q164" s="3" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="165" spans="1:19" customHeight="1" ht="28.5">
@@ -10410,7 +10349,7 @@
       <c r="M165" s="113"/>
       <c r="N165" s="113"/>
       <c r="Q165" s="3" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="166" spans="1:19" customHeight="1" ht="14.25">
@@ -10429,7 +10368,7 @@
       <c r="M166" s="113"/>
       <c r="N166" s="113"/>
       <c r="Q166" s="3" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="167" spans="1:19" customHeight="1" ht="42.75">
@@ -10448,7 +10387,7 @@
       <c r="M167" s="113"/>
       <c r="N167" s="113"/>
       <c r="Q167" s="3" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="168" spans="1:19" customHeight="1" ht="14.25">
@@ -10467,7 +10406,7 @@
       <c r="M168" s="113"/>
       <c r="N168" s="113"/>
       <c r="Q168" s="3" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="169" spans="1:19" customHeight="1" ht="14.25">
@@ -10486,7 +10425,7 @@
       <c r="M169" s="113"/>
       <c r="N169" s="113"/>
       <c r="Q169" s="3" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="170" spans="1:19" customHeight="1" ht="28.5">
@@ -10505,7 +10444,7 @@
       <c r="M170" s="113"/>
       <c r="N170" s="113"/>
       <c r="Q170" s="3" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="171" spans="1:19" customHeight="1" ht="14.25">
@@ -10524,7 +10463,7 @@
       <c r="M171" s="113"/>
       <c r="N171" s="113"/>
       <c r="Q171" s="3" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="172" spans="1:19" customHeight="1" ht="14.25">
@@ -10543,7 +10482,7 @@
       <c r="M172" s="113"/>
       <c r="N172" s="113"/>
       <c r="Q172" s="3" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="173" spans="1:19" customHeight="1" ht="14.25">
@@ -10562,7 +10501,7 @@
       <c r="M173" s="113"/>
       <c r="N173" s="113"/>
       <c r="Q173" s="3" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="174" spans="1:19" customHeight="1" ht="14.25">
@@ -10581,7 +10520,7 @@
       <c r="M174" s="113"/>
       <c r="N174" s="113"/>
       <c r="Q174" s="3" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="175" spans="1:19" customHeight="1" ht="14.25">
@@ -10600,7 +10539,7 @@
       <c r="M175" s="113"/>
       <c r="N175" s="113"/>
       <c r="Q175" s="3" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="176" spans="1:19" customHeight="1" ht="14.25">
@@ -10619,7 +10558,7 @@
       <c r="M176" s="113"/>
       <c r="N176" s="113"/>
       <c r="Q176" s="3" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="177" spans="1:19" customHeight="1" ht="14.25">
@@ -10638,7 +10577,7 @@
       <c r="M177" s="113"/>
       <c r="N177" s="113"/>
       <c r="Q177" s="3" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="178" spans="1:19" customHeight="1" ht="14.25">
@@ -10657,7 +10596,7 @@
       <c r="M178" s="113"/>
       <c r="N178" s="113"/>
       <c r="Q178" s="3" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="179" spans="1:19" customHeight="1" ht="14.25">
@@ -10676,7 +10615,7 @@
       <c r="M179" s="113"/>
       <c r="N179" s="113"/>
       <c r="Q179" s="3" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="180" spans="1:19" customHeight="1" ht="28.5">
@@ -10695,7 +10634,7 @@
       <c r="M180" s="113"/>
       <c r="N180" s="113"/>
       <c r="Q180" s="3" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
     </row>
     <row r="181" spans="1:19" customHeight="1" ht="14.25">
@@ -10714,7 +10653,7 @@
       <c r="M181" s="113"/>
       <c r="N181" s="113"/>
       <c r="Q181" s="3" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
     </row>
     <row r="182" spans="1:19" customHeight="1" ht="14.25">
@@ -10733,7 +10672,7 @@
       <c r="M182" s="113"/>
       <c r="N182" s="113"/>
       <c r="Q182" s="3" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="183" spans="1:19" customHeight="1" ht="14.25">
@@ -10752,7 +10691,7 @@
       <c r="M183" s="113"/>
       <c r="N183" s="113"/>
       <c r="Q183" s="3" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
     </row>
     <row r="184" spans="1:19" customHeight="1" ht="14.25">
@@ -10771,7 +10710,7 @@
       <c r="M184" s="113"/>
       <c r="N184" s="113"/>
       <c r="Q184" s="3" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
     </row>
     <row r="185" spans="1:19" customHeight="1" ht="14.25">
@@ -10790,7 +10729,7 @@
       <c r="M185" s="113"/>
       <c r="N185" s="113"/>
       <c r="Q185" s="3" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="186" spans="1:19" customHeight="1" ht="14.25">
@@ -10809,7 +10748,7 @@
       <c r="M186" s="113"/>
       <c r="N186" s="113"/>
       <c r="Q186" s="3" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
     </row>
     <row r="187" spans="1:19" customHeight="1" ht="14.25">
@@ -10828,7 +10767,7 @@
       <c r="M187" s="113"/>
       <c r="N187" s="113"/>
       <c r="Q187" s="3" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
     </row>
     <row r="188" spans="1:19" customHeight="1" ht="14.25">
@@ -10847,7 +10786,7 @@
       <c r="M188" s="113"/>
       <c r="N188" s="113"/>
       <c r="Q188" s="3" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="189" spans="1:19" customHeight="1" ht="14.25">
@@ -10866,7 +10805,7 @@
       <c r="M189" s="113"/>
       <c r="N189" s="113"/>
       <c r="Q189" s="3" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="190" spans="1:19" customHeight="1" ht="14.25">
@@ -10885,7 +10824,7 @@
       <c r="M190" s="113"/>
       <c r="N190" s="113"/>
       <c r="Q190" s="3" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
     </row>
     <row r="191" spans="1:19" customHeight="1" ht="14.25">
@@ -10904,7 +10843,7 @@
       <c r="M191" s="113"/>
       <c r="N191" s="113"/>
       <c r="Q191" s="3" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
     </row>
     <row r="192" spans="1:19" customHeight="1" ht="14.25">
@@ -10923,7 +10862,7 @@
       <c r="M192" s="113"/>
       <c r="N192" s="113"/>
       <c r="Q192" s="3" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="193" spans="1:19" customHeight="1" ht="14.25">
@@ -10942,7 +10881,7 @@
       <c r="M193" s="113"/>
       <c r="N193" s="113"/>
       <c r="Q193" s="3" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="194" spans="1:19" customHeight="1" ht="14.25">
@@ -10961,7 +10900,7 @@
       <c r="M194" s="113"/>
       <c r="N194" s="113"/>
       <c r="Q194" s="3" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="195" spans="1:19" customHeight="1" ht="14.25">
@@ -10980,7 +10919,7 @@
       <c r="M195" s="113"/>
       <c r="N195" s="113"/>
       <c r="Q195" s="3" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="196" spans="1:19" customHeight="1" ht="14.25">
@@ -10999,7 +10938,7 @@
       <c r="M196" s="113"/>
       <c r="N196" s="113"/>
       <c r="Q196" s="3" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="197" spans="1:19" customHeight="1" ht="14.25">
@@ -11018,7 +10957,7 @@
       <c r="M197" s="113"/>
       <c r="N197" s="113"/>
       <c r="Q197" s="3" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="198" spans="1:19" customHeight="1" ht="14.25">
@@ -11037,7 +10976,7 @@
       <c r="M198" s="113"/>
       <c r="N198" s="113"/>
       <c r="Q198" s="3" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="199" spans="1:19" customHeight="1" ht="14.25">
@@ -11056,7 +10995,7 @@
       <c r="M199" s="113"/>
       <c r="N199" s="113"/>
       <c r="Q199" s="3" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="200" spans="1:19" customHeight="1" ht="28.5">
@@ -11075,7 +11014,7 @@
       <c r="M200" s="113"/>
       <c r="N200" s="113"/>
       <c r="Q200" s="3" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="201" spans="1:19" customHeight="1" ht="14.25">
@@ -11094,7 +11033,7 @@
       <c r="M201" s="113"/>
       <c r="N201" s="113"/>
       <c r="Q201" s="3" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="202" spans="1:19" customHeight="1" ht="14.25">
@@ -11113,7 +11052,7 @@
       <c r="M202" s="113"/>
       <c r="N202" s="113"/>
       <c r="Q202" s="3" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="203" spans="1:19" customHeight="1" ht="14.25">
@@ -11132,7 +11071,7 @@
       <c r="M203" s="113"/>
       <c r="N203" s="113"/>
       <c r="Q203" s="3" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="204" spans="1:19" customHeight="1" ht="14.25">
@@ -11151,7 +11090,7 @@
       <c r="M204" s="113"/>
       <c r="N204" s="113"/>
       <c r="Q204" s="3" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="205" spans="1:19" customHeight="1" ht="14.25">
@@ -11170,7 +11109,7 @@
       <c r="M205" s="113"/>
       <c r="N205" s="113"/>
       <c r="Q205" s="3" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="206" spans="1:19" customHeight="1" ht="14.25">
@@ -11189,7 +11128,7 @@
       <c r="M206" s="113"/>
       <c r="N206" s="113"/>
       <c r="Q206" s="3" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="207" spans="1:19" customHeight="1" ht="28.5">
@@ -11208,7 +11147,7 @@
       <c r="M207" s="113"/>
       <c r="N207" s="113"/>
       <c r="Q207" s="3" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="208" spans="1:19" customHeight="1" ht="28.5">
@@ -11227,7 +11166,7 @@
       <c r="M208" s="113"/>
       <c r="N208" s="113"/>
       <c r="Q208" s="3" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="209" spans="1:19" customHeight="1" ht="14.25">
@@ -11246,7 +11185,7 @@
       <c r="M209" s="113"/>
       <c r="N209" s="113"/>
       <c r="Q209" s="3" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="210" spans="1:19" customHeight="1" ht="14.25">
@@ -11265,7 +11204,7 @@
       <c r="M210" s="113"/>
       <c r="N210" s="113"/>
       <c r="Q210" s="3" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="211" spans="1:19" customHeight="1" ht="14.25">
@@ -11284,7 +11223,7 @@
       <c r="M211" s="113"/>
       <c r="N211" s="113"/>
       <c r="Q211" s="3" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="212" spans="1:19" customHeight="1" ht="14.25">
@@ -11303,7 +11242,7 @@
       <c r="M212" s="113"/>
       <c r="N212" s="113"/>
       <c r="Q212" s="3" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="213" spans="1:19" customHeight="1" ht="14.25">
@@ -11322,7 +11261,7 @@
       <c r="M213" s="113"/>
       <c r="N213" s="113"/>
       <c r="Q213" s="3" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="214" spans="1:19" customHeight="1" ht="14.25">
@@ -11341,7 +11280,7 @@
       <c r="M214" s="113"/>
       <c r="N214" s="113"/>
       <c r="Q214" s="3" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="215" spans="1:19" customHeight="1" ht="14.25">
@@ -11360,7 +11299,7 @@
       <c r="M215" s="113"/>
       <c r="N215" s="113"/>
       <c r="Q215" s="3" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="216" spans="1:19" customHeight="1" ht="14.25">
@@ -11379,7 +11318,7 @@
       <c r="M216" s="113"/>
       <c r="N216" s="113"/>
       <c r="Q216" s="3" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="217" spans="1:19">
@@ -12559,7 +12498,7 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="18">
       <c r="A2" s="490" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="B2" s="491"/>
       <c r="C2" s="491"/>
@@ -12576,28 +12515,28 @@
     </row>
     <row r="3" spans="1:14" customHeight="1" ht="15">
       <c r="A3" s="144" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="B3" s="480" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="C3" s="480"/>
       <c r="D3" s="480"/>
       <c r="E3" s="481"/>
       <c r="F3" s="488" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="G3" s="484" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="H3" s="481"/>
       <c r="I3" s="484" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="J3" s="480"/>
       <c r="K3" s="481"/>
       <c r="L3" s="486" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="M3" s="487"/>
     </row>
@@ -12614,37 +12553,37 @@
       <c r="J4" s="482"/>
       <c r="K4" s="483"/>
       <c r="L4" s="5" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:14" customHeight="1" ht="27">
       <c r="A5" s="497" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" s="498"/>
       <c r="C5" s="498"/>
       <c r="D5" s="498"/>
       <c r="E5" s="498"/>
       <c r="F5" s="16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G5" s="495" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H5" s="495"/>
       <c r="I5" s="496" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J5" s="496"/>
       <c r="K5" s="496"/>
       <c r="L5" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:14" customHeight="1" ht="27">
@@ -12739,7 +12678,7 @@
     </row>
     <row r="12" spans="1:14" customHeight="1" ht="12">
       <c r="A12" s="515" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B12" s="516"/>
       <c r="C12" s="516"/>
@@ -12756,7 +12695,7 @@
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="518" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="B13" s="519"/>
       <c r="C13" s="519"/>
@@ -12773,7 +12712,7 @@
     </row>
     <row r="14" spans="1:14" customHeight="1" ht="12">
       <c r="A14" s="217" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="B14" s="105"/>
       <c r="C14" s="105"/>
@@ -12790,33 +12729,33 @@
     </row>
     <row r="15" spans="1:14" customHeight="1" ht="18">
       <c r="A15" s="4" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="B15" s="504" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="C15" s="505"/>
       <c r="D15" s="503" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="E15" s="504"/>
       <c r="F15" s="505"/>
       <c r="G15" s="503" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="H15" s="504"/>
       <c r="I15" s="505"/>
       <c r="J15" s="509" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="K15" s="499" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="L15" s="524" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="M15" s="493" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="16" spans="1:14" customHeight="1" ht="15">
@@ -12836,11 +12775,11 @@
     </row>
     <row r="17" spans="1:14" customHeight="1" ht="18.75">
       <c r="A17" s="501" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B17" s="502"/>
       <c r="C17" s="8" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D17" s="485"/>
       <c r="E17" s="482"/>
@@ -12855,33 +12794,33 @@
     </row>
     <row r="18" spans="1:14" customHeight="1" ht="24" s="13" customFormat="1">
       <c r="A18" s="511" t="s">
-        <v>348</v>
+        <v>17</v>
       </c>
       <c r="B18" s="512"/>
       <c r="C18" s="24" t="s">
-        <v>349</v>
+        <v>17</v>
       </c>
       <c r="D18" s="498" t="s">
-        <v>350</v>
+        <v>17</v>
       </c>
       <c r="E18" s="498"/>
       <c r="F18" s="498"/>
       <c r="G18" s="498" t="s">
-        <v>351</v>
+        <v>17</v>
       </c>
       <c r="H18" s="498"/>
       <c r="I18" s="498"/>
-      <c r="J18" s="14">
-        <v>25000</v>
-      </c>
-      <c r="K18" s="9">
-        <v>5</v>
+      <c r="J18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="M18" s="10">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:14" customHeight="1" ht="24" s="13" customFormat="1">
@@ -13291,7 +13230,7 @@
     </row>
     <row r="46" spans="1:14" customHeight="1" ht="9.75">
       <c r="A46" s="526" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B46" s="527"/>
       <c r="C46" s="527"/>
@@ -13308,7 +13247,7 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="27.75">
       <c r="A47" s="272" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B47" s="273"/>
       <c r="C47" s="274"/>
@@ -13318,10 +13257,10 @@
       <c r="G47" s="475"/>
       <c r="H47" s="476"/>
       <c r="I47" s="248" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="J47" s="249" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="K47" s="250"/>
       <c r="L47" s="250"/>
@@ -13330,7 +13269,7 @@
     </row>
     <row r="48" spans="1:14" customHeight="1" ht="9">
       <c r="A48" s="473" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="B48" s="473"/>
       <c r="C48" s="473"/>
@@ -13534,7 +13473,7 @@
     </row>
     <row r="2" spans="1:13" customHeight="1" ht="22.5">
       <c r="A2" s="579" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="B2" s="580"/>
       <c r="C2" s="580"/>
@@ -13549,22 +13488,22 @@
     </row>
     <row r="3" spans="1:13" customHeight="1" ht="15">
       <c r="A3" s="565" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="B3" s="567" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="C3" s="567"/>
       <c r="D3" s="568"/>
       <c r="E3" s="480" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="F3" s="481"/>
       <c r="G3" s="543" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="H3" s="484" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="I3" s="574"/>
       <c r="J3" s="574"/>
@@ -13589,10 +13528,10 @@
       <c r="C5" s="582"/>
       <c r="D5" s="583"/>
       <c r="E5" s="29" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="G5" s="500"/>
       <c r="H5" s="578"/>
@@ -13602,22 +13541,22 @@
     </row>
     <row r="6" spans="1:13" customHeight="1" ht="27.75">
       <c r="A6" s="540" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6" s="541"/>
       <c r="C6" s="541"/>
       <c r="D6" s="542"/>
       <c r="E6" s="38" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G6" s="39" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H6" s="544" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I6" s="545"/>
       <c r="J6" s="545"/>
@@ -13703,7 +13642,7 @@
     </row>
     <row r="13" spans="1:13" customHeight="1" ht="11.25">
       <c r="A13" s="515" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B13" s="516"/>
       <c r="C13" s="516"/>
@@ -13718,7 +13657,7 @@
     </row>
     <row r="14" spans="1:13" customHeight="1" ht="18">
       <c r="A14" s="587" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="B14" s="588"/>
       <c r="C14" s="588"/>
@@ -13733,25 +13672,25 @@
     </row>
     <row r="15" spans="1:13" customHeight="1" ht="18">
       <c r="A15" s="566" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="B15" s="504" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="C15" s="562"/>
       <c r="D15" s="563"/>
       <c r="E15" s="504" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="F15" s="505"/>
       <c r="G15" s="499" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="H15" s="509" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="I15" s="503" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="J15" s="562"/>
       <c r="K15" s="577"/>
@@ -13775,10 +13714,10 @@
       <c r="C17" s="329"/>
       <c r="D17" s="564"/>
       <c r="E17" s="29" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="G17" s="500"/>
       <c r="H17" s="510"/>
@@ -13788,25 +13727,25 @@
     </row>
     <row r="18" spans="1:13" customHeight="1" ht="24.75">
       <c r="A18" s="547" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B18" s="548"/>
       <c r="C18" s="548"/>
       <c r="D18" s="549"/>
       <c r="E18" s="30" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I18" s="553" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J18" s="554"/>
       <c r="K18" s="555"/>
@@ -14073,7 +14012,7 @@
     </row>
     <row r="39" spans="1:13" customHeight="1" ht="13.5">
       <c r="A39" s="275" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B39" s="276"/>
       <c r="C39" s="276"/>
@@ -14088,7 +14027,7 @@
     </row>
     <row r="40" spans="1:13" customHeight="1" ht="22.5">
       <c r="A40" s="556" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="B40" s="557"/>
       <c r="C40" s="557"/>
@@ -14103,36 +14042,36 @@
     </row>
     <row r="41" spans="1:13" customHeight="1" ht="33.75">
       <c r="A41" s="145" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="B41" s="150" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="C41" s="146" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="D41" s="537" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="E41" s="537"/>
       <c r="F41" s="537"/>
       <c r="G41" s="537"/>
       <c r="H41" s="538"/>
       <c r="I41" s="146" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="J41" s="537" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="K41" s="539"/>
     </row>
     <row r="42" spans="1:13" customHeight="1" ht="24.75">
       <c r="A42" s="532" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="533"/>
       <c r="C42" s="534" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D42" s="535"/>
       <c r="E42" s="535"/>
@@ -14140,7 +14079,7 @@
       <c r="G42" s="535"/>
       <c r="H42" s="533"/>
       <c r="I42" s="534" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J42" s="535"/>
       <c r="K42" s="536"/>
@@ -14225,7 +14164,7 @@
     </row>
     <row r="49" spans="1:13" customHeight="1" ht="11.25">
       <c r="A49" s="275" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B49" s="276"/>
       <c r="C49" s="276"/>
@@ -14240,7 +14179,7 @@
     </row>
     <row r="50" spans="1:13" customHeight="1" ht="28.5">
       <c r="A50" s="272" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B50" s="274"/>
       <c r="C50" s="474"/>
@@ -14248,11 +14187,11 @@
       <c r="E50" s="475"/>
       <c r="F50" s="476"/>
       <c r="G50" s="530" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="H50" s="531"/>
       <c r="I50" s="474" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="J50" s="475"/>
       <c r="K50" s="476"/>
@@ -14261,7 +14200,7 @@
     </row>
     <row r="51" spans="1:13" customHeight="1" ht="9.75">
       <c r="K51" s="256" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
     </row>
     <row r="52" spans="1:13" customHeight="1" ht="3"/>
@@ -14412,11 +14351,11 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="13.5">
       <c r="A2" s="694" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="B2" s="695"/>
       <c r="C2" s="721" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="D2" s="721"/>
       <c r="E2" s="721"/>
@@ -14433,7 +14372,7 @@
       <c r="A3" s="44"/>
       <c r="B3" s="45"/>
       <c r="C3" s="710" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="D3" s="710"/>
       <c r="E3" s="710"/>
@@ -14450,7 +14389,7 @@
       <c r="A4" s="44"/>
       <c r="B4" s="45"/>
       <c r="C4" s="710" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="D4" s="710"/>
       <c r="E4" s="710"/>
@@ -14476,14 +14415,12 @@
       <c r="A6" s="44"/>
       <c r="B6" s="45"/>
       <c r="C6" s="710" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="D6" s="710"/>
       <c r="E6" s="710"/>
       <c r="F6" s="711"/>
-      <c r="G6" s="618" t="s">
-        <v>379</v>
-      </c>
+      <c r="G6" s="618"/>
       <c r="H6" s="619"/>
       <c r="I6" s="619"/>
       <c r="J6" s="619"/>
@@ -14508,14 +14445,12 @@
       <c r="A8" s="44"/>
       <c r="B8" s="45"/>
       <c r="C8" s="710" t="s">
-        <v>380</v>
+        <v>363</v>
       </c>
       <c r="D8" s="710"/>
       <c r="E8" s="710"/>
       <c r="F8" s="711"/>
-      <c r="G8" s="618" t="s">
-        <v>381</v>
-      </c>
+      <c r="G8" s="618"/>
       <c r="H8" s="619"/>
       <c r="I8" s="619"/>
       <c r="J8" s="619"/>
@@ -14540,7 +14475,7 @@
       <c r="E10" s="710"/>
       <c r="F10" s="711"/>
       <c r="G10" s="601" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="H10" s="601"/>
       <c r="I10" s="601"/>
@@ -14557,9 +14492,7 @@
       <c r="E11" s="710"/>
       <c r="F11" s="711"/>
       <c r="G11" s="151"/>
-      <c r="H11" s="715" t="s">
-        <v>383</v>
-      </c>
+      <c r="H11" s="715"/>
       <c r="I11" s="715"/>
       <c r="J11" s="715"/>
       <c r="K11" s="715"/>
@@ -14583,18 +14516,16 @@
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="733" t="s">
-        <v>384</v>
+        <v>365</v>
       </c>
       <c r="B13" s="734"/>
       <c r="C13" s="729" t="s">
-        <v>385</v>
+        <v>366</v>
       </c>
       <c r="D13" s="729"/>
       <c r="E13" s="562"/>
       <c r="F13" s="563"/>
-      <c r="G13" s="615" t="s">
-        <v>379</v>
-      </c>
+      <c r="G13" s="615"/>
       <c r="H13" s="616"/>
       <c r="I13" s="616"/>
       <c r="J13" s="616"/>
@@ -14610,7 +14541,7 @@
       <c r="E14" s="562"/>
       <c r="F14" s="563"/>
       <c r="G14" s="600" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="H14" s="601"/>
       <c r="I14" s="601"/>
@@ -14627,9 +14558,7 @@
       <c r="E15" s="562"/>
       <c r="F15" s="563"/>
       <c r="G15" s="46"/>
-      <c r="H15" s="735" t="s">
-        <v>386</v>
-      </c>
+      <c r="H15" s="735"/>
       <c r="I15" s="735"/>
       <c r="J15" s="735"/>
       <c r="K15" s="735"/>
@@ -14670,14 +14599,12 @@
       <c r="A18" s="55"/>
       <c r="B18" s="56"/>
       <c r="C18" s="603" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="D18" s="603"/>
       <c r="E18" s="604"/>
       <c r="F18" s="605"/>
-      <c r="G18" s="737" t="s">
-        <v>381</v>
-      </c>
+      <c r="G18" s="737"/>
       <c r="H18" s="738"/>
       <c r="I18" s="738"/>
       <c r="J18" s="738"/>
@@ -14693,7 +14620,7 @@
       <c r="E19" s="604"/>
       <c r="F19" s="605"/>
       <c r="G19" s="600" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="H19" s="601"/>
       <c r="I19" s="601"/>
@@ -14711,13 +14638,11 @@
       <c r="F20" s="605"/>
       <c r="G20" s="60"/>
       <c r="H20" s="742" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="I20" s="742"/>
       <c r="J20" s="266"/>
-      <c r="K20" s="740" t="s">
-        <v>21</v>
-      </c>
+      <c r="K20" s="740"/>
       <c r="L20" s="740"/>
       <c r="M20" s="61"/>
     </row>
@@ -14729,14 +14654,12 @@
       <c r="E21" s="604"/>
       <c r="F21" s="605"/>
       <c r="G21" s="743" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="H21" s="744"/>
       <c r="I21" s="744"/>
       <c r="J21" s="266"/>
-      <c r="K21" s="741" t="s">
-        <v>21</v>
-      </c>
+      <c r="K21" s="741"/>
       <c r="L21" s="741"/>
       <c r="M21" s="61"/>
     </row>
@@ -14748,7 +14671,7 @@
       <c r="E22" s="606"/>
       <c r="F22" s="607"/>
       <c r="G22" s="130" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="H22" s="257"/>
       <c r="I22" s="608"/>
@@ -14759,18 +14682,16 @@
     </row>
     <row r="23" spans="1:14" customHeight="1" ht="18">
       <c r="A23" s="596" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="B23" s="597"/>
       <c r="C23" s="609" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="D23" s="609"/>
       <c r="E23" s="609"/>
       <c r="F23" s="610"/>
-      <c r="G23" s="615" t="s">
-        <v>381</v>
-      </c>
+      <c r="G23" s="615"/>
       <c r="H23" s="616"/>
       <c r="I23" s="616"/>
       <c r="J23" s="616"/>
@@ -14786,7 +14707,7 @@
       <c r="E24" s="611"/>
       <c r="F24" s="612"/>
       <c r="G24" s="600" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="H24" s="601"/>
       <c r="I24" s="601"/>
@@ -14803,9 +14724,7 @@
       <c r="E25" s="611"/>
       <c r="F25" s="612"/>
       <c r="G25" s="128"/>
-      <c r="H25" s="736" t="s">
-        <v>21</v>
-      </c>
+      <c r="H25" s="736"/>
       <c r="I25" s="736"/>
       <c r="J25" s="736"/>
       <c r="K25" s="736"/>
@@ -14829,18 +14748,16 @@
     </row>
     <row r="27" spans="1:14" customHeight="1" ht="14.25">
       <c r="A27" s="596" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="B27" s="597"/>
       <c r="C27" s="609" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="D27" s="609"/>
       <c r="E27" s="609"/>
       <c r="F27" s="610"/>
-      <c r="G27" s="615" t="s">
-        <v>381</v>
-      </c>
+      <c r="G27" s="615"/>
       <c r="H27" s="616"/>
       <c r="I27" s="616"/>
       <c r="J27" s="616"/>
@@ -14856,7 +14773,7 @@
       <c r="E28" s="611"/>
       <c r="F28" s="612"/>
       <c r="G28" s="600" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="H28" s="601"/>
       <c r="I28" s="601"/>
@@ -14872,9 +14789,7 @@
       <c r="D29" s="611"/>
       <c r="E29" s="611"/>
       <c r="F29" s="612"/>
-      <c r="H29" s="668" t="s">
-        <v>21</v>
-      </c>
+      <c r="H29" s="668"/>
       <c r="I29" s="668"/>
       <c r="J29" s="668"/>
       <c r="K29" s="668"/>
@@ -14898,18 +14813,16 @@
     </row>
     <row r="31" spans="1:14" customHeight="1" ht="18">
       <c r="A31" s="596" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="B31" s="597"/>
       <c r="C31" s="609" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="D31" s="609"/>
       <c r="E31" s="609"/>
       <c r="F31" s="610"/>
-      <c r="G31" s="615" t="s">
-        <v>381</v>
-      </c>
+      <c r="G31" s="615"/>
       <c r="H31" s="616"/>
       <c r="I31" s="616"/>
       <c r="J31" s="616"/>
@@ -14925,14 +14838,12 @@
       <c r="E32" s="611"/>
       <c r="F32" s="612"/>
       <c r="G32" s="669" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="H32" s="670"/>
       <c r="I32" s="670"/>
       <c r="J32" s="670"/>
-      <c r="K32" s="668" t="s">
-        <v>21</v>
-      </c>
+      <c r="K32" s="668"/>
       <c r="L32" s="668"/>
       <c r="M32" s="129"/>
     </row>
@@ -14955,14 +14866,12 @@
       <c r="A34" s="53"/>
       <c r="B34" s="54"/>
       <c r="C34" s="611" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="D34" s="611"/>
       <c r="E34" s="611"/>
       <c r="F34" s="612"/>
-      <c r="G34" s="671" t="s">
-        <v>381</v>
-      </c>
+      <c r="G34" s="671"/>
       <c r="H34" s="672"/>
       <c r="I34" s="672"/>
       <c r="J34" s="672"/>
@@ -14978,14 +14887,12 @@
       <c r="E35" s="611"/>
       <c r="F35" s="612"/>
       <c r="G35" s="669" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="H35" s="670"/>
       <c r="I35" s="670"/>
       <c r="J35" s="670"/>
-      <c r="K35" s="668" t="s">
-        <v>21</v>
-      </c>
+      <c r="K35" s="668"/>
       <c r="L35" s="668"/>
       <c r="M35" s="129"/>
     </row>
@@ -15005,18 +14912,16 @@
     </row>
     <row r="37" spans="1:14" customHeight="1" ht="18">
       <c r="A37" s="596" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="B37" s="597"/>
       <c r="C37" s="727" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="D37" s="727"/>
       <c r="E37" s="727"/>
       <c r="F37" s="728"/>
-      <c r="G37" s="615" t="s">
-        <v>381</v>
-      </c>
+      <c r="G37" s="615"/>
       <c r="H37" s="616"/>
       <c r="I37" s="616"/>
       <c r="J37" s="616"/>
@@ -15032,7 +14937,7 @@
       <c r="E38" s="729"/>
       <c r="F38" s="730"/>
       <c r="G38" s="600" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="H38" s="601"/>
       <c r="I38" s="601"/>
@@ -15049,9 +14954,7 @@
       <c r="E39" s="729"/>
       <c r="F39" s="730"/>
       <c r="G39" s="128"/>
-      <c r="H39" s="736" t="s">
-        <v>21</v>
-      </c>
+      <c r="H39" s="736"/>
       <c r="I39" s="736"/>
       <c r="J39" s="736"/>
       <c r="K39" s="736"/>
@@ -15075,11 +14978,11 @@
     </row>
     <row r="41" spans="1:14" customHeight="1" ht="28.5">
       <c r="A41" s="724" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="B41" s="725"/>
       <c r="C41" s="611" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="D41" s="611"/>
       <c r="E41" s="611"/>
@@ -15109,18 +15012,16 @@
     </row>
     <row r="43" spans="1:14" customHeight="1" ht="13.5">
       <c r="A43" s="68" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="B43" s="69"/>
       <c r="C43" s="611" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="D43" s="611"/>
       <c r="E43" s="611"/>
       <c r="F43" s="612"/>
-      <c r="G43" s="618" t="s">
-        <v>381</v>
-      </c>
+      <c r="G43" s="618"/>
       <c r="H43" s="619"/>
       <c r="I43" s="619"/>
       <c r="J43" s="619"/>
@@ -15136,31 +15037,27 @@
       <c r="E44" s="611"/>
       <c r="F44" s="612"/>
       <c r="G44" s="198" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="H44" s="259"/>
       <c r="I44" s="123"/>
       <c r="J44" s="123"/>
-      <c r="L44" s="127" t="s">
-        <v>21</v>
-      </c>
+      <c r="L44" s="127"/>
       <c r="M44" s="124"/>
       <c r="N44" s="75"/>
     </row>
     <row r="45" spans="1:14" customHeight="1" ht="13.5">
       <c r="A45" s="68" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="B45" s="69"/>
       <c r="C45" s="612" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="D45" s="612"/>
       <c r="E45" s="612"/>
       <c r="F45" s="612"/>
-      <c r="G45" s="618" t="s">
-        <v>381</v>
-      </c>
+      <c r="G45" s="618"/>
       <c r="H45" s="619"/>
       <c r="I45" s="619"/>
       <c r="J45" s="619"/>
@@ -15176,32 +15073,28 @@
       <c r="E46" s="612"/>
       <c r="F46" s="612"/>
       <c r="G46" s="199" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="H46" s="260"/>
       <c r="I46" s="123"/>
       <c r="J46" s="123"/>
       <c r="K46" s="123"/>
-      <c r="L46" s="127" t="s">
-        <v>21</v>
-      </c>
+      <c r="L46" s="127"/>
       <c r="M46" s="124"/>
       <c r="N46" s="75"/>
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="13.5">
       <c r="A47" s="68" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="B47" s="69"/>
       <c r="C47" s="611" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="D47" s="611"/>
       <c r="E47" s="120"/>
       <c r="F47" s="121"/>
-      <c r="G47" s="618" t="s">
-        <v>379</v>
-      </c>
+      <c r="G47" s="618"/>
       <c r="H47" s="619"/>
       <c r="I47" s="619"/>
       <c r="J47" s="619"/>
@@ -15217,15 +15110,13 @@
       <c r="E48" s="688"/>
       <c r="F48" s="689"/>
       <c r="G48" s="200" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="H48" s="261"/>
       <c r="I48" s="125"/>
       <c r="J48" s="125"/>
       <c r="K48" s="125"/>
-      <c r="L48" s="127" t="s">
-        <v>412</v>
-      </c>
+      <c r="L48" s="127"/>
       <c r="M48" s="126"/>
       <c r="N48" s="75"/>
     </row>
@@ -15247,11 +15138,11 @@
     </row>
     <row r="50" spans="1:14" customHeight="1" ht="23.25">
       <c r="A50" s="598" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
       <c r="B50" s="599"/>
       <c r="C50" s="196" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="D50" s="196"/>
       <c r="E50" s="196"/>
@@ -15266,17 +15157,17 @@
     </row>
     <row r="51" spans="1:14" customHeight="1" ht="18">
       <c r="A51" s="684" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
       <c r="B51" s="685"/>
       <c r="C51" s="685"/>
       <c r="D51" s="685"/>
       <c r="E51" s="686"/>
       <c r="F51" s="187" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="G51" s="693" t="s">
-        <v>417</v>
+        <v>396</v>
       </c>
       <c r="H51" s="537"/>
       <c r="I51" s="539"/>
@@ -15286,19 +15177,13 @@
       <c r="M51" s="679"/>
     </row>
     <row r="52" spans="1:14" customHeight="1" ht="24">
-      <c r="A52" s="703" t="s">
-        <v>21</v>
-      </c>
+      <c r="A52" s="703"/>
       <c r="B52" s="704"/>
       <c r="C52" s="706"/>
       <c r="D52" s="706"/>
       <c r="E52" s="707"/>
-      <c r="F52" s="76" t="s">
-        <v>21</v>
-      </c>
-      <c r="G52" s="696" t="s">
-        <v>21</v>
-      </c>
+      <c r="F52" s="76"/>
+      <c r="G52" s="696"/>
       <c r="H52" s="697"/>
       <c r="I52" s="698"/>
       <c r="J52" s="677"/>
@@ -15338,11 +15223,11 @@
     </row>
     <row r="55" spans="1:14" customHeight="1" ht="39.75">
       <c r="A55" s="694" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
       <c r="B55" s="695"/>
       <c r="C55" s="708" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
       <c r="D55" s="708"/>
       <c r="E55" s="708"/>
@@ -15367,7 +15252,7 @@
       <c r="I56" s="263"/>
       <c r="J56" s="207"/>
       <c r="K56" s="680" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
       <c r="L56" s="680"/>
       <c r="M56" s="186"/>
@@ -15417,7 +15302,7 @@
     <row r="60" spans="1:14" customHeight="1" ht="25.5">
       <c r="A60" s="79"/>
       <c r="B60" s="661" t="s">
-        <v>421</v>
+        <v>400</v>
       </c>
       <c r="C60" s="662"/>
       <c r="D60" s="663"/>
@@ -15432,7 +15317,7 @@
     <row r="61" spans="1:14" customHeight="1" ht="20.25">
       <c r="A61" s="79"/>
       <c r="B61" s="648" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="C61" s="649"/>
       <c r="D61" s="136"/>
@@ -15447,7 +15332,7 @@
     <row r="62" spans="1:14" customHeight="1" ht="9">
       <c r="A62" s="79"/>
       <c r="B62" s="636" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="C62" s="637"/>
       <c r="D62" s="640"/>
@@ -15465,7 +15350,7 @@
       <c r="C63" s="651"/>
       <c r="D63" s="664"/>
       <c r="F63" s="665" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="G63" s="666"/>
       <c r="H63" s="666"/>
@@ -15477,13 +15362,11 @@
     <row r="64" spans="1:14" customHeight="1" ht="10.5">
       <c r="A64" s="79"/>
       <c r="B64" s="636" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
       <c r="C64" s="637"/>
       <c r="D64" s="640"/>
-      <c r="F64" s="81" t="s">
-        <v>170</v>
-      </c>
+      <c r="F64" s="81"/>
       <c r="G64" s="188"/>
       <c r="H64" s="188"/>
       <c r="I64" s="189"/>
@@ -15498,14 +15381,14 @@
       <c r="C65" s="639"/>
       <c r="D65" s="641"/>
       <c r="F65" s="633" t="s">
-        <v>426</v>
+        <v>405</v>
       </c>
       <c r="G65" s="634"/>
       <c r="H65" s="634"/>
       <c r="I65" s="635"/>
       <c r="J65" s="82"/>
       <c r="K65" s="631" t="s">
-        <v>427</v>
+        <v>406</v>
       </c>
       <c r="L65" s="632"/>
       <c r="M65" s="80"/>
@@ -15527,7 +15410,7 @@
     </row>
     <row r="67" spans="1:14" customHeight="1" ht="28.5">
       <c r="A67" s="628" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="B67" s="629"/>
       <c r="C67" s="629"/>
@@ -15562,7 +15445,7 @@
       <c r="C69" s="247"/>
       <c r="D69" s="247"/>
       <c r="E69" s="622" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
       <c r="F69" s="623"/>
       <c r="G69" s="623"/>
@@ -15590,7 +15473,7 @@
     </row>
     <row r="71" spans="1:14" customHeight="1" ht="10.5">
       <c r="A71" s="621" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
       <c r="B71" s="621"/>
       <c r="C71" s="621"/>
@@ -15769,35 +15652,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>431</v>
+        <v>410</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>433</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
       <c r="B2" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C2" t="s">
-        <v>436</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>437</v>
+        <v>416</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>438</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -15807,7 +15690,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor export, forms, and CTO logic; remove assignment forms
Improved export logic for unique file naming and children/references handling in PersonnelDataExport and related sheets. Enhanced CTORequestController to better populate template fields and robustly calculate hours. Updated validation in EducationForm and ReferencesForm for stricter year and reference count checks. Removed AssignmentDetailsForm and related views/components. Minor UI/UX improvements in education form view.
</commit_message>
<xml_diff>
--- a/public/report/pds_generated.xlsx
+++ b/public/report/pds_generated.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="429">
   <si>
     <t xml:space="preserve">        </t>
   </si>
@@ -103,19 +103,19 @@
     <t>SURNAME</t>
   </si>
   <si>
-    <t>Moen</t>
+    <t>Schulist</t>
   </si>
   <si>
     <t>FIRST NAME</t>
   </si>
   <si>
-    <t>Cristina</t>
+    <t>Landen</t>
   </si>
   <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                           </t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>V</t>
   </si>
   <si>
     <t>Married</t>
@@ -127,7 +127,7 @@
     <t>MIDDLE NAME</t>
   </si>
   <si>
-    <t>Pascale</t>
+    <t>Crawford</t>
   </si>
   <si>
     <t>Widow/er</t>
@@ -143,7 +143,7 @@
 (mm/dd/yyyy)  </t>
   </si>
   <si>
-    <t>1978-01-20</t>
+    <t>2021-04-19</t>
   </si>
   <si>
     <t>16. CITIZENSHIP</t>
@@ -164,7 +164,7 @@
     <t>PLACE OF BIRTH</t>
   </si>
   <si>
-    <t>Port Jessycafort</t>
+    <t>New Waino</t>
   </si>
   <si>
     <t xml:space="preserve">If holder of  dual citizenship, </t>
@@ -182,10 +182,10 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>Male ☑</t>
-  </si>
-  <si>
-    <t>Female ☐</t>
+    <t>Make ☐</t>
+  </si>
+  <si>
+    <t>Female ☑</t>
   </si>
   <si>
     <t>please indicate the details.</t>
@@ -200,12 +200,15 @@
     <t>CIVIL STATUS</t>
   </si>
   <si>
-    <t>☐Single ☑Married ☐Widowed</t>
+    <t>☐Single ☐Married ☑Widowed</t>
   </si>
   <si>
     <t>17. RESIDENTIAL ADDRESS</t>
   </si>
   <si>
+    <t>asdasd</t>
+  </si>
+  <si>
     <t>Angola</t>
   </si>
   <si>
@@ -218,12 +221,12 @@
     <t>Antigua and Barbuda</t>
   </si>
   <si>
+    <t>asdasdasd</t>
+  </si>
+  <si>
     <t>Argentina</t>
   </si>
   <si>
-    <t>☐Separated ☐Others:</t>
-  </si>
-  <si>
     <t>Armenia</t>
   </si>
   <si>
@@ -272,7 +275,7 @@
     <t>BLOOD TYPE</t>
   </si>
   <si>
-    <t>B</t>
+    <t>O</t>
   </si>
   <si>
     <t>18. PERMANENT ADDRESS</t>
@@ -290,6 +293,9 @@
     <t>GSIS ID NO.</t>
   </si>
   <si>
+    <t>dfdsfsadasd</t>
+  </si>
+  <si>
     <t>Bangladesh</t>
   </si>
   <si>
@@ -314,6 +320,9 @@
     <t>PHILHEALTH NO.</t>
   </si>
   <si>
+    <t>02652461016</t>
+  </si>
+  <si>
     <t>Belize</t>
   </si>
   <si>
@@ -326,7 +335,7 @@
     <t>19. TELEPHONE NO.</t>
   </si>
   <si>
-    <t>+1-732-672-7585</t>
+    <t>1-479-946-2555</t>
   </si>
   <si>
     <t>Benin</t>
@@ -338,7 +347,7 @@
     <t>20. MOBILE NO.</t>
   </si>
   <si>
-    <t>(479) 970-1393</t>
+    <t>+1-650-268-0367</t>
   </si>
   <si>
     <t>Bhutan</t>
@@ -350,7 +359,7 @@
     <t>21. E-MAIL ADDRESS (if any)</t>
   </si>
   <si>
-    <t>rutherford.daren@example.com</t>
+    <t>judge45@example.net</t>
   </si>
   <si>
     <t>Bolivia</t>
@@ -368,6 +377,9 @@
     <t>SPOUSE'S SURNAME</t>
   </si>
   <si>
+    <t>dasdasd</t>
+  </si>
+  <si>
     <t>23. NAME of CHILDREN  (Write full name and list all)</t>
   </si>
   <si>
@@ -380,15 +392,24 @@
     <t xml:space="preserve">  FIRST NAME</t>
   </si>
   <si>
+    <t>asdasdas</t>
+  </si>
+  <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                     </t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>Brazil</t>
   </si>
   <si>
     <t xml:space="preserve">  MIDDLE NAME</t>
   </si>
   <si>
+    <t>dasdasdas</t>
+  </si>
+  <si>
     <t>Brunei </t>
   </si>
   <si>
@@ -422,7 +443,13 @@
     <t>FATHER'S SURNAME</t>
   </si>
   <si>
+    <t>Gotardo</t>
+  </si>
+  <si>
     <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Harley</t>
   </si>
   <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                                  </t>
@@ -525,6 +552,9 @@
     <t>COLLEGE</t>
   </si>
   <si>
+    <t>asdasda</t>
+  </si>
+  <si>
     <t>Croatia</t>
   </si>
   <si>
@@ -543,7 +573,7 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>12/16/2025</t>
+    <t>12/20/2025</t>
   </si>
   <si>
     <t>Cyprus</t>
@@ -7213,17 +7243,17 @@
       </c>
       <c r="H17" s="108"/>
       <c r="I17" s="331" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="J17" s="332"/>
       <c r="K17" s="332"/>
       <c r="L17" s="332" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="M17" s="332"/>
       <c r="N17" s="333"/>
       <c r="Q17" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:19" customHeight="1" ht="9">
@@ -7236,17 +7266,17 @@
       <c r="G18" s="156"/>
       <c r="H18" s="109"/>
       <c r="I18" s="454" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J18" s="419"/>
       <c r="K18" s="419"/>
       <c r="L18" s="419" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M18" s="419"/>
       <c r="N18" s="420"/>
       <c r="Q18" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:19" customHeight="1" ht="5.25">
@@ -7259,26 +7289,24 @@
       <c r="G19" s="156"/>
       <c r="H19" s="109"/>
       <c r="I19" s="421" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="J19" s="422"/>
       <c r="K19" s="422"/>
       <c r="L19" s="425" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="M19" s="422"/>
       <c r="N19" s="426"/>
       <c r="Q19" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:19" customHeight="1" ht="9.75">
       <c r="A20" s="431"/>
       <c r="B20" s="228"/>
       <c r="C20" s="143"/>
-      <c r="D20" s="391" t="s">
-        <v>52</v>
-      </c>
+      <c r="D20" s="391"/>
       <c r="E20" s="392"/>
       <c r="F20" s="393"/>
       <c r="G20" s="154"/>
@@ -7290,7 +7318,7 @@
       <c r="M20" s="424"/>
       <c r="N20" s="427"/>
       <c r="Q20" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:19" customHeight="1" ht="9">
@@ -7303,46 +7331,46 @@
       <c r="G21" s="154"/>
       <c r="H21" s="162"/>
       <c r="I21" s="428" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J21" s="429"/>
       <c r="K21" s="429"/>
       <c r="L21" s="328" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M21" s="329"/>
       <c r="N21" s="330"/>
       <c r="Q21" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:19" customHeight="1" ht="15.75">
       <c r="A22" s="433" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B22" s="404" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C22" s="405"/>
       <c r="D22" s="397">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="E22" s="374"/>
       <c r="F22" s="398"/>
       <c r="G22" s="154"/>
       <c r="H22" s="162"/>
       <c r="I22" s="331" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="J22" s="332"/>
       <c r="K22" s="332"/>
       <c r="L22" s="332" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="M22" s="332"/>
       <c r="N22" s="333"/>
       <c r="Q22" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:19" customHeight="1" ht="8.25">
@@ -7355,38 +7383,38 @@
       <c r="G23" s="154"/>
       <c r="H23" s="162"/>
       <c r="I23" s="336" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J23" s="337"/>
       <c r="K23" s="337"/>
       <c r="L23" s="334" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M23" s="334"/>
       <c r="N23" s="335"/>
       <c r="Q23" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:19" customHeight="1" ht="22.5">
       <c r="A24" s="172" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B24" s="408" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C24" s="382"/>
       <c r="D24" s="415">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E24" s="415"/>
       <c r="F24" s="415"/>
       <c r="G24" s="343" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H24" s="321"/>
-      <c r="I24" s="344" t="s">
-        <v>17</v>
+      <c r="I24" s="344">
+        <v>6616</v>
       </c>
       <c r="J24" s="345"/>
       <c r="K24" s="345"/>
@@ -7394,38 +7422,38 @@
       <c r="M24" s="345"/>
       <c r="N24" s="346"/>
       <c r="Q24" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:19" customHeight="1" ht="15.75">
       <c r="A25" s="402" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B25" s="404" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C25" s="405"/>
       <c r="D25" s="374" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E25" s="374"/>
       <c r="F25" s="374"/>
       <c r="G25" s="114" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H25" s="103"/>
       <c r="I25" s="347" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="J25" s="341"/>
       <c r="K25" s="341"/>
       <c r="L25" s="341" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="M25" s="341"/>
       <c r="N25" s="342"/>
       <c r="Q25" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:19" customHeight="1" ht="9">
@@ -7438,46 +7466,46 @@
       <c r="G26" s="154"/>
       <c r="H26" s="162"/>
       <c r="I26" s="454" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J26" s="419"/>
       <c r="K26" s="419"/>
       <c r="L26" s="419" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M26" s="419"/>
       <c r="N26" s="420"/>
       <c r="Q26" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:19" customHeight="1" ht="15.75">
       <c r="A27" s="402" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B27" s="404" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C27" s="405"/>
       <c r="D27" s="374">
-        <v>12338687692</v>
+        <v>94835897231</v>
       </c>
       <c r="E27" s="374"/>
       <c r="F27" s="374"/>
       <c r="G27" s="156"/>
       <c r="H27" s="109"/>
       <c r="I27" s="347" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="J27" s="341"/>
       <c r="K27" s="341"/>
       <c r="L27" s="341" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="M27" s="341"/>
       <c r="N27" s="342"/>
       <c r="Q27" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:19" customHeight="1" ht="9">
@@ -7490,46 +7518,46 @@
       <c r="G28" s="156"/>
       <c r="H28" s="109"/>
       <c r="I28" s="409" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J28" s="410"/>
       <c r="K28" s="410"/>
       <c r="L28" s="411" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M28" s="410"/>
       <c r="N28" s="412"/>
       <c r="Q28" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:19" customHeight="1" ht="15.75">
       <c r="A29" s="402" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B29" s="404" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C29" s="405"/>
       <c r="D29" s="374">
-        <v>50256946020</v>
+        <v>49151569592</v>
       </c>
       <c r="E29" s="374"/>
       <c r="F29" s="374"/>
       <c r="G29" s="156"/>
       <c r="H29" s="165"/>
       <c r="I29" s="158" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="J29" s="159"/>
       <c r="K29" s="159"/>
       <c r="L29" s="159" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="M29" s="159"/>
       <c r="N29" s="177"/>
       <c r="Q29" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:19" customHeight="1" ht="9.75">
@@ -7542,38 +7570,38 @@
       <c r="G30" s="156"/>
       <c r="H30" s="165"/>
       <c r="I30" s="338" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J30" s="338"/>
       <c r="K30" s="338"/>
       <c r="L30" s="338" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M30" s="338"/>
       <c r="N30" s="339"/>
       <c r="Q30" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:19" customHeight="1" ht="24.75">
       <c r="A31" s="174" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B31" s="101" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C31" s="102"/>
-      <c r="D31" s="453">
-        <v>45496335892</v>
+      <c r="D31" s="453" t="s">
+        <v>85</v>
       </c>
       <c r="E31" s="453"/>
       <c r="F31" s="453"/>
       <c r="G31" s="343" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H31" s="321"/>
-      <c r="I31" s="336" t="s">
-        <v>17</v>
+      <c r="I31" s="336">
+        <v>6616</v>
       </c>
       <c r="J31" s="337"/>
       <c r="K31" s="337"/>
@@ -7581,28 +7609,28 @@
       <c r="M31" s="328"/>
       <c r="N31" s="340"/>
       <c r="Q31" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:19" customHeight="1" ht="24.75">
       <c r="A32" s="172" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B32" s="101" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C32" s="102"/>
       <c r="D32" s="415">
-        <v>6262025914</v>
+        <v>4709167259</v>
       </c>
       <c r="E32" s="415"/>
       <c r="F32" s="415"/>
       <c r="G32" s="153" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H32" s="157"/>
       <c r="I32" s="344" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="J32" s="345"/>
       <c r="K32" s="345"/>
@@ -7610,26 +7638,26 @@
       <c r="M32" s="345"/>
       <c r="N32" s="346"/>
       <c r="Q32" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:19" customHeight="1" ht="24.75">
       <c r="A33" s="381" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B33" s="382"/>
       <c r="C33" s="383"/>
       <c r="D33" s="384">
-        <v>69987792505</v>
+        <v>65420348715</v>
       </c>
       <c r="E33" s="384"/>
       <c r="F33" s="384"/>
       <c r="G33" s="211" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H33" s="155"/>
       <c r="I33" s="344" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="J33" s="345"/>
       <c r="K33" s="345"/>
@@ -7637,26 +7665,26 @@
       <c r="M33" s="345"/>
       <c r="N33" s="346"/>
       <c r="Q33" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:19" customHeight="1" ht="24.75">
       <c r="A34" s="178" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B34" s="230"/>
       <c r="C34" s="160"/>
       <c r="D34" s="374">
-        <v>1829661</v>
+        <v>4167226</v>
       </c>
       <c r="E34" s="374"/>
       <c r="F34" s="374"/>
       <c r="G34" s="114" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H34" s="103"/>
       <c r="I34" s="394" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J34" s="395"/>
       <c r="K34" s="395"/>
@@ -7664,12 +7692,12 @@
       <c r="M34" s="395"/>
       <c r="N34" s="396"/>
       <c r="Q34" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:19" customHeight="1" ht="16.5">
       <c r="A35" s="221" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B35" s="222"/>
       <c r="C35" s="222"/>
@@ -7685,77 +7713,77 @@
       <c r="M35" s="222"/>
       <c r="N35" s="223"/>
       <c r="Q35" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:19" customHeight="1" ht="21">
       <c r="A36" s="106" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B36" s="234" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C36" s="235"/>
       <c r="D36" s="463" t="s">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="E36" s="463"/>
       <c r="F36" s="463"/>
       <c r="G36" s="463"/>
       <c r="H36" s="463"/>
       <c r="I36" s="348" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="J36" s="348"/>
       <c r="K36" s="348"/>
       <c r="L36" s="349"/>
       <c r="M36" s="364" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="N36" s="365"/>
       <c r="Q36" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:19" customHeight="1" ht="21">
       <c r="A37" s="154"/>
       <c r="B37" s="109" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C37" s="165"/>
       <c r="D37" s="285" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="E37" s="286"/>
       <c r="F37" s="287"/>
       <c r="G37" s="300" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="H37" s="300" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="I37" s="283" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="J37" s="283"/>
       <c r="K37" s="283"/>
       <c r="L37" s="284"/>
       <c r="M37" s="281" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="N37" s="282"/>
       <c r="Q37" s="3" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:19" customHeight="1" ht="21">
       <c r="A38" s="179"/>
       <c r="B38" s="226" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C38" s="225"/>
       <c r="D38" s="285" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="E38" s="286"/>
       <c r="F38" s="286"/>
@@ -7768,17 +7796,17 @@
       <c r="M38" s="281"/>
       <c r="N38" s="282"/>
       <c r="Q38" s="3" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:19" customHeight="1" ht="21">
       <c r="A39" s="180"/>
       <c r="B39" s="101" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C39" s="102"/>
       <c r="D39" s="298" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E39" s="298"/>
       <c r="F39" s="298"/>
@@ -7791,17 +7819,17 @@
       <c r="M39" s="281"/>
       <c r="N39" s="282"/>
       <c r="Q39" s="3" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:19" customHeight="1" ht="21">
       <c r="A40" s="180"/>
       <c r="B40" s="101" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C40" s="102"/>
       <c r="D40" s="298" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E40" s="298"/>
       <c r="F40" s="298"/>
@@ -7814,17 +7842,17 @@
       <c r="M40" s="281"/>
       <c r="N40" s="282"/>
       <c r="Q40" s="3" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:19" customHeight="1" ht="21">
       <c r="A41" s="180"/>
       <c r="B41" s="101" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C41" s="102"/>
-      <c r="D41" s="298" t="s">
-        <v>17</v>
+      <c r="D41" s="298">
+        <v>123123123123</v>
       </c>
       <c r="E41" s="298"/>
       <c r="F41" s="298"/>
@@ -7837,17 +7865,17 @@
       <c r="M41" s="281"/>
       <c r="N41" s="282"/>
       <c r="Q41" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:19" customHeight="1" ht="21">
       <c r="A42" s="107"/>
       <c r="B42" s="108" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C42" s="142"/>
       <c r="D42" s="298" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="E42" s="298"/>
       <c r="F42" s="298"/>
@@ -7860,19 +7888,19 @@
       <c r="M42" s="281"/>
       <c r="N42" s="282"/>
       <c r="Q42" s="3" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:19" customHeight="1" ht="21">
       <c r="A43" s="224" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B43" s="231" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C43" s="108"/>
       <c r="D43" s="298" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="E43" s="298"/>
       <c r="F43" s="298"/>
@@ -7885,7 +7913,7 @@
       <c r="M43" s="281"/>
       <c r="N43" s="282"/>
       <c r="Q43" s="3" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:19" customHeight="1" ht="21">
@@ -7895,15 +7923,15 @@
       </c>
       <c r="C44" s="162"/>
       <c r="D44" s="285" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="E44" s="286"/>
       <c r="F44" s="287"/>
       <c r="G44" s="300" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="H44" s="300" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="I44" s="283"/>
       <c r="J44" s="283"/>
@@ -7912,7 +7940,7 @@
       <c r="M44" s="281"/>
       <c r="N44" s="282"/>
       <c r="Q44" s="3" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:19" customHeight="1" ht="21">
@@ -7922,7 +7950,7 @@
       </c>
       <c r="C45" s="218"/>
       <c r="D45" s="285" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E45" s="286"/>
       <c r="F45" s="286"/>
@@ -7935,15 +7963,15 @@
       <c r="M45" s="281"/>
       <c r="N45" s="282"/>
       <c r="Q45" s="3" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:19" customHeight="1" ht="21">
       <c r="A46" s="154" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B46" s="404" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C46" s="404"/>
       <c r="D46" s="404"/>
@@ -7958,7 +7986,7 @@
       <c r="M46" s="281"/>
       <c r="N46" s="282"/>
       <c r="Q46" s="3" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:19" customHeight="1" ht="21">
@@ -7968,7 +7996,7 @@
       </c>
       <c r="C47" s="162"/>
       <c r="D47" s="299" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="E47" s="299"/>
       <c r="F47" s="299"/>
@@ -7981,7 +8009,7 @@
       <c r="M47" s="281"/>
       <c r="N47" s="282"/>
       <c r="Q47" s="3" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:19" customHeight="1" ht="21">
@@ -7991,7 +8019,7 @@
       </c>
       <c r="C48" s="162"/>
       <c r="D48" s="299" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="E48" s="299"/>
       <c r="F48" s="299"/>
@@ -8004,7 +8032,7 @@
       <c r="M48" s="281"/>
       <c r="N48" s="282"/>
       <c r="Q48" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:19" customHeight="1" ht="21">
@@ -8014,14 +8042,14 @@
       </c>
       <c r="C49" s="220"/>
       <c r="D49" s="448" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="E49" s="448"/>
       <c r="F49" s="448"/>
       <c r="G49" s="448"/>
       <c r="H49" s="448"/>
       <c r="I49" s="446" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="J49" s="446"/>
       <c r="K49" s="446"/>
@@ -8029,12 +8057,12 @@
       <c r="M49" s="446"/>
       <c r="N49" s="447"/>
       <c r="Q49" s="3" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:19" customHeight="1" ht="15.75">
       <c r="A50" s="182" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="B50" s="182"/>
       <c r="C50" s="104"/>
@@ -8044,7 +8072,7 @@
       <c r="G50" s="105"/>
       <c r="H50" s="105"/>
       <c r="I50" s="372" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="J50" s="372"/>
       <c r="K50" s="372"/>
@@ -8052,42 +8080,42 @@
       <c r="M50" s="372"/>
       <c r="N50" s="373"/>
       <c r="Q50" s="3" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:19" customHeight="1" ht="14.25">
       <c r="A51" s="366" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B51" s="316" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C51" s="316"/>
       <c r="D51" s="301" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="E51" s="302"/>
       <c r="F51" s="319"/>
       <c r="G51" s="301" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="H51" s="302"/>
       <c r="I51" s="303"/>
       <c r="J51" s="449" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="K51" s="450"/>
       <c r="L51" s="293" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="M51" s="368" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="N51" s="362" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:19" customHeight="1" ht="19.5">
@@ -8106,7 +8134,7 @@
       <c r="M52" s="368"/>
       <c r="N52" s="362"/>
       <c r="Q52" s="3" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:19" customHeight="1" ht="14.25">
@@ -8120,10 +8148,10 @@
       <c r="H53" s="308"/>
       <c r="I53" s="309"/>
       <c r="J53" s="110" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="K53" s="111" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="L53" s="294"/>
       <c r="M53" s="369"/>
@@ -8131,187 +8159,187 @@
       <c r="O53" s="112"/>
       <c r="P53" s="112"/>
       <c r="Q53" s="3" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:19" customHeight="1" ht="28.5">
       <c r="A54" s="238"/>
       <c r="B54" s="239" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="C54" s="239"/>
       <c r="D54" s="322" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="E54" s="323"/>
       <c r="F54" s="324"/>
       <c r="G54" s="295" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="H54" s="296"/>
       <c r="I54" s="297"/>
-      <c r="J54" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="K54" s="232" t="s">
-        <v>17</v>
-      </c>
-      <c r="L54" s="166" t="s">
-        <v>17</v>
-      </c>
-      <c r="M54" s="18" t="s">
-        <v>17</v>
+      <c r="J54" s="26">
+        <v>2002</v>
+      </c>
+      <c r="K54" s="232">
+        <v>2005</v>
+      </c>
+      <c r="L54" s="166">
+        <v>23</v>
+      </c>
+      <c r="M54" s="18">
+        <v>2005</v>
       </c>
       <c r="N54" s="161" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:19" customHeight="1" ht="28.5">
       <c r="A55" s="238"/>
       <c r="B55" s="239" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C55" s="239"/>
       <c r="D55" s="322" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="E55" s="323"/>
       <c r="F55" s="324"/>
       <c r="G55" s="295" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="H55" s="296"/>
       <c r="I55" s="297"/>
-      <c r="J55" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="K55" s="27" t="s">
-        <v>17</v>
+      <c r="J55" s="26">
+        <v>2002</v>
+      </c>
+      <c r="K55" s="27">
+        <v>2005</v>
       </c>
       <c r="L55" s="242" t="s">
-        <v>17</v>
-      </c>
-      <c r="M55" s="19" t="s">
-        <v>17</v>
+        <v>47</v>
+      </c>
+      <c r="M55" s="19">
+        <v>2005</v>
       </c>
       <c r="N55" s="161" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:19" customHeight="1" ht="28.5">
       <c r="A56" s="238"/>
       <c r="B56" s="239" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C56" s="239"/>
       <c r="D56" s="322" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="E56" s="323"/>
       <c r="F56" s="324"/>
       <c r="G56" s="310" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="H56" s="311"/>
       <c r="I56" s="312"/>
       <c r="J56" s="26" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="K56" s="27" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="L56" s="166" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="M56" s="18" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="N56" s="161" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:19" customHeight="1" ht="28.5">
       <c r="A57" s="238"/>
       <c r="B57" s="239" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C57" s="239"/>
       <c r="D57" s="322" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="E57" s="323"/>
       <c r="F57" s="324"/>
       <c r="G57" s="310" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H57" s="311"/>
       <c r="I57" s="312"/>
-      <c r="J57" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="K57" s="27" t="s">
-        <v>17</v>
+      <c r="J57" s="26">
+        <v>2006</v>
+      </c>
+      <c r="K57" s="27">
+        <v>2009</v>
       </c>
       <c r="L57" s="166" t="s">
-        <v>17</v>
-      </c>
-      <c r="M57" s="19" t="s">
-        <v>17</v>
+        <v>162</v>
+      </c>
+      <c r="M57" s="19">
+        <v>2009</v>
       </c>
       <c r="N57" s="161" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="Q57" s="3" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:19" customHeight="1" ht="28.5">
       <c r="A58" s="240"/>
       <c r="B58" s="241" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C58" s="241"/>
       <c r="D58" s="325" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="E58" s="326"/>
       <c r="F58" s="327"/>
       <c r="G58" s="313" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="H58" s="314"/>
       <c r="I58" s="315"/>
       <c r="J58" s="236" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="K58" s="237" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="L58" s="20" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="M58" s="21" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="N58" s="161" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="Q58" s="3" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:19" customHeight="1" ht="12">
       <c r="A59" s="275" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B59" s="276"/>
       <c r="C59" s="276"/>
@@ -8327,12 +8355,12 @@
       <c r="M59" s="276"/>
       <c r="N59" s="277"/>
       <c r="Q59" s="3" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:19" customHeight="1" ht="27.75">
       <c r="A60" s="272" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B60" s="273"/>
       <c r="C60" s="274"/>
@@ -8343,21 +8371,21 @@
       <c r="H60" s="289"/>
       <c r="I60" s="290"/>
       <c r="J60" s="291" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="K60" s="292"/>
       <c r="L60" s="278" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="M60" s="279"/>
       <c r="N60" s="280"/>
       <c r="Q60" s="3" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:19" customHeight="1" ht="12" s="147" customFormat="1">
       <c r="A61" s="271" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B61" s="271"/>
       <c r="C61" s="271"/>
@@ -8373,7 +8401,7 @@
       <c r="M61" s="271"/>
       <c r="N61" s="271"/>
       <c r="Q61" s="253" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="1:19" customHeight="1" ht="14.25">
@@ -8392,7 +8420,7 @@
       <c r="M62" s="113"/>
       <c r="N62" s="113"/>
       <c r="Q62" s="3" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:19" customHeight="1" ht="14.25">
@@ -8411,7 +8439,7 @@
       <c r="M63" s="113"/>
       <c r="N63" s="113"/>
       <c r="Q63" s="3" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:19" customHeight="1" ht="28.5">
@@ -8430,7 +8458,7 @@
       <c r="M64" s="113"/>
       <c r="N64" s="113"/>
       <c r="Q64" s="3" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:19" customHeight="1" ht="14.25">
@@ -8449,7 +8477,7 @@
       <c r="M65" s="113"/>
       <c r="N65" s="113"/>
       <c r="Q65" s="3" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="66" spans="1:19" customHeight="1" ht="14.25">
@@ -8468,7 +8496,7 @@
       <c r="M66" s="113"/>
       <c r="N66" s="113"/>
       <c r="Q66" s="3" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:19" customHeight="1" ht="14.25">
@@ -8487,7 +8515,7 @@
       <c r="M67" s="113"/>
       <c r="N67" s="113"/>
       <c r="Q67" s="3" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:19" customHeight="1" ht="14.25">
@@ -8506,7 +8534,7 @@
       <c r="M68" s="113"/>
       <c r="N68" s="113"/>
       <c r="Q68" s="3" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:19" customHeight="1" ht="28.5">
@@ -8525,7 +8553,7 @@
       <c r="M69" s="113"/>
       <c r="N69" s="113"/>
       <c r="Q69" s="3" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="70" spans="1:19" customHeight="1" ht="14.25">
@@ -8544,7 +8572,7 @@
       <c r="M70" s="113"/>
       <c r="N70" s="113"/>
       <c r="Q70" s="3" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:19" customHeight="1" ht="14.25">
@@ -8563,7 +8591,7 @@
       <c r="M71" s="113"/>
       <c r="N71" s="113"/>
       <c r="Q71" s="3" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="72" spans="1:19" customHeight="1" ht="14.25">
@@ -8582,7 +8610,7 @@
       <c r="M72" s="113"/>
       <c r="N72" s="113"/>
       <c r="Q72" s="3" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:19" customHeight="1" ht="14.25">
@@ -8601,7 +8629,7 @@
       <c r="M73" s="113"/>
       <c r="N73" s="113"/>
       <c r="Q73" s="3" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="74" spans="1:19" customHeight="1" ht="14.25">
@@ -8620,7 +8648,7 @@
       <c r="M74" s="113"/>
       <c r="N74" s="113"/>
       <c r="Q74" s="3" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="75" spans="1:19" customHeight="1" ht="14.25">
@@ -8639,7 +8667,7 @@
       <c r="M75" s="113"/>
       <c r="N75" s="113"/>
       <c r="Q75" s="3" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:19" customHeight="1" ht="14.25">
@@ -8658,7 +8686,7 @@
       <c r="M76" s="113"/>
       <c r="N76" s="113"/>
       <c r="Q76" s="3" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="77" spans="1:19" customHeight="1" ht="14.25">
@@ -8677,7 +8705,7 @@
       <c r="M77" s="113"/>
       <c r="N77" s="113"/>
       <c r="Q77" s="3" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="78" spans="1:19" customHeight="1" ht="14.25">
@@ -8696,7 +8724,7 @@
       <c r="M78" s="113"/>
       <c r="N78" s="113"/>
       <c r="Q78" s="3" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="79" spans="1:19" customHeight="1" ht="14.25">
@@ -8715,7 +8743,7 @@
       <c r="M79" s="113"/>
       <c r="N79" s="113"/>
       <c r="Q79" s="3" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:19" customHeight="1" ht="14.25">
@@ -8734,7 +8762,7 @@
       <c r="M80" s="113"/>
       <c r="N80" s="113"/>
       <c r="Q80" s="3" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:19" customHeight="1" ht="14.25">
@@ -8753,7 +8781,7 @@
       <c r="M81" s="113"/>
       <c r="N81" s="113"/>
       <c r="Q81" s="3" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" spans="1:19" customHeight="1" ht="14.25">
@@ -8772,7 +8800,7 @@
       <c r="M82" s="113"/>
       <c r="N82" s="113"/>
       <c r="Q82" s="3" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="83" spans="1:19" customHeight="1" ht="14.25">
@@ -8791,7 +8819,7 @@
       <c r="M83" s="113"/>
       <c r="N83" s="113"/>
       <c r="Q83" s="3" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="84" spans="1:19" customHeight="1" ht="14.25">
@@ -8810,7 +8838,7 @@
       <c r="M84" s="113"/>
       <c r="N84" s="113"/>
       <c r="Q84" s="3" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="85" spans="1:19" customHeight="1" ht="28.5">
@@ -8829,7 +8857,7 @@
       <c r="M85" s="113"/>
       <c r="N85" s="113"/>
       <c r="Q85" s="3" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86" spans="1:19" customHeight="1" ht="14.25">
@@ -8848,7 +8876,7 @@
       <c r="M86" s="113"/>
       <c r="N86" s="113"/>
       <c r="Q86" s="3" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="87" spans="1:19" customHeight="1" ht="14.25">
@@ -8867,7 +8895,7 @@
       <c r="M87" s="113"/>
       <c r="N87" s="113"/>
       <c r="Q87" s="3" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
     </row>
     <row r="88" spans="1:19" customHeight="1" ht="14.25">
@@ -8886,7 +8914,7 @@
       <c r="M88" s="113"/>
       <c r="N88" s="113"/>
       <c r="Q88" s="3" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="89" spans="1:19" customHeight="1" ht="14.25">
@@ -8905,7 +8933,7 @@
       <c r="M89" s="113"/>
       <c r="N89" s="113"/>
       <c r="Q89" s="3" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90" spans="1:19" customHeight="1" ht="14.25">
@@ -8924,7 +8952,7 @@
       <c r="M90" s="113"/>
       <c r="N90" s="113"/>
       <c r="Q90" s="3" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="91" spans="1:19" customHeight="1" ht="14.25">
@@ -8943,7 +8971,7 @@
       <c r="M91" s="113"/>
       <c r="N91" s="113"/>
       <c r="Q91" s="3" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:19" customHeight="1" ht="14.25">
@@ -8962,7 +8990,7 @@
       <c r="M92" s="113"/>
       <c r="N92" s="113"/>
       <c r="Q92" s="3" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="93" spans="1:19" customHeight="1" ht="14.25">
@@ -8981,7 +9009,7 @@
       <c r="M93" s="113"/>
       <c r="N93" s="113"/>
       <c r="Q93" s="3" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
     </row>
     <row r="94" spans="1:19" customHeight="1" ht="14.25">
@@ -9000,7 +9028,7 @@
       <c r="M94" s="113"/>
       <c r="N94" s="113"/>
       <c r="Q94" s="3" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="95" spans="1:19" customHeight="1" ht="14.25">
@@ -9019,7 +9047,7 @@
       <c r="M95" s="113"/>
       <c r="N95" s="113"/>
       <c r="Q95" s="3" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
     </row>
     <row r="96" spans="1:19" customHeight="1" ht="14.25">
@@ -9038,7 +9066,7 @@
       <c r="M96" s="113"/>
       <c r="N96" s="113"/>
       <c r="Q96" s="3" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="97" spans="1:19" customHeight="1" ht="14.25">
@@ -9057,7 +9085,7 @@
       <c r="M97" s="113"/>
       <c r="N97" s="113"/>
       <c r="Q97" s="3" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
     </row>
     <row r="98" spans="1:19" customHeight="1" ht="14.25">
@@ -9076,7 +9104,7 @@
       <c r="M98" s="113"/>
       <c r="N98" s="113"/>
       <c r="Q98" s="3" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="99" spans="1:19" customHeight="1" ht="14.25">
@@ -9095,7 +9123,7 @@
       <c r="M99" s="113"/>
       <c r="N99" s="113"/>
       <c r="Q99" s="3" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="100" spans="1:19" customHeight="1" ht="14.25">
@@ -9114,7 +9142,7 @@
       <c r="M100" s="113"/>
       <c r="N100" s="113"/>
       <c r="Q100" s="3" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="101" spans="1:19" customHeight="1" ht="14.25">
@@ -9133,7 +9161,7 @@
       <c r="M101" s="113"/>
       <c r="N101" s="113"/>
       <c r="Q101" s="3" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
     </row>
     <row r="102" spans="1:19" customHeight="1" ht="14.25">
@@ -9152,7 +9180,7 @@
       <c r="M102" s="113"/>
       <c r="N102" s="113"/>
       <c r="Q102" s="3" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="103" spans="1:19" customHeight="1" ht="14.25">
@@ -9171,7 +9199,7 @@
       <c r="M103" s="113"/>
       <c r="N103" s="113"/>
       <c r="Q103" s="3" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="104" spans="1:19" customHeight="1" ht="14.25">
@@ -9190,7 +9218,7 @@
       <c r="M104" s="113"/>
       <c r="N104" s="113"/>
       <c r="Q104" s="3" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="105" spans="1:19" customHeight="1" ht="14.25">
@@ -9209,7 +9237,7 @@
       <c r="M105" s="113"/>
       <c r="N105" s="113"/>
       <c r="Q105" s="3" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
     </row>
     <row r="106" spans="1:19" customHeight="1" ht="14.25">
@@ -9228,7 +9256,7 @@
       <c r="M106" s="113"/>
       <c r="N106" s="113"/>
       <c r="Q106" s="3" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="107" spans="1:19" customHeight="1" ht="14.25">
@@ -9247,7 +9275,7 @@
       <c r="M107" s="113"/>
       <c r="N107" s="113"/>
       <c r="Q107" s="3" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="108" spans="1:19" customHeight="1" ht="14.25">
@@ -9266,7 +9294,7 @@
       <c r="M108" s="113"/>
       <c r="N108" s="113"/>
       <c r="Q108" s="3" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="109" spans="1:19" customHeight="1" ht="14.25">
@@ -9285,7 +9313,7 @@
       <c r="M109" s="113"/>
       <c r="N109" s="113"/>
       <c r="Q109" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
     </row>
     <row r="110" spans="1:19" customHeight="1" ht="14.25">
@@ -9304,7 +9332,7 @@
       <c r="M110" s="113"/>
       <c r="N110" s="113"/>
       <c r="Q110" s="3" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="111" spans="1:19" customHeight="1" ht="14.25">
@@ -9323,7 +9351,7 @@
       <c r="M111" s="113"/>
       <c r="N111" s="113"/>
       <c r="Q111" s="3" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="112" spans="1:19" customHeight="1" ht="14.25">
@@ -9342,7 +9370,7 @@
       <c r="M112" s="113"/>
       <c r="N112" s="113"/>
       <c r="Q112" s="3" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="113" spans="1:19" customHeight="1" ht="14.25">
@@ -9361,7 +9389,7 @@
       <c r="M113" s="113"/>
       <c r="N113" s="113"/>
       <c r="Q113" s="3" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
     <row r="114" spans="1:19" customHeight="1" ht="14.25">
@@ -9380,7 +9408,7 @@
       <c r="M114" s="113"/>
       <c r="N114" s="113"/>
       <c r="Q114" s="3" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="115" spans="1:19" customHeight="1" ht="14.25">
@@ -9399,7 +9427,7 @@
       <c r="M115" s="113"/>
       <c r="N115" s="113"/>
       <c r="Q115" s="3" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
     <row r="116" spans="1:19" customHeight="1" ht="14.25">
@@ -9418,7 +9446,7 @@
       <c r="M116" s="113"/>
       <c r="N116" s="113"/>
       <c r="Q116" s="3" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="117" spans="1:19" customHeight="1" ht="14.25">
@@ -9437,7 +9465,7 @@
       <c r="M117" s="113"/>
       <c r="N117" s="113"/>
       <c r="Q117" s="3" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="118" spans="1:19" customHeight="1" ht="14.25">
@@ -9456,7 +9484,7 @@
       <c r="M118" s="113"/>
       <c r="N118" s="113"/>
       <c r="Q118" s="3" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
     </row>
     <row r="119" spans="1:19" customHeight="1" ht="14.25">
@@ -9475,7 +9503,7 @@
       <c r="M119" s="113"/>
       <c r="N119" s="113"/>
       <c r="Q119" s="3" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:19" customHeight="1" ht="14.25">
@@ -9494,7 +9522,7 @@
       <c r="M120" s="113"/>
       <c r="N120" s="113"/>
       <c r="Q120" s="3" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="121" spans="1:19" customHeight="1" ht="14.25">
@@ -9513,7 +9541,7 @@
       <c r="M121" s="113"/>
       <c r="N121" s="113"/>
       <c r="Q121" s="3" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
     </row>
     <row r="122" spans="1:19" customHeight="1" ht="14.25">
@@ -9532,7 +9560,7 @@
       <c r="M122" s="113"/>
       <c r="N122" s="113"/>
       <c r="Q122" s="3" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="123" spans="1:19" customHeight="1" ht="14.25">
@@ -9551,7 +9579,7 @@
       <c r="M123" s="113"/>
       <c r="N123" s="113"/>
       <c r="Q123" s="3" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="124" spans="1:19" customHeight="1" ht="14.25">
@@ -9570,7 +9598,7 @@
       <c r="M124" s="113"/>
       <c r="N124" s="113"/>
       <c r="Q124" s="3" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="125" spans="1:19" customHeight="1" ht="14.25">
@@ -9589,7 +9617,7 @@
       <c r="M125" s="113"/>
       <c r="N125" s="113"/>
       <c r="Q125" s="3" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
     </row>
     <row r="126" spans="1:19" customHeight="1" ht="14.25">
@@ -9608,7 +9636,7 @@
       <c r="M126" s="113"/>
       <c r="N126" s="113"/>
       <c r="Q126" s="3" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" spans="1:19" customHeight="1" ht="14.25">
@@ -9627,7 +9655,7 @@
       <c r="M127" s="113"/>
       <c r="N127" s="113"/>
       <c r="Q127" s="3" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="128" spans="1:19" customHeight="1" ht="28.5">
@@ -9646,7 +9674,7 @@
       <c r="M128" s="113"/>
       <c r="N128" s="113"/>
       <c r="Q128" s="3" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="129" spans="1:19" customHeight="1" ht="14.25">
@@ -9665,7 +9693,7 @@
       <c r="M129" s="113"/>
       <c r="N129" s="113"/>
       <c r="Q129" s="3" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="130" spans="1:19" customHeight="1" ht="14.25">
@@ -9684,7 +9712,7 @@
       <c r="M130" s="113"/>
       <c r="N130" s="113"/>
       <c r="Q130" s="3" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="131" spans="1:19" customHeight="1" ht="14.25">
@@ -9703,7 +9731,7 @@
       <c r="M131" s="113"/>
       <c r="N131" s="113"/>
       <c r="Q131" s="3" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
     </row>
     <row r="132" spans="1:19" customHeight="1" ht="14.25">
@@ -9722,7 +9750,7 @@
       <c r="M132" s="113"/>
       <c r="N132" s="113"/>
       <c r="Q132" s="3" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="133" spans="1:19" customHeight="1" ht="14.25">
@@ -9741,7 +9769,7 @@
       <c r="M133" s="113"/>
       <c r="N133" s="113"/>
       <c r="Q133" s="3" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
     </row>
     <row r="134" spans="1:19" customHeight="1" ht="14.25">
@@ -9760,7 +9788,7 @@
       <c r="M134" s="113"/>
       <c r="N134" s="113"/>
       <c r="Q134" s="3" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
     </row>
     <row r="135" spans="1:19" customHeight="1" ht="14.25">
@@ -9779,7 +9807,7 @@
       <c r="M135" s="113"/>
       <c r="N135" s="113"/>
       <c r="Q135" s="3" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" spans="1:19" customHeight="1" ht="14.25">
@@ -9798,7 +9826,7 @@
       <c r="M136" s="113"/>
       <c r="N136" s="113"/>
       <c r="Q136" s="3" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="137" spans="1:19" customHeight="1" ht="14.25">
@@ -9817,7 +9845,7 @@
       <c r="M137" s="113"/>
       <c r="N137" s="113"/>
       <c r="Q137" s="3" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
     </row>
     <row r="138" spans="1:19" customHeight="1" ht="14.25">
@@ -9836,7 +9864,7 @@
       <c r="M138" s="113"/>
       <c r="N138" s="113"/>
       <c r="Q138" s="3" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="139" spans="1:19" customHeight="1" ht="14.25">
@@ -9855,7 +9883,7 @@
       <c r="M139" s="113"/>
       <c r="N139" s="113"/>
       <c r="Q139" s="3" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
     </row>
     <row r="140" spans="1:19" customHeight="1" ht="14.25">
@@ -9874,7 +9902,7 @@
       <c r="M140" s="113"/>
       <c r="N140" s="113"/>
       <c r="Q140" s="3" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
     </row>
     <row r="141" spans="1:19" customHeight="1" ht="14.25">
@@ -9893,7 +9921,7 @@
       <c r="M141" s="113"/>
       <c r="N141" s="113"/>
       <c r="Q141" s="3" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
     </row>
     <row r="142" spans="1:19" customHeight="1" ht="14.25">
@@ -9912,7 +9940,7 @@
       <c r="M142" s="113"/>
       <c r="N142" s="113"/>
       <c r="Q142" s="3" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
     </row>
     <row r="143" spans="1:19" customHeight="1" ht="28.5">
@@ -9931,7 +9959,7 @@
       <c r="M143" s="113"/>
       <c r="N143" s="113"/>
       <c r="Q143" s="3" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
     </row>
     <row r="144" spans="1:19" customHeight="1" ht="14.25">
@@ -9950,7 +9978,7 @@
       <c r="M144" s="113"/>
       <c r="N144" s="113"/>
       <c r="Q144" s="3" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
     </row>
     <row r="145" spans="1:19" customHeight="1" ht="14.25">
@@ -9969,7 +9997,7 @@
       <c r="M145" s="113"/>
       <c r="N145" s="113"/>
       <c r="Q145" s="3" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
     </row>
     <row r="146" spans="1:19" customHeight="1" ht="14.25">
@@ -9988,7 +10016,7 @@
       <c r="M146" s="113"/>
       <c r="N146" s="113"/>
       <c r="Q146" s="3" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
     </row>
     <row r="147" spans="1:19" customHeight="1" ht="14.25">
@@ -10007,7 +10035,7 @@
       <c r="M147" s="113"/>
       <c r="N147" s="113"/>
       <c r="Q147" s="3" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
     </row>
     <row r="148" spans="1:19" customHeight="1" ht="14.25">
@@ -10026,7 +10054,7 @@
       <c r="M148" s="113"/>
       <c r="N148" s="113"/>
       <c r="Q148" s="3" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
     <row r="149" spans="1:19" customHeight="1" ht="14.25">
@@ -10045,7 +10073,7 @@
       <c r="M149" s="113"/>
       <c r="N149" s="113"/>
       <c r="Q149" s="3" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
     </row>
     <row r="150" spans="1:19" customHeight="1" ht="14.25">
@@ -10064,7 +10092,7 @@
       <c r="M150" s="113"/>
       <c r="N150" s="113"/>
       <c r="Q150" s="3" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
     </row>
     <row r="151" spans="1:19" customHeight="1" ht="14.25">
@@ -10083,7 +10111,7 @@
       <c r="M151" s="113"/>
       <c r="N151" s="113"/>
       <c r="Q151" s="3" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
     </row>
     <row r="152" spans="1:19" customHeight="1" ht="14.25">
@@ -10102,7 +10130,7 @@
       <c r="M152" s="113"/>
       <c r="N152" s="113"/>
       <c r="Q152" s="3" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="153" spans="1:19" customHeight="1" ht="28.5">
@@ -10121,7 +10149,7 @@
       <c r="M153" s="113"/>
       <c r="N153" s="113"/>
       <c r="Q153" s="3" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
     </row>
     <row r="154" spans="1:19" customHeight="1" ht="14.25">
@@ -10140,7 +10168,7 @@
       <c r="M154" s="113"/>
       <c r="N154" s="113"/>
       <c r="Q154" s="3" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
     </row>
     <row r="155" spans="1:19" customHeight="1" ht="28.5">
@@ -10159,7 +10187,7 @@
       <c r="M155" s="113"/>
       <c r="N155" s="113"/>
       <c r="Q155" s="3" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
     </row>
     <row r="156" spans="1:19" customHeight="1" ht="14.25">
@@ -10178,7 +10206,7 @@
       <c r="M156" s="113"/>
       <c r="N156" s="113"/>
       <c r="Q156" s="3" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
     </row>
     <row r="157" spans="1:19" customHeight="1" ht="14.25">
@@ -10197,7 +10225,7 @@
       <c r="M157" s="113"/>
       <c r="N157" s="113"/>
       <c r="Q157" s="3" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
     </row>
     <row r="158" spans="1:19" customHeight="1" ht="14.25">
@@ -10216,7 +10244,7 @@
       <c r="M158" s="113"/>
       <c r="N158" s="113"/>
       <c r="Q158" s="3" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="159" spans="1:19" customHeight="1" ht="14.25">
@@ -10235,7 +10263,7 @@
       <c r="M159" s="113"/>
       <c r="N159" s="113"/>
       <c r="Q159" s="3" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
     </row>
     <row r="160" spans="1:19" customHeight="1" ht="14.25">
@@ -10254,7 +10282,7 @@
       <c r="M160" s="113"/>
       <c r="N160" s="113"/>
       <c r="Q160" s="3" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
     </row>
     <row r="161" spans="1:19" customHeight="1" ht="14.25">
@@ -10273,7 +10301,7 @@
       <c r="M161" s="113"/>
       <c r="N161" s="113"/>
       <c r="Q161" s="3" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
     </row>
     <row r="162" spans="1:19" customHeight="1" ht="14.25">
@@ -10292,7 +10320,7 @@
       <c r="M162" s="113"/>
       <c r="N162" s="113"/>
       <c r="Q162" s="3" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
     </row>
     <row r="163" spans="1:19" customHeight="1" ht="14.25">
@@ -10311,7 +10339,7 @@
       <c r="M163" s="113"/>
       <c r="N163" s="113"/>
       <c r="Q163" s="3" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
     </row>
     <row r="164" spans="1:19" customHeight="1" ht="14.25">
@@ -10330,7 +10358,7 @@
       <c r="M164" s="113"/>
       <c r="N164" s="113"/>
       <c r="Q164" s="3" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
     </row>
     <row r="165" spans="1:19" customHeight="1" ht="28.5">
@@ -10349,7 +10377,7 @@
       <c r="M165" s="113"/>
       <c r="N165" s="113"/>
       <c r="Q165" s="3" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
     </row>
     <row r="166" spans="1:19" customHeight="1" ht="14.25">
@@ -10368,7 +10396,7 @@
       <c r="M166" s="113"/>
       <c r="N166" s="113"/>
       <c r="Q166" s="3" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="167" spans="1:19" customHeight="1" ht="42.75">
@@ -10387,7 +10415,7 @@
       <c r="M167" s="113"/>
       <c r="N167" s="113"/>
       <c r="Q167" s="3" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
     </row>
     <row r="168" spans="1:19" customHeight="1" ht="14.25">
@@ -10406,7 +10434,7 @@
       <c r="M168" s="113"/>
       <c r="N168" s="113"/>
       <c r="Q168" s="3" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
     </row>
     <row r="169" spans="1:19" customHeight="1" ht="14.25">
@@ -10425,7 +10453,7 @@
       <c r="M169" s="113"/>
       <c r="N169" s="113"/>
       <c r="Q169" s="3" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
     </row>
     <row r="170" spans="1:19" customHeight="1" ht="28.5">
@@ -10444,7 +10472,7 @@
       <c r="M170" s="113"/>
       <c r="N170" s="113"/>
       <c r="Q170" s="3" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
     </row>
     <row r="171" spans="1:19" customHeight="1" ht="14.25">
@@ -10463,7 +10491,7 @@
       <c r="M171" s="113"/>
       <c r="N171" s="113"/>
       <c r="Q171" s="3" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
     </row>
     <row r="172" spans="1:19" customHeight="1" ht="14.25">
@@ -10482,7 +10510,7 @@
       <c r="M172" s="113"/>
       <c r="N172" s="113"/>
       <c r="Q172" s="3" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
     </row>
     <row r="173" spans="1:19" customHeight="1" ht="14.25">
@@ -10501,7 +10529,7 @@
       <c r="M173" s="113"/>
       <c r="N173" s="113"/>
       <c r="Q173" s="3" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
     </row>
     <row r="174" spans="1:19" customHeight="1" ht="14.25">
@@ -10520,7 +10548,7 @@
       <c r="M174" s="113"/>
       <c r="N174" s="113"/>
       <c r="Q174" s="3" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
     </row>
     <row r="175" spans="1:19" customHeight="1" ht="14.25">
@@ -10539,7 +10567,7 @@
       <c r="M175" s="113"/>
       <c r="N175" s="113"/>
       <c r="Q175" s="3" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
     </row>
     <row r="176" spans="1:19" customHeight="1" ht="14.25">
@@ -10558,7 +10586,7 @@
       <c r="M176" s="113"/>
       <c r="N176" s="113"/>
       <c r="Q176" s="3" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
     </row>
     <row r="177" spans="1:19" customHeight="1" ht="14.25">
@@ -10577,7 +10605,7 @@
       <c r="M177" s="113"/>
       <c r="N177" s="113"/>
       <c r="Q177" s="3" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
     </row>
     <row r="178" spans="1:19" customHeight="1" ht="14.25">
@@ -10596,7 +10624,7 @@
       <c r="M178" s="113"/>
       <c r="N178" s="113"/>
       <c r="Q178" s="3" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
     </row>
     <row r="179" spans="1:19" customHeight="1" ht="14.25">
@@ -10615,7 +10643,7 @@
       <c r="M179" s="113"/>
       <c r="N179" s="113"/>
       <c r="Q179" s="3" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
     </row>
     <row r="180" spans="1:19" customHeight="1" ht="28.5">
@@ -10634,7 +10662,7 @@
       <c r="M180" s="113"/>
       <c r="N180" s="113"/>
       <c r="Q180" s="3" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
     </row>
     <row r="181" spans="1:19" customHeight="1" ht="14.25">
@@ -10653,7 +10681,7 @@
       <c r="M181" s="113"/>
       <c r="N181" s="113"/>
       <c r="Q181" s="3" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
     </row>
     <row r="182" spans="1:19" customHeight="1" ht="14.25">
@@ -10672,7 +10700,7 @@
       <c r="M182" s="113"/>
       <c r="N182" s="113"/>
       <c r="Q182" s="3" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
     </row>
     <row r="183" spans="1:19" customHeight="1" ht="14.25">
@@ -10691,7 +10719,7 @@
       <c r="M183" s="113"/>
       <c r="N183" s="113"/>
       <c r="Q183" s="3" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
     </row>
     <row r="184" spans="1:19" customHeight="1" ht="14.25">
@@ -10710,7 +10738,7 @@
       <c r="M184" s="113"/>
       <c r="N184" s="113"/>
       <c r="Q184" s="3" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="185" spans="1:19" customHeight="1" ht="14.25">
@@ -10729,7 +10757,7 @@
       <c r="M185" s="113"/>
       <c r="N185" s="113"/>
       <c r="Q185" s="3" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
     <row r="186" spans="1:19" customHeight="1" ht="14.25">
@@ -10748,7 +10776,7 @@
       <c r="M186" s="113"/>
       <c r="N186" s="113"/>
       <c r="Q186" s="3" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
     </row>
     <row r="187" spans="1:19" customHeight="1" ht="14.25">
@@ -10767,7 +10795,7 @@
       <c r="M187" s="113"/>
       <c r="N187" s="113"/>
       <c r="Q187" s="3" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
     </row>
     <row r="188" spans="1:19" customHeight="1" ht="14.25">
@@ -10786,7 +10814,7 @@
       <c r="M188" s="113"/>
       <c r="N188" s="113"/>
       <c r="Q188" s="3" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
     </row>
     <row r="189" spans="1:19" customHeight="1" ht="14.25">
@@ -10805,7 +10833,7 @@
       <c r="M189" s="113"/>
       <c r="N189" s="113"/>
       <c r="Q189" s="3" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="190" spans="1:19" customHeight="1" ht="14.25">
@@ -10824,7 +10852,7 @@
       <c r="M190" s="113"/>
       <c r="N190" s="113"/>
       <c r="Q190" s="3" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
     </row>
     <row r="191" spans="1:19" customHeight="1" ht="14.25">
@@ -10843,7 +10871,7 @@
       <c r="M191" s="113"/>
       <c r="N191" s="113"/>
       <c r="Q191" s="3" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
     </row>
     <row r="192" spans="1:19" customHeight="1" ht="14.25">
@@ -10862,7 +10890,7 @@
       <c r="M192" s="113"/>
       <c r="N192" s="113"/>
       <c r="Q192" s="3" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
     </row>
     <row r="193" spans="1:19" customHeight="1" ht="14.25">
@@ -10881,7 +10909,7 @@
       <c r="M193" s="113"/>
       <c r="N193" s="113"/>
       <c r="Q193" s="3" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
     </row>
     <row r="194" spans="1:19" customHeight="1" ht="14.25">
@@ -10900,7 +10928,7 @@
       <c r="M194" s="113"/>
       <c r="N194" s="113"/>
       <c r="Q194" s="3" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
     </row>
     <row r="195" spans="1:19" customHeight="1" ht="14.25">
@@ -10919,7 +10947,7 @@
       <c r="M195" s="113"/>
       <c r="N195" s="113"/>
       <c r="Q195" s="3" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
     </row>
     <row r="196" spans="1:19" customHeight="1" ht="14.25">
@@ -10938,7 +10966,7 @@
       <c r="M196" s="113"/>
       <c r="N196" s="113"/>
       <c r="Q196" s="3" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
     </row>
     <row r="197" spans="1:19" customHeight="1" ht="14.25">
@@ -10957,7 +10985,7 @@
       <c r="M197" s="113"/>
       <c r="N197" s="113"/>
       <c r="Q197" s="3" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
     </row>
     <row r="198" spans="1:19" customHeight="1" ht="14.25">
@@ -10976,7 +11004,7 @@
       <c r="M198" s="113"/>
       <c r="N198" s="113"/>
       <c r="Q198" s="3" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
     </row>
     <row r="199" spans="1:19" customHeight="1" ht="14.25">
@@ -10995,7 +11023,7 @@
       <c r="M199" s="113"/>
       <c r="N199" s="113"/>
       <c r="Q199" s="3" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
     </row>
     <row r="200" spans="1:19" customHeight="1" ht="28.5">
@@ -11014,7 +11042,7 @@
       <c r="M200" s="113"/>
       <c r="N200" s="113"/>
       <c r="Q200" s="3" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
     </row>
     <row r="201" spans="1:19" customHeight="1" ht="14.25">
@@ -11033,7 +11061,7 @@
       <c r="M201" s="113"/>
       <c r="N201" s="113"/>
       <c r="Q201" s="3" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
     </row>
     <row r="202" spans="1:19" customHeight="1" ht="14.25">
@@ -11052,7 +11080,7 @@
       <c r="M202" s="113"/>
       <c r="N202" s="113"/>
       <c r="Q202" s="3" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
     </row>
     <row r="203" spans="1:19" customHeight="1" ht="14.25">
@@ -11071,7 +11099,7 @@
       <c r="M203" s="113"/>
       <c r="N203" s="113"/>
       <c r="Q203" s="3" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
     </row>
     <row r="204" spans="1:19" customHeight="1" ht="14.25">
@@ -11090,7 +11118,7 @@
       <c r="M204" s="113"/>
       <c r="N204" s="113"/>
       <c r="Q204" s="3" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="205" spans="1:19" customHeight="1" ht="14.25">
@@ -11109,7 +11137,7 @@
       <c r="M205" s="113"/>
       <c r="N205" s="113"/>
       <c r="Q205" s="3" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
     </row>
     <row r="206" spans="1:19" customHeight="1" ht="14.25">
@@ -11128,7 +11156,7 @@
       <c r="M206" s="113"/>
       <c r="N206" s="113"/>
       <c r="Q206" s="3" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
     </row>
     <row r="207" spans="1:19" customHeight="1" ht="28.5">
@@ -11147,7 +11175,7 @@
       <c r="M207" s="113"/>
       <c r="N207" s="113"/>
       <c r="Q207" s="3" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
     </row>
     <row r="208" spans="1:19" customHeight="1" ht="28.5">
@@ -11166,7 +11194,7 @@
       <c r="M208" s="113"/>
       <c r="N208" s="113"/>
       <c r="Q208" s="3" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
     </row>
     <row r="209" spans="1:19" customHeight="1" ht="14.25">
@@ -11185,7 +11213,7 @@
       <c r="M209" s="113"/>
       <c r="N209" s="113"/>
       <c r="Q209" s="3" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
     </row>
     <row r="210" spans="1:19" customHeight="1" ht="14.25">
@@ -11204,7 +11232,7 @@
       <c r="M210" s="113"/>
       <c r="N210" s="113"/>
       <c r="Q210" s="3" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
     </row>
     <row r="211" spans="1:19" customHeight="1" ht="14.25">
@@ -11223,7 +11251,7 @@
       <c r="M211" s="113"/>
       <c r="N211" s="113"/>
       <c r="Q211" s="3" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
     </row>
     <row r="212" spans="1:19" customHeight="1" ht="14.25">
@@ -11242,7 +11270,7 @@
       <c r="M212" s="113"/>
       <c r="N212" s="113"/>
       <c r="Q212" s="3" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
     </row>
     <row r="213" spans="1:19" customHeight="1" ht="14.25">
@@ -11261,7 +11289,7 @@
       <c r="M213" s="113"/>
       <c r="N213" s="113"/>
       <c r="Q213" s="3" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
     </row>
     <row r="214" spans="1:19" customHeight="1" ht="14.25">
@@ -11280,7 +11308,7 @@
       <c r="M214" s="113"/>
       <c r="N214" s="113"/>
       <c r="Q214" s="3" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
     </row>
     <row r="215" spans="1:19" customHeight="1" ht="14.25">
@@ -11299,7 +11327,7 @@
       <c r="M215" s="113"/>
       <c r="N215" s="113"/>
       <c r="Q215" s="3" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
     </row>
     <row r="216" spans="1:19" customHeight="1" ht="14.25">
@@ -11318,7 +11346,7 @@
       <c r="M216" s="113"/>
       <c r="N216" s="113"/>
       <c r="Q216" s="3" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
     </row>
     <row r="217" spans="1:19">
@@ -12498,7 +12526,7 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="18">
       <c r="A2" s="490" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="B2" s="491"/>
       <c r="C2" s="491"/>
@@ -12515,28 +12543,28 @@
     </row>
     <row r="3" spans="1:14" customHeight="1" ht="15">
       <c r="A3" s="144" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="B3" s="480" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="C3" s="480"/>
       <c r="D3" s="480"/>
       <c r="E3" s="481"/>
       <c r="F3" s="488" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="G3" s="484" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="H3" s="481"/>
       <c r="I3" s="484" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="J3" s="480"/>
       <c r="K3" s="481"/>
       <c r="L3" s="486" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="M3" s="487"/>
     </row>
@@ -12553,37 +12581,37 @@
       <c r="J4" s="482"/>
       <c r="K4" s="483"/>
       <c r="L4" s="5" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:14" customHeight="1" ht="27">
       <c r="A5" s="497" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B5" s="498"/>
       <c r="C5" s="498"/>
       <c r="D5" s="498"/>
       <c r="E5" s="498"/>
       <c r="F5" s="16" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="G5" s="495" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="H5" s="495"/>
       <c r="I5" s="496" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="J5" s="496"/>
       <c r="K5" s="496"/>
       <c r="L5" s="9" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:14" customHeight="1" ht="27">
@@ -12678,7 +12706,7 @@
     </row>
     <row r="12" spans="1:14" customHeight="1" ht="12">
       <c r="A12" s="515" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B12" s="516"/>
       <c r="C12" s="516"/>
@@ -12695,7 +12723,7 @@
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="518" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="B13" s="519"/>
       <c r="C13" s="519"/>
@@ -12712,7 +12740,7 @@
     </row>
     <row r="14" spans="1:14" customHeight="1" ht="12">
       <c r="A14" s="217" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="B14" s="105"/>
       <c r="C14" s="105"/>
@@ -12729,33 +12757,33 @@
     </row>
     <row r="15" spans="1:14" customHeight="1" ht="18">
       <c r="A15" s="4" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="B15" s="504" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="C15" s="505"/>
       <c r="D15" s="503" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="E15" s="504"/>
       <c r="F15" s="505"/>
       <c r="G15" s="503" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="H15" s="504"/>
       <c r="I15" s="505"/>
       <c r="J15" s="509" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="K15" s="499" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="L15" s="524" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="M15" s="493" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:14" customHeight="1" ht="15">
@@ -12775,11 +12803,11 @@
     </row>
     <row r="17" spans="1:14" customHeight="1" ht="18.75">
       <c r="A17" s="501" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="B17" s="502"/>
       <c r="C17" s="8" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="D17" s="485"/>
       <c r="E17" s="482"/>
@@ -12794,33 +12822,33 @@
     </row>
     <row r="18" spans="1:14" customHeight="1" ht="24" s="13" customFormat="1">
       <c r="A18" s="511" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B18" s="512"/>
       <c r="C18" s="24" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="D18" s="498" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="E18" s="498"/>
       <c r="F18" s="498"/>
       <c r="G18" s="498" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="H18" s="498"/>
       <c r="I18" s="498"/>
       <c r="J18" s="14" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:14" customHeight="1" ht="24" s="13" customFormat="1">
@@ -13230,7 +13258,7 @@
     </row>
     <row r="46" spans="1:14" customHeight="1" ht="9.75">
       <c r="A46" s="526" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B46" s="527"/>
       <c r="C46" s="527"/>
@@ -13247,7 +13275,7 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="27.75">
       <c r="A47" s="272" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B47" s="273"/>
       <c r="C47" s="274"/>
@@ -13257,10 +13285,10 @@
       <c r="G47" s="475"/>
       <c r="H47" s="476"/>
       <c r="I47" s="248" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="J47" s="249" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="K47" s="250"/>
       <c r="L47" s="250"/>
@@ -13269,7 +13297,7 @@
     </row>
     <row r="48" spans="1:14" customHeight="1" ht="9">
       <c r="A48" s="473" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="B48" s="473"/>
       <c r="C48" s="473"/>
@@ -13473,7 +13501,7 @@
     </row>
     <row r="2" spans="1:13" customHeight="1" ht="22.5">
       <c r="A2" s="579" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="B2" s="580"/>
       <c r="C2" s="580"/>
@@ -13488,22 +13516,22 @@
     </row>
     <row r="3" spans="1:13" customHeight="1" ht="15">
       <c r="A3" s="565" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="B3" s="567" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="C3" s="567"/>
       <c r="D3" s="568"/>
       <c r="E3" s="480" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="F3" s="481"/>
       <c r="G3" s="543" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="H3" s="484" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="I3" s="574"/>
       <c r="J3" s="574"/>
@@ -13528,10 +13556,10 @@
       <c r="C5" s="582"/>
       <c r="D5" s="583"/>
       <c r="E5" s="29" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="G5" s="500"/>
       <c r="H5" s="578"/>
@@ -13541,22 +13569,22 @@
     </row>
     <row r="6" spans="1:13" customHeight="1" ht="27.75">
       <c r="A6" s="540" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B6" s="541"/>
       <c r="C6" s="541"/>
       <c r="D6" s="542"/>
       <c r="E6" s="38" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="G6" s="39" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="H6" s="544" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="I6" s="545"/>
       <c r="J6" s="545"/>
@@ -13642,7 +13670,7 @@
     </row>
     <row r="13" spans="1:13" customHeight="1" ht="11.25">
       <c r="A13" s="515" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B13" s="516"/>
       <c r="C13" s="516"/>
@@ -13657,7 +13685,7 @@
     </row>
     <row r="14" spans="1:13" customHeight="1" ht="18">
       <c r="A14" s="587" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="B14" s="588"/>
       <c r="C14" s="588"/>
@@ -13672,25 +13700,25 @@
     </row>
     <row r="15" spans="1:13" customHeight="1" ht="18">
       <c r="A15" s="566" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="B15" s="504" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="C15" s="562"/>
       <c r="D15" s="563"/>
       <c r="E15" s="504" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="F15" s="505"/>
       <c r="G15" s="499" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="H15" s="509" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="I15" s="503" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="J15" s="562"/>
       <c r="K15" s="577"/>
@@ -13714,10 +13742,10 @@
       <c r="C17" s="329"/>
       <c r="D17" s="564"/>
       <c r="E17" s="29" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="G17" s="500"/>
       <c r="H17" s="510"/>
@@ -13727,25 +13755,25 @@
     </row>
     <row r="18" spans="1:13" customHeight="1" ht="24.75">
       <c r="A18" s="547" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B18" s="548"/>
       <c r="C18" s="548"/>
       <c r="D18" s="549"/>
       <c r="E18" s="30" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="I18" s="553" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="J18" s="554"/>
       <c r="K18" s="555"/>
@@ -14012,7 +14040,7 @@
     </row>
     <row r="39" spans="1:13" customHeight="1" ht="13.5">
       <c r="A39" s="275" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B39" s="276"/>
       <c r="C39" s="276"/>
@@ -14027,7 +14055,7 @@
     </row>
     <row r="40" spans="1:13" customHeight="1" ht="22.5">
       <c r="A40" s="556" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="B40" s="557"/>
       <c r="C40" s="557"/>
@@ -14042,36 +14070,36 @@
     </row>
     <row r="41" spans="1:13" customHeight="1" ht="33.75">
       <c r="A41" s="145" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="B41" s="150" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="C41" s="146" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="D41" s="537" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="E41" s="537"/>
       <c r="F41" s="537"/>
       <c r="G41" s="537"/>
       <c r="H41" s="538"/>
       <c r="I41" s="146" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="J41" s="537" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="K41" s="539"/>
     </row>
     <row r="42" spans="1:13" customHeight="1" ht="24.75">
       <c r="A42" s="532" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B42" s="533"/>
       <c r="C42" s="534" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="D42" s="535"/>
       <c r="E42" s="535"/>
@@ -14079,7 +14107,7 @@
       <c r="G42" s="535"/>
       <c r="H42" s="533"/>
       <c r="I42" s="534" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="J42" s="535"/>
       <c r="K42" s="536"/>
@@ -14164,7 +14192,7 @@
     </row>
     <row r="49" spans="1:13" customHeight="1" ht="11.25">
       <c r="A49" s="275" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B49" s="276"/>
       <c r="C49" s="276"/>
@@ -14179,7 +14207,7 @@
     </row>
     <row r="50" spans="1:13" customHeight="1" ht="28.5">
       <c r="A50" s="272" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B50" s="274"/>
       <c r="C50" s="474"/>
@@ -14187,11 +14215,11 @@
       <c r="E50" s="475"/>
       <c r="F50" s="476"/>
       <c r="G50" s="530" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="H50" s="531"/>
       <c r="I50" s="474" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="J50" s="475"/>
       <c r="K50" s="476"/>
@@ -14200,7 +14228,7 @@
     </row>
     <row r="51" spans="1:13" customHeight="1" ht="9.75">
       <c r="K51" s="256" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
     </row>
     <row r="52" spans="1:13" customHeight="1" ht="3"/>
@@ -14351,11 +14379,11 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="13.5">
       <c r="A2" s="694" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="B2" s="695"/>
       <c r="C2" s="721" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="D2" s="721"/>
       <c r="E2" s="721"/>
@@ -14372,7 +14400,7 @@
       <c r="A3" s="44"/>
       <c r="B3" s="45"/>
       <c r="C3" s="710" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="D3" s="710"/>
       <c r="E3" s="710"/>
@@ -14389,7 +14417,7 @@
       <c r="A4" s="44"/>
       <c r="B4" s="45"/>
       <c r="C4" s="710" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="D4" s="710"/>
       <c r="E4" s="710"/>
@@ -14415,7 +14443,7 @@
       <c r="A6" s="44"/>
       <c r="B6" s="45"/>
       <c r="C6" s="710" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="D6" s="710"/>
       <c r="E6" s="710"/>
@@ -14445,7 +14473,7 @@
       <c r="A8" s="44"/>
       <c r="B8" s="45"/>
       <c r="C8" s="710" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="D8" s="710"/>
       <c r="E8" s="710"/>
@@ -14475,7 +14503,7 @@
       <c r="E10" s="710"/>
       <c r="F10" s="711"/>
       <c r="G10" s="601" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="H10" s="601"/>
       <c r="I10" s="601"/>
@@ -14516,11 +14544,11 @@
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="733" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="B13" s="734"/>
       <c r="C13" s="729" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="D13" s="729"/>
       <c r="E13" s="562"/>
@@ -14541,7 +14569,7 @@
       <c r="E14" s="562"/>
       <c r="F14" s="563"/>
       <c r="G14" s="600" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="H14" s="601"/>
       <c r="I14" s="601"/>
@@ -14599,7 +14627,7 @@
       <c r="A18" s="55"/>
       <c r="B18" s="56"/>
       <c r="C18" s="603" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="D18" s="603"/>
       <c r="E18" s="604"/>
@@ -14620,7 +14648,7 @@
       <c r="E19" s="604"/>
       <c r="F19" s="605"/>
       <c r="G19" s="600" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="H19" s="601"/>
       <c r="I19" s="601"/>
@@ -14638,7 +14666,7 @@
       <c r="F20" s="605"/>
       <c r="G20" s="60"/>
       <c r="H20" s="742" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="I20" s="742"/>
       <c r="J20" s="266"/>
@@ -14654,7 +14682,7 @@
       <c r="E21" s="604"/>
       <c r="F21" s="605"/>
       <c r="G21" s="743" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="H21" s="744"/>
       <c r="I21" s="744"/>
@@ -14671,7 +14699,7 @@
       <c r="E22" s="606"/>
       <c r="F22" s="607"/>
       <c r="G22" s="130" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="H22" s="257"/>
       <c r="I22" s="608"/>
@@ -14682,11 +14710,11 @@
     </row>
     <row r="23" spans="1:14" customHeight="1" ht="18">
       <c r="A23" s="596" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="B23" s="597"/>
       <c r="C23" s="609" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="D23" s="609"/>
       <c r="E23" s="609"/>
@@ -14707,7 +14735,7 @@
       <c r="E24" s="611"/>
       <c r="F24" s="612"/>
       <c r="G24" s="600" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="H24" s="601"/>
       <c r="I24" s="601"/>
@@ -14748,11 +14776,11 @@
     </row>
     <row r="27" spans="1:14" customHeight="1" ht="14.25">
       <c r="A27" s="596" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="B27" s="597"/>
       <c r="C27" s="609" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="D27" s="609"/>
       <c r="E27" s="609"/>
@@ -14773,7 +14801,7 @@
       <c r="E28" s="611"/>
       <c r="F28" s="612"/>
       <c r="G28" s="600" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="H28" s="601"/>
       <c r="I28" s="601"/>
@@ -14813,11 +14841,11 @@
     </row>
     <row r="31" spans="1:14" customHeight="1" ht="18">
       <c r="A31" s="596" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="B31" s="597"/>
       <c r="C31" s="609" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="D31" s="609"/>
       <c r="E31" s="609"/>
@@ -14838,7 +14866,7 @@
       <c r="E32" s="611"/>
       <c r="F32" s="612"/>
       <c r="G32" s="669" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="H32" s="670"/>
       <c r="I32" s="670"/>
@@ -14866,7 +14894,7 @@
       <c r="A34" s="53"/>
       <c r="B34" s="54"/>
       <c r="C34" s="611" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="D34" s="611"/>
       <c r="E34" s="611"/>
@@ -14887,7 +14915,7 @@
       <c r="E35" s="611"/>
       <c r="F35" s="612"/>
       <c r="G35" s="669" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="H35" s="670"/>
       <c r="I35" s="670"/>
@@ -14912,11 +14940,11 @@
     </row>
     <row r="37" spans="1:14" customHeight="1" ht="18">
       <c r="A37" s="596" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="B37" s="597"/>
       <c r="C37" s="727" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="D37" s="727"/>
       <c r="E37" s="727"/>
@@ -14937,7 +14965,7 @@
       <c r="E38" s="729"/>
       <c r="F38" s="730"/>
       <c r="G38" s="600" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="H38" s="601"/>
       <c r="I38" s="601"/>
@@ -14978,11 +15006,11 @@
     </row>
     <row r="41" spans="1:14" customHeight="1" ht="28.5">
       <c r="A41" s="724" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="B41" s="725"/>
       <c r="C41" s="611" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="D41" s="611"/>
       <c r="E41" s="611"/>
@@ -15012,11 +15040,11 @@
     </row>
     <row r="43" spans="1:14" customHeight="1" ht="13.5">
       <c r="A43" s="68" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="B43" s="69"/>
       <c r="C43" s="611" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="D43" s="611"/>
       <c r="E43" s="611"/>
@@ -15037,7 +15065,7 @@
       <c r="E44" s="611"/>
       <c r="F44" s="612"/>
       <c r="G44" s="198" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="H44" s="259"/>
       <c r="I44" s="123"/>
@@ -15048,11 +15076,11 @@
     </row>
     <row r="45" spans="1:14" customHeight="1" ht="13.5">
       <c r="A45" s="68" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="B45" s="69"/>
       <c r="C45" s="612" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="D45" s="612"/>
       <c r="E45" s="612"/>
@@ -15073,7 +15101,7 @@
       <c r="E46" s="612"/>
       <c r="F46" s="612"/>
       <c r="G46" s="199" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="H46" s="260"/>
       <c r="I46" s="123"/>
@@ -15085,11 +15113,11 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="13.5">
       <c r="A47" s="68" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="B47" s="69"/>
       <c r="C47" s="611" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="D47" s="611"/>
       <c r="E47" s="120"/>
@@ -15110,7 +15138,7 @@
       <c r="E48" s="688"/>
       <c r="F48" s="689"/>
       <c r="G48" s="200" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="H48" s="261"/>
       <c r="I48" s="125"/>
@@ -15138,11 +15166,11 @@
     </row>
     <row r="50" spans="1:14" customHeight="1" ht="23.25">
       <c r="A50" s="598" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="B50" s="599"/>
       <c r="C50" s="196" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
       <c r="D50" s="196"/>
       <c r="E50" s="196"/>
@@ -15157,17 +15185,17 @@
     </row>
     <row r="51" spans="1:14" customHeight="1" ht="18">
       <c r="A51" s="684" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="B51" s="685"/>
       <c r="C51" s="685"/>
       <c r="D51" s="685"/>
       <c r="E51" s="686"/>
       <c r="F51" s="187" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
       <c r="G51" s="693" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="H51" s="537"/>
       <c r="I51" s="539"/>
@@ -15223,11 +15251,11 @@
     </row>
     <row r="55" spans="1:14" customHeight="1" ht="39.75">
       <c r="A55" s="694" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="B55" s="695"/>
       <c r="C55" s="708" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="D55" s="708"/>
       <c r="E55" s="708"/>
@@ -15252,7 +15280,7 @@
       <c r="I56" s="263"/>
       <c r="J56" s="207"/>
       <c r="K56" s="680" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="L56" s="680"/>
       <c r="M56" s="186"/>
@@ -15302,7 +15330,7 @@
     <row r="60" spans="1:14" customHeight="1" ht="25.5">
       <c r="A60" s="79"/>
       <c r="B60" s="661" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="C60" s="662"/>
       <c r="D60" s="663"/>
@@ -15317,7 +15345,7 @@
     <row r="61" spans="1:14" customHeight="1" ht="20.25">
       <c r="A61" s="79"/>
       <c r="B61" s="648" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="C61" s="649"/>
       <c r="D61" s="136"/>
@@ -15332,7 +15360,7 @@
     <row r="62" spans="1:14" customHeight="1" ht="9">
       <c r="A62" s="79"/>
       <c r="B62" s="636" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="C62" s="637"/>
       <c r="D62" s="640"/>
@@ -15350,7 +15378,7 @@
       <c r="C63" s="651"/>
       <c r="D63" s="664"/>
       <c r="F63" s="665" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="G63" s="666"/>
       <c r="H63" s="666"/>
@@ -15362,7 +15390,7 @@
     <row r="64" spans="1:14" customHeight="1" ht="10.5">
       <c r="A64" s="79"/>
       <c r="B64" s="636" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="C64" s="637"/>
       <c r="D64" s="640"/>
@@ -15381,14 +15409,14 @@
       <c r="C65" s="639"/>
       <c r="D65" s="641"/>
       <c r="F65" s="633" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="G65" s="634"/>
       <c r="H65" s="634"/>
       <c r="I65" s="635"/>
       <c r="J65" s="82"/>
       <c r="K65" s="631" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="L65" s="632"/>
       <c r="M65" s="80"/>
@@ -15410,7 +15438,7 @@
     </row>
     <row r="67" spans="1:14" customHeight="1" ht="28.5">
       <c r="A67" s="628" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="B67" s="629"/>
       <c r="C67" s="629"/>
@@ -15445,7 +15473,7 @@
       <c r="C69" s="247"/>
       <c r="D69" s="247"/>
       <c r="E69" s="622" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="F69" s="623"/>
       <c r="G69" s="623"/>
@@ -15473,7 +15501,7 @@
     </row>
     <row r="71" spans="1:14" customHeight="1" ht="10.5">
       <c r="A71" s="621" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="B71" s="621"/>
       <c r="C71" s="621"/>
@@ -15652,35 +15680,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="B2" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="C2" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -15690,7 +15718,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>